<commit_message>
Recommend using ENA checklist variables for emof data.
</commit_message>
<xml_diff>
--- a/molmod/static/downloads/SBDI-ASV-template.xlsx
+++ b/molmod/static/downloads/SBDI-ASV-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/molmod/static/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731F32DB-BFC4-264E-8373-996B62AAE8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C159091B-0625-E043-9921-D0EA15C325A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="460" windowWidth="26580" windowHeight="16300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10780" yWindow="8740" windowWidth="26580" windowHeight="16300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event" sheetId="1" r:id="rId1"/>
@@ -746,12 +746,6 @@
     <t>emof-simple</t>
   </si>
   <si>
-    <t>Use this, simplified, version of emof if you only want to submit measurementType (i.e. name), measurementUnit and measurementValue for some contextual variable, i.e. no additional metadata regarding these. Add a single field for every measured variable, and a single row for every event with measured variables(s).</t>
-  </si>
-  <si>
-    <t>Use this full version of emof to report contextual data if you, in addition to measurementType (i.e. name), measurementUnit and measurementValue, also want to refer to some controlled vocabulary or system for e.g. variables, units and values etc. Otherwise, see emof-simpler below.</t>
-  </si>
-  <si>
     <t>SAMEA3724531</t>
   </si>
   <si>
@@ -788,19 +782,7 @@
     <t>marine pelagic zone [ENVO:00000208]</t>
   </si>
   <si>
-    <t>Preferrably, this value should correspond to environment (biome) in your ENA submission, when applicable. You can search for ENVO_00000428 in https://www.ebi.ac.uk/ols/index, then continue downwards in the biome subtree, until you find the most specific term that accurately describes your data.</t>
-  </si>
-  <si>
-    <t>Preferrably, this value should correspond to environment (feature) in your ENA submission, when applicable. A good starting point for searching in https://www.ebi.ac.uk/ols/index could be ENVO_01000813. Again, continue downwards in the subtree, until you find the most specific term that accurately describes your data.</t>
-  </si>
-  <si>
-    <t>Preferrably, this value should correspond to environment (material) in your ENA submission, when applicable. A good starting point for searching in https://www.ebi.ac.uk/ols/index could be ENVO_00010483 . Again, continue downwards in the subtree, until you find the most specific term that accurately describes your data.</t>
-  </si>
-  <si>
     <t>brackish water [ENVO:00002019]</t>
-  </si>
-  <si>
-    <t>Unique identifier for event, as provided by data contributor. Preferrably use event (sample) names that correspond to what you use in related publications.</t>
   </si>
   <si>
     <t>Anna Andersson|Björn Bengtsson</t>
@@ -817,6 +799,24 @@
   <si>
     <t>Note that, for practical reasons, we currently follow GBIF in grouping prokaryote domains Archaea and Bacteria together with e.g. eukaryote kingdoms under header 'kingdom'.</t>
   </si>
+  <si>
+    <t>Unique identifier for event, as provided by data contributor. Preferably use event (sample) names that correspond to what you use in related publications.</t>
+  </si>
+  <si>
+    <t>Preferably, this value should correspond to environment (biome) in your ENA submission, when applicable. You can search for ENVO_00000428 in https://www.ebi.ac.uk/ols/index, then continue downwards in the biome subtree, until you find the most specific term that accurately describes your data.</t>
+  </si>
+  <si>
+    <t>Preferably, this value should correspond to environment (feature) in your ENA submission, when applicable. A good starting point for searching in https://www.ebi.ac.uk/ols/index could be ENVO_01000813. Again, continue downwards in the subtree, until you find the most specific term that accurately describes your data.</t>
+  </si>
+  <si>
+    <t>Preferably, this value should correspond to environment (material) in your ENA submission, when applicable. A good starting point for searching in https://www.ebi.ac.uk/ols/index could be ENVO_00010483 . Again, continue downwards in the subtree, until you find the most specific term that accurately describes your data.</t>
+  </si>
+  <si>
+    <t>Use this full version of emof to report contextual data if you, in addition to measurementType (i.e. name), measurementUnit and measurementValue, also want to refer to some controlled vocabulary or system for e.g. variables, units and values etc. Otherwise, see emof-simpler below. Preferably use variable names and unists listed in a relevant GCS Checklist, see https://www.ebi.ac.uk/ena/browser/checklists.</t>
+  </si>
+  <si>
+    <t>Use this, simplified, version of emof if you only want to submit measurementType (i.e. name), measurementUnit and measurementValue for some contextual variable, i.e. no additional metadata regarding these. Preferably use variable names and unists listed in a relevant GCS Checklist, see https://www.ebi.ac.uk/ena/browser/checklists. Add a single field for every measured variable, and a single row for every event with measured variables(s).</t>
+  </si>
 </sst>
 </file>
 
@@ -826,11 +826,18 @@
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1121,127 +1128,133 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1576,7 +1589,7 @@
         <v>211</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>214</v>
@@ -1608,7 +1621,7 @@
         <v>210</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>213</v>
@@ -1651,7 +1664,7 @@
         <v>209</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>212</v>
@@ -4988,7 +5001,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:V9">
     <sortCondition ref="A3:A9"/>
   </sortState>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -6140,7 +6153,7 @@
     <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -13348,10 +13361,10 @@
   </sheetPr>
   <dimension ref="A1:AA1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
+      <selection pane="bottomLeft" activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13476,10 +13489,10 @@
         <v>69</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H3" s="42" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
@@ -13515,13 +13528,13 @@
         <v>70</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F4" s="28" t="s">
         <v>71</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H4" s="47" t="s">
         <v>214</v>
@@ -13860,7 +13873,7 @@
         <v>99</v>
       </c>
       <c r="H12" s="42" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="I12" s="21"/>
       <c r="J12" s="21"/>
@@ -14180,7 +14193,7 @@
       </c>
       <c r="G20" s="29" t="str">
         <f>G2</f>
-        <v>Unique identifier for event, as provided by data contributor. Preferrably use event (sample) names that correspond to what you use in related publications.</v>
+        <v>Unique identifier for event, as provided by data contributor. Preferably use event (sample) names that correspond to what you use in related publications.</v>
       </c>
       <c r="H20" s="29" t="str">
         <f>H2</f>
@@ -14531,19 +14544,19 @@
         <v>63</v>
       </c>
       <c r="D29" s="28" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E29" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="F29" s="30" t="s">
+        <v>240</v>
+      </c>
+      <c r="G29" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="H29" s="42" t="s">
         <v>241</v>
-      </c>
-      <c r="F29" s="30" t="s">
-        <v>242</v>
-      </c>
-      <c r="G29" s="29" t="s">
-        <v>249</v>
-      </c>
-      <c r="H29" s="42" t="s">
-        <v>243</v>
       </c>
       <c r="I29" s="21"/>
       <c r="J29" s="21"/>
@@ -14576,19 +14589,19 @@
         <v>63</v>
       </c>
       <c r="D30" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="F30" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="E30" s="28" t="s">
+      <c r="G30" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="H30" s="42" t="s">
         <v>246</v>
-      </c>
-      <c r="F30" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="G30" s="29" t="s">
-        <v>250</v>
-      </c>
-      <c r="H30" s="42" t="s">
-        <v>248</v>
       </c>
       <c r="I30" s="21"/>
       <c r="J30" s="21"/>
@@ -14630,10 +14643,10 @@
         <v>136</v>
       </c>
       <c r="G31" s="34" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="H31" s="44" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="I31" s="21"/>
       <c r="J31" s="21"/>
@@ -14676,7 +14689,7 @@
       </c>
       <c r="G32" s="25" t="str">
         <f>G2</f>
-        <v>Unique identifier for event, as provided by data contributor. Preferrably use event (sample) names that correspond to what you use in related publications.</v>
+        <v>Unique identifier for event, as provided by data contributor. Preferably use event (sample) names that correspond to what you use in related publications.</v>
       </c>
       <c r="H32" s="25" t="str">
         <f>H2</f>
@@ -14702,7 +14715,7 @@
       <c r="Z32" s="21"/>
       <c r="AA32" s="21"/>
     </row>
-    <row r="33" spans="1:27" ht="136" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A33" s="26" t="s">
         <v>138</v>
       </c>
@@ -14721,8 +14734,8 @@
       <c r="F33" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="G33" s="29" t="s">
-        <v>236</v>
+      <c r="G33" s="50" t="s">
+        <v>257</v>
       </c>
       <c r="H33" s="42"/>
       <c r="I33" s="21"/>
@@ -15198,7 +15211,7 @@
       <c r="Z44" s="21"/>
       <c r="AA44" s="21"/>
     </row>
-    <row r="45" spans="1:27" ht="154" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" ht="205" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
         <v>234</v>
       </c>
@@ -15217,11 +15230,11 @@
       <c r="F45" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="G45" s="34" t="s">
-        <v>235</v>
+      <c r="G45" s="51" t="s">
+        <v>258</v>
       </c>
       <c r="H45" s="44" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="I45" s="21"/>
       <c r="J45" s="21"/>
@@ -15309,7 +15322,7 @@
       </c>
       <c r="G47" s="25" t="str">
         <f>G2</f>
-        <v>Unique identifier for event, as provided by data contributor. Preferrably use event (sample) names that correspond to what you use in related publications.</v>
+        <v>Unique identifier for event, as provided by data contributor. Preferably use event (sample) names that correspond to what you use in related publications.</v>
       </c>
       <c r="H47" s="25" t="str">
         <f>H2</f>
@@ -15482,7 +15495,7 @@
         <v>189</v>
       </c>
       <c r="G51" s="49" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="H51" s="42"/>
       <c r="I51" s="21"/>

</xml_diff>

<commit_message>
Fix missing ASV table data in template
</commit_message>
<xml_diff>
--- a/molmod/static/downloads/SBDI-ASV-template.xlsx
+++ b/molmod/static/downloads/SBDI-ASV-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/molmod/static/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C159091B-0625-E043-9921-D0EA15C325A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898E2871-BB16-5B4F-A5D6-5EC06317E0C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10780" yWindow="8740" windowWidth="26580" windowHeight="16300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10780" yWindow="8740" windowWidth="38000" windowHeight="14600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="302">
   <si>
     <t>event_id_alias</t>
   </si>
@@ -817,6 +817,135 @@
   <si>
     <t>Use this, simplified, version of emof if you only want to submit measurementType (i.e. name), measurementUnit and measurementValue for some contextual variable, i.e. no additional metadata regarding these. Preferably use variable names and unists listed in a relevant GCS Checklist, see https://www.ebi.ac.uk/ena/browser/checklists. Add a single field for every measured variable, and a single row for every event with measured variables(s).</t>
   </si>
+  <si>
+    <t>919a2aa9d306e4cf3fa9ca02a2aa5730</t>
+  </si>
+  <si>
+    <t>TCGAGAATTTTTCACAATGGGGGAAACCCTGATGGAGCGACGCCGCGTGGAGGATGAAGGTTTTCGGATTGTAAACTCCTGTCATTAGAGAACAAGGCACATGGTTTAACTGGCCGTGTGTTGATAGTATCTGAAGAGGAAGGGACGGCTAACTCTGTGCCAGCAGCCGCGGTAATACAGAGGTCTCAAGCGTTGTTCGGATTCATTGGGCGTAAAGGGTGCGTAGGTGGCGAGGTAAGTCGGATGTGAAATCTCCAAGCTCAACTTGGAAACTGCATTCGATACTGCTTTGCTAGAGGATTGTAGAGGGCATTGGAATTCACGGTGTAGCAGTGAAATGCGTAGATATCGTGAGGAAGACCAGTGGCGAAGGCGAATGCCTGGGCAATTCCTGACACTGAGGCACGAAGGCCAGGGGAGCAAACG</t>
+  </si>
+  <si>
+    <t>Bacteria</t>
+  </si>
+  <si>
+    <t>Verrucomicrobiota</t>
+  </si>
+  <si>
+    <t>Verrucomicrobiae</t>
+  </si>
+  <si>
+    <t>Chthoniobacterales</t>
+  </si>
+  <si>
+    <t>UBA6821</t>
+  </si>
+  <si>
+    <t>1ead98754d34073a4606f7ff1e94126e</t>
+  </si>
+  <si>
+    <t>TGGGGAATTTTCCGCAATGGGCGCAAGCCTGACGGAGCAACGCCGCGTGAGGGATGAAGGCCTCTGGGCTGTAAACCTCTTTTATCAAGGAAGAAGATCTGACGGTACTTGATGAATAAGCCACGGCTAATTCCGTGCCAGCAGCCGCGGTAATACGGGAGTGGCAAGCGTTATCCGGAATTATTGGGCGTAAAGCGTCCGCAGGCGGTTTTACAAGTCTGTCGTTAAAACGTGGAGCTCAACTCCATTTCGGCGATGGAAACTGTAAGACTAGAGTGTGGTAGGGGCAGAGGGAATTCCCGGTGTAGCGGTGAAATGCGTAGATATCGGGAAGAACACCAGTGGCGAAGGCGCTCTGCTGGGCCATAACTGACGCTCATGGACGAAAGCTAGGGGAGCGAAAG</t>
+  </si>
+  <si>
+    <t>Cyanobacteria</t>
+  </si>
+  <si>
+    <t>Cyanobacteriia</t>
+  </si>
+  <si>
+    <t>PCC-6307</t>
+  </si>
+  <si>
+    <t>Cyanobiaceae</t>
+  </si>
+  <si>
+    <t>Synechococcus_D</t>
+  </si>
+  <si>
+    <t>43e088977eba5732bfa45e20b1d8cdd2</t>
+  </si>
+  <si>
+    <t>TCGAGAATTTTTCACAATGGGGGAAACCCTGATGGAGCGACGCCGCGTGGAGGATGAAGGTTTTCGGATCGTAAACTCCTGTCATTAGAGAACAAGGCACACGGTTTAACTGGCTGTGTGTTGATAGTATCTGAAGAGGAAGGGACGGCTAACTCTGTGCCAGCAGCCGCGGTAATACAGAGGTCTCAAGCGTTGTTCGGATTCATTGGGCGTAAAGGGTGCGTAGGTGGCGAGGTAAGTCGGATGTGAAATCTCCAAGCTCAACTTGGAAACTGCATTCGATACTGCTTTGCTAGAGGATTGTAGAGGGCATTGGAATTCACGGTGTAGCAGTGAAATGCGTAGATATCGTGAGGAAGACCAGTGGCGAAGGCGAATGCCTGGGCAATTCCTGACACTGAGGCACGAAGGCCAGGGGAGCAAACG</t>
+  </si>
+  <si>
+    <t>1b2c41577c16f4c672a2a861e6b89b14</t>
+  </si>
+  <si>
+    <t>TAGGGAATATTGGGCAATGGGCGAAAGCCTGACCCAGCGACGCCGCGTGAGGGATGAAGGTCTTCGGATTGTAAACCTCTTTCAGTAGGGAAGAAGCGAAAGTGACGGTACCTAAAGAAGAAGCACCGGCTAACTATGTGCCAGCAGCCGCGGTAATACATAGGGTGCAAGCGTTGTCCGGAATTATTGGGCGTAAAGAGCTCGTAGGTCGTTTGTCGCGTCGATTGTGAAAATCTGAGGCTCAACCTCAGACCTGCAGTCGATACGGGCAAACTAGAGTGTGGTAGGGGAGACTGGAATTCCTGGTGTAGCGGTGGAATGCGCAGATATCAGGAGGAACACCAATGGCGAAGGCAGGTCTCTGGGCCATAACTGACACTGAGGAGCGAAAGTGCGGGGAGCGAACA</t>
+  </si>
+  <si>
+    <t>Actinobacteriota</t>
+  </si>
+  <si>
+    <t>Actinomycetia</t>
+  </si>
+  <si>
+    <t>Nanopelagicales</t>
+  </si>
+  <si>
+    <t>Nanopelagicaceae</t>
+  </si>
+  <si>
+    <t>Nanopelagicus</t>
+  </si>
+  <si>
+    <t>40b37890b1b1fcdf0ece91f1da34c1ca</t>
+  </si>
+  <si>
+    <t>TGGGGAATTTTCCGCAATGGGCGCAAGCCTGACGGAGCAACGCCGCGTGAGGGATGAAGGCCTCTGGGCTGTAAACCTCTTTTATCAAGGAAGAAGATCTGACGGTACTTGATGAATAAGCCACGGCTAATTCCGTGCCAGCAGCCGCGGTAATACGGGAGTGGCAAGCGTTATCCGGAATTATTGGGCGTAAAGCGTCCGCAGGCGGTCTTGAAAGTCTGTTGTTAAAGCGTGGAGCTCAACTCCATTTCAGCAATGGAAACTAGAAGACTAGAGTGTGGTAGGGGCAGAGGGAATTCCCGGTGTAGCGGTGAAATGCGTAGATATCGGGAAGAACACCAGTGGCGAAGGCGCTCTGCTGGGCCATAACTGACGCTCATGGACGAAAGCCAGGGGAGCGAAAG</t>
+  </si>
+  <si>
+    <t>UBA5018</t>
+  </si>
+  <si>
+    <t>ae71bf7c99d3583a2d8841e5911c5716</t>
+  </si>
+  <si>
+    <t>TGGGGAATATTGGGCAATGGAGGAAACTCTGACCCAGCGACGCCGCGTGCGGGATGAAGGCCTTCGGGTTGTAAACCGCTTTCAGTAGGGAAGAAGCGAAAGTGACGGTACCTACAAAAGAAGCACCGGCTAACTATGTGCCAGCAGCCGCGGTAATACATAGGGTGCAAGCGTTGTCCGGAATTATTGGGCGTAAAGAGCTCGTAGGTCGTTTGTTACGTCGGATGTGAAAACCTGAGGCTCAACCTCAGGCCTGCATTCGATACGGGCAAACTAGAGTTTGGTAGGGGAGACTGGAATTCCTGGTGTAGCGGTGGAATGCGCAGATATCAGGAGGAACACCAATGGCGAAGGCAGGTCTCTGGGCCAATACTGACACTGAGGAGCGAAAGTCTGGGGAGCGAACA</t>
+  </si>
+  <si>
+    <t>887bc7033b46d960e893caceb711700b</t>
+  </si>
+  <si>
+    <t>TGGGGAATCTTGCGCAATGGGCGAAAGCCTGACGCAGCAACGCCGCGTGCGGGAAGAAGGCTTTCGGGCTGTAAACCGCTTTCAGCAGGAACGAAAATGACGGTACCTGCAGAAGAAGGAGCGGCCAACTATGTGCCAGCAGCCGCGGTGATACATAGGCTTCAAGCGTTGTCCGGATTTATTGGGCGTAAAGAGTTCGTAGGCGGTCGAGTAAGTCGGGTGTGAAAATTCTGGGCTCAACCCAGAGACGCCACCCGATACTGCTTAACTTGAGTTCGATAGGGGAGTGGGGAATTCCTAGTGTAGCGGTGAAATGCGCAGATATTAGGAGGAACACCGGTGGCGAAGGCGCCACTCTGGATCGACACTGACGCTGAGGAACGAAAGCATGGGTAGCAAACA</t>
+  </si>
+  <si>
+    <t>Acidimicrobiia</t>
+  </si>
+  <si>
+    <t>Acidimicrobiales</t>
+  </si>
+  <si>
+    <t>Ilumatobacteraceae</t>
+  </si>
+  <si>
+    <t>BACL27</t>
+  </si>
+  <si>
+    <t>sp014190055</t>
+  </si>
+  <si>
+    <t>88b5b5240649749ca876d10823045b01</t>
+  </si>
+  <si>
+    <t>TGGGGAATCTTGCGCAATGGGCGAAAGCCTGACGCAGCAACGCCGCGTGCGGGATGAAGGCCTTCGGGCTGTAAACCGCTTTCAGCAGGAACGAAAATGACGGTACCTGCAGAAGAAGGAGCGGCCAACTACGTGCCAGCAGCCGCGGTGACACGTAGGCTCCAAGCGTTGTCCGGATTTATTGGGCGTAAAGAGCTCGTAGGCGGTTGAGTAAGTCGGGTGTGAAAACTCTGGGCTTAACCCGGAGACGCCATCCGATACTGCTCTGACTAGAGTTCAGGAGGGGAGTGGGGAATTCCTAGTGTAGCGGTGAAATGCGCAGATATTAGGAGGAACACCGGTGGCGAAGGCGCCACTCTGGACTGAAACTGACGCTGAGGAGCGAAAGCATGGGTAGCAAACA</t>
+  </si>
+  <si>
+    <t>UBA3006</t>
+  </si>
+  <si>
+    <t>95efad17b5fb6b91274a6ef3c47a098a</t>
+  </si>
+  <si>
+    <t>TGGGGAATTTTCCGCAATGGGCGCAAGCCTGACGGAGCAACGCCGCGTGAGGGATGAAGGCCTCTGGGCTGTAAACCTCTTTTATCAAGGAAGAAGATCTGACGGTACTTGATGAATAAGCCACGGCTAATTCCGTGCCAGCAGCCGCGGTAATACGGGAGTGGCAAGCGTTATCCGGAATTATTGGGCGTAAAGCGTCCGCAGGCGGTTTTACAAGTCTGTCGTTAAAACGTGGAGCTCAACTCCATTTCGGCGATGGAAACTGTAAGACTAGAGTGTGGTAGGGGCAGAGGGAATTCCCGGTGTAGCGGTGAAATGCGTAGATATCGGGAAGAACACCAGTGGCGAAGGCGCTCTGCTGGGCCATAACTGACGCTCATGGACGAAAGCCAGGGGAGCGAAAG</t>
+  </si>
+  <si>
+    <t>c366064866eaed18a54d15640272ab34</t>
+  </si>
+  <si>
+    <t>TGGGGAATATTGGGCAATGGAGGAAACTCTGACCCAGCGACGCCGCGTGCGGGATGAAGGCCTTCGGGTTGTAAACCGCTTTCAGCAGGGAAGAAGCGAAAGTGACGGTACCTGCAGAAGAAGCACCGGCTAACTATGTGCCAGCAGCCGCGGTAATACATAGGGTGCAAGCGTTGTCCGGAATTATTGGGCGTAAAGAGCTCGTAGGTGGTTCGTCACGTCGGATGTGAAACTCTGGGGCTTAACCCCAGACCTGCATTCGATACGGGCGAGCTTGAGTATGGTAGGGGAGTCTGGAATTCCTGGTGTAGCGGTGGAATGCGCAGATATCAGGAGGAACACCAATGGCGAAGGCAGGACTCTGGGCCATTACTGACACTGAGGAGCGAAAGCGTGGGGAGCGAACA</t>
+  </si>
+  <si>
+    <t>Planktophila</t>
+  </si>
 </sst>
 </file>
 
@@ -826,11 +955,18 @@
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1128,133 +1264,133 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1503,8 +1639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD991"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1597,6 +1733,9 @@
       <c r="D2" s="16" t="s">
         <v>215</v>
       </c>
+      <c r="E2" s="7">
+        <v>5414</v>
+      </c>
       <c r="G2" s="6">
         <v>55.185000000000002</v>
       </c>
@@ -1628,6 +1767,9 @@
       </c>
       <c r="D3" s="16" t="s">
         <v>215</v>
+      </c>
+      <c r="E3" s="7">
+        <v>37676</v>
       </c>
       <c r="G3" s="6">
         <v>55.433999999999997</v>
@@ -1671,6 +1813,9 @@
       </c>
       <c r="D4" s="16" t="s">
         <v>215</v>
+      </c>
+      <c r="E4" s="7">
+        <v>41973</v>
       </c>
       <c r="G4" s="6">
         <v>56.031999999999996</v>
@@ -5001,7 +5146,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:V9">
     <sortCondition ref="A3:A9"/>
   </sortState>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -6153,7 +6298,7 @@
     <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -6164,24 +6309,13 @@
   <dimension ref="A1:M982"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.7109375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" style="7" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="27" style="7" customWidth="1"/>
-    <col min="10" max="10" width="25" style="7" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" style="7" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" style="7" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" style="7" customWidth="1"/>
+    <col min="2" max="13" width="17.28515625" style="7" customWidth="1"/>
     <col min="14" max="16384" width="11.28515625" style="7"/>
   </cols>
   <sheetData>
@@ -9468,7 +9602,7 @@
   <dimension ref="A1:E973"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12478,24 +12612,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AE472"/>
+  <dimension ref="A1:O472"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.140625" style="7" customWidth="1"/>
     <col min="2" max="2" width="13.140625" style="7" customWidth="1"/>
-    <col min="3" max="15" width="12.140625" style="7" customWidth="1"/>
-    <col min="16" max="21" width="9.5703125" style="7" customWidth="1"/>
-    <col min="22" max="23" width="8.5703125" style="7" customWidth="1"/>
-    <col min="24" max="31" width="11.28515625" style="7" customWidth="1"/>
-    <col min="32" max="16384" width="11.28515625" style="7"/>
+    <col min="3" max="13" width="12.140625" style="7" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" style="7" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="7" customWidth="1"/>
+    <col min="16" max="16384" width="11.28515625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>41</v>
       </c>
@@ -12541,369 +12674,372 @@
       <c r="O1" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-    </row>
-    <row r="2" spans="1:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="6"/>
-    </row>
-    <row r="3" spans="1:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
-    </row>
-    <row r="4" spans="1:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="6"/>
-      <c r="AB4" s="6"/>
-      <c r="AC4" s="6"/>
-      <c r="AD4" s="6"/>
-      <c r="AE4" s="6"/>
-    </row>
-    <row r="5" spans="1:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6"/>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="6"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="6"/>
-      <c r="AE5" s="6"/>
-    </row>
-    <row r="6" spans="1:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="6"/>
-      <c r="AA6" s="6"/>
-      <c r="AB6" s="6"/>
-      <c r="AC6" s="6"/>
-      <c r="AD6" s="6"/>
-      <c r="AE6" s="6"/>
-    </row>
-    <row r="7" spans="1:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="6"/>
-      <c r="AB7" s="6"/>
-      <c r="AC7" s="6"/>
-      <c r="AD7" s="6"/>
-      <c r="AE7" s="6"/>
-    </row>
-    <row r="8" spans="1:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="6"/>
-      <c r="AB8" s="6"/>
-      <c r="AC8" s="6"/>
-      <c r="AD8" s="6"/>
-      <c r="AE8" s="6"/>
-    </row>
-    <row r="9" spans="1:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="6"/>
-      <c r="AB9" s="6"/>
-      <c r="AC9" s="6"/>
-      <c r="AD9" s="6"/>
-      <c r="AE9" s="6"/>
-    </row>
-    <row r="10" spans="1:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="6"/>
-      <c r="AB10" s="6"/>
-      <c r="AC10" s="6"/>
-      <c r="AD10" s="6"/>
-      <c r="AE10" s="6"/>
-    </row>
-    <row r="11" spans="1:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
-      <c r="AA11" s="6"/>
-      <c r="AB11" s="6"/>
-      <c r="AC11" s="6"/>
-      <c r="AD11" s="6"/>
-      <c r="AE11" s="6"/>
-    </row>
-    <row r="12" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="14:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N17" s="6"/>
-    </row>
-    <row r="18" spans="14:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N18" s="6"/>
-    </row>
-    <row r="19" spans="14:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N19" s="6"/>
-    </row>
-    <row r="20" spans="14:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="14:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="14:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="14:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="14:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="14:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="14:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="14:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="14:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="14:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="14:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="14:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="14:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="2" spans="1:15" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="M2" s="6">
+        <v>2235</v>
+      </c>
+      <c r="N2" s="6">
+        <v>16165</v>
+      </c>
+      <c r="O2" s="6">
+        <v>12855</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="M3" s="6">
+        <v>1033</v>
+      </c>
+      <c r="N3" s="6">
+        <v>6836</v>
+      </c>
+      <c r="O3" s="6">
+        <v>12742</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="M4" s="6">
+        <v>795</v>
+      </c>
+      <c r="N4" s="6">
+        <v>4941</v>
+      </c>
+      <c r="O4" s="6">
+        <v>3666</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="M5" s="6">
+        <v>134</v>
+      </c>
+      <c r="N5" s="6">
+        <v>1187</v>
+      </c>
+      <c r="O5" s="6">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="M6" s="6">
+        <v>572</v>
+      </c>
+      <c r="N6" s="6">
+        <v>2827</v>
+      </c>
+      <c r="O6" s="6">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="M7" s="6">
+        <v>47</v>
+      </c>
+      <c r="N7" s="6">
+        <v>464</v>
+      </c>
+      <c r="O7" s="6">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="M8" s="6">
+        <v>40</v>
+      </c>
+      <c r="N8" s="6">
+        <v>494</v>
+      </c>
+      <c r="O8" s="6">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="M9" s="6">
+        <v>99</v>
+      </c>
+      <c r="N9" s="6">
+        <v>1641</v>
+      </c>
+      <c r="O9" s="6">
+        <v>2961</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M10" s="6">
+        <v>312</v>
+      </c>
+      <c r="N10" s="6">
+        <v>1685</v>
+      </c>
+      <c r="O10" s="6">
+        <v>1689</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="M11" s="6">
+        <v>147</v>
+      </c>
+      <c r="N11" s="6">
+        <v>1436</v>
+      </c>
+      <c r="O11" s="6">
+        <v>2784</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13362,9 +13498,9 @@
   <dimension ref="A1:AA1002"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="H45" sqref="H45"/>
+      <selection pane="bottomLeft" activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14734,7 +14870,7 @@
       <c r="F33" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="G33" s="50" t="s">
+      <c r="G33" s="51" t="s">
         <v>257</v>
       </c>
       <c r="H33" s="42"/>
@@ -15230,7 +15366,7 @@
       <c r="F45" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="G45" s="51" t="s">
+      <c r="G45" s="50" t="s">
         <v>258</v>
       </c>
       <c r="H45" s="44" t="s">

</xml_diff>

<commit_message>
Clarfiy separation between physical sampling and mol-bio/bioinf methods
</commit_message>
<xml_diff>
--- a/molmod/static/downloads/SBDI-ASV-template.xlsx
+++ b/molmod/static/downloads/SBDI-ASV-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/molmod/static/downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7071E71B-0FC3-9A4F-BC7E-45C33B26721D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1352FDDC-9FA7-454C-AFA7-ABE502BC7244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10780" yWindow="8740" windowWidth="38000" windowHeight="14600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10780" yWindow="8720" windowWidth="38000" windowHeight="14600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="302">
   <si>
     <t>event_id_alias</t>
   </si>
@@ -250,9 +250,6 @@
   </si>
   <si>
     <t>'UV light trap', 'mist net', 'bottom trawl', 'ad hoc observation', 'point count', 'Penguins from space: faecal stains reveal the location of emperor penguin colonies, https://doi.org/10.1111/j.1466-8238.2009.00467.x', 'Takats et al. 2001. Guidelines for Nocturnal Owl Monitoring in North America. Beaverhill Bird Observatory and Bird Studies Canada, Edmonton, Alberta. 32 pp.', 'http://www.bsc-eoc.org/download/Owl.pdf'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sampling methods should include sequence processing, e.g. denoising. </t>
   </si>
   <si>
     <t>https://doi.org/10.3389/fmicb.2016.00679</t>
@@ -943,6 +940,16 @@
   <si>
     <t>Use this, simplified, version of emof if you only want to submit measurementType, measurementUnit and measurementValue for some contextual variable, i.e. no additional metadata regarding these. Preferably use variable names and units listed in a relevant GCS Checklist, see https://www.ebi.ac.uk/ena/browser/checklists. Add a single field for every measured variable, and a single row for every event with measured variables(s).</t>
   </si>
+  <si>
+    <t>DNA extraction, PCR, sequencing: https://doi.org/10.3389/fmicb.2016.00679
+Sequence processing/denoising: https://nf-co.re/ampliseq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We suggest that you describe your molecular lab and bioinformatics methods here, and document the method used for taking the material sample under 'samplingProtocol in sheet 'event'. If you refer to a published paper or protocol, however, this may include both types of methods, of course. </t>
+  </si>
+  <si>
+    <t>We suggest that you describe your method for taking the material sample here, and document subsequent molecular lab and bioinformatics steps under 'sop' in sheet 'mixs'. If you refer to a published paper or protocol, however, this may include both types of methods, of course.</t>
+  </si>
 </sst>
 </file>
 
@@ -952,11 +959,18 @@
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1254,133 +1268,139 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1712,16 +1732,16 @@
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>209</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>210</v>
       </c>
       <c r="E2" s="6">
         <v>5414</v>
@@ -1733,10 +1753,10 @@
         <v>13.791</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Q2" s="5">
         <v>3</v>
@@ -1747,16 +1767,16 @@
     </row>
     <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E3" s="6">
         <v>37676</v>
@@ -1768,10 +1788,10 @@
         <v>14.813000000000001</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q3" s="5">
         <v>3</v>
@@ -1793,16 +1813,16 @@
     </row>
     <row r="4" spans="1:30" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E4" s="6">
         <v>41973</v>
@@ -1814,10 +1834,10 @@
         <v>16.649999999999999</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q4" s="5">
         <v>3</v>
@@ -5136,7 +5156,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:V9">
     <sortCondition ref="A3:A9"/>
   </sortState>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -5206,107 +5226,107 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>212</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>213</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>215</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>212</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>213</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>215</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>212</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>213</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F4" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>215</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6288,7 +6308,7 @@
     <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -6349,10 +6369,10 @@
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5">
@@ -6360,7 +6380,7 @@
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -6371,38 +6391,38 @@
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D3" s="5">
         <v>7.23</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D4" s="5">
         <v>6.97</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5">
@@ -6410,21 +6430,21 @@
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D6" s="5">
         <v>17.399999999999999</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -6435,16 +6455,16 @@
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D7" s="5">
         <v>16.899999999999999</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -9606,15 +9626,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B2" s="5">
         <v>7.25</v>
@@ -9625,7 +9645,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B3" s="5">
         <v>7.23</v>
@@ -9636,7 +9656,7 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B4" s="5">
         <v>6.97</v>
@@ -12656,39 +12676,39 @@
         <v>52</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>258</v>
-      </c>
       <c r="I2" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M2" s="5">
         <v>2235</v>
@@ -12702,28 +12722,28 @@
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="D3" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>264</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>265</v>
       </c>
       <c r="M3" s="5">
         <v>1033</v>
@@ -12737,22 +12757,22 @@
     </row>
     <row r="4" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="D4" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>256</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>257</v>
       </c>
       <c r="M4" s="5">
         <v>795</v>
@@ -12766,28 +12786,28 @@
     </row>
     <row r="5" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="D5" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>273</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>274</v>
       </c>
       <c r="M5" s="5">
         <v>134</v>
@@ -12801,28 +12821,28 @@
     </row>
     <row r="6" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="D6" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>276</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>277</v>
       </c>
       <c r="M6" s="5">
         <v>572</v>
@@ -12836,28 +12856,28 @@
     </row>
     <row r="7" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>279</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>273</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>274</v>
       </c>
       <c r="M7" s="5">
         <v>47</v>
@@ -12871,31 +12891,31 @@
     </row>
     <row r="8" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="D8" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="H8" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>285</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>286</v>
       </c>
       <c r="M8" s="5">
         <v>40</v>
@@ -12909,28 +12929,28 @@
     </row>
     <row r="9" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="D9" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>288</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>289</v>
       </c>
       <c r="M9" s="5">
         <v>99</v>
@@ -12944,25 +12964,25 @@
     </row>
     <row r="10" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>291</v>
-      </c>
       <c r="D10" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="H10" s="5" t="s">
         <v>263</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>264</v>
       </c>
       <c r="M10" s="5">
         <v>312</v>
@@ -12976,28 +12996,28 @@
     </row>
     <row r="11" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="D11" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>293</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>294</v>
       </c>
       <c r="M11" s="5">
         <v>147</v>
@@ -13488,9 +13508,9 @@
   <dimension ref="A1:AA1002"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13572,10 +13592,10 @@
         <v>64</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H2" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>
@@ -13615,10 +13635,10 @@
         <v>67</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
@@ -13654,16 +13674,16 @@
         <v>68</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F4" s="27" t="s">
         <v>69</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H4" s="46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
@@ -13702,11 +13722,11 @@
       <c r="F5" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="52" t="s">
+        <v>301</v>
+      </c>
+      <c r="H5" s="47" t="s">
         <v>72</v>
-      </c>
-      <c r="H5" s="47" t="s">
-        <v>73</v>
       </c>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
@@ -13739,14 +13759,14 @@
         <v>63</v>
       </c>
       <c r="D6" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="27" t="s">
         <v>74</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>75</v>
       </c>
       <c r="F6" s="27"/>
       <c r="G6" s="49" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H6" s="41">
         <v>80698</v>
@@ -13779,20 +13799,20 @@
         <v>5</v>
       </c>
       <c r="C7" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>76</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>77</v>
       </c>
       <c r="E7" s="27"/>
       <c r="F7" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="49" t="s">
+        <v>295</v>
+      </c>
+      <c r="H7" s="42" t="s">
         <v>78</v>
-      </c>
-      <c r="G7" s="49" t="s">
-        <v>296</v>
-      </c>
-      <c r="H7" s="42" t="s">
-        <v>79</v>
       </c>
       <c r="I7" s="20"/>
       <c r="J7" s="20"/>
@@ -13825,11 +13845,11 @@
         <v>63</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E8" s="27"/>
       <c r="F8" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G8" s="28"/>
       <c r="H8" s="41"/>
@@ -13864,11 +13884,11 @@
         <v>63</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E9" s="27"/>
       <c r="F9" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G9" s="28"/>
       <c r="H9" s="41"/>
@@ -13903,19 +13923,19 @@
         <v>63</v>
       </c>
       <c r="D10" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="F10" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="G10" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="H10" s="41" t="s">
         <v>87</v>
-      </c>
-      <c r="H10" s="41" t="s">
-        <v>88</v>
       </c>
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
@@ -13945,14 +13965,14 @@
         <v>9</v>
       </c>
       <c r="C11" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="27" t="s">
         <v>89</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>90</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G11" s="28"/>
       <c r="H11" s="41"/>
@@ -13984,22 +14004,22 @@
         <v>10</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D12" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="F12" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="F12" s="27" t="s">
-        <v>94</v>
-      </c>
       <c r="G12" s="49" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H12" s="41" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I12" s="20"/>
       <c r="J12" s="20"/>
@@ -14029,16 +14049,16 @@
         <v>11</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D13" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="F13" s="29" t="s">
         <v>96</v>
-      </c>
-      <c r="F13" s="29" t="s">
-        <v>97</v>
       </c>
       <c r="G13" s="28"/>
       <c r="H13" s="41"/>
@@ -14070,16 +14090,16 @@
         <v>12</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D14" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="F14" s="29" t="s">
         <v>99</v>
-      </c>
-      <c r="F14" s="29" t="s">
-        <v>100</v>
       </c>
       <c r="G14" s="28"/>
       <c r="H14" s="41"/>
@@ -14111,14 +14131,14 @@
         <v>13</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E15" s="27"/>
       <c r="F15" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G15" s="28"/>
       <c r="H15" s="41"/>
@@ -14150,14 +14170,14 @@
         <v>14</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E16" s="27"/>
       <c r="F16" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G16" s="28"/>
       <c r="H16" s="41"/>
@@ -14189,14 +14209,14 @@
         <v>15</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E17" s="27"/>
       <c r="F17" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="41"/>
@@ -14228,14 +14248,14 @@
         <v>16</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E18" s="27"/>
       <c r="F18" s="29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G18" s="28"/>
       <c r="H18" s="41"/>
@@ -14267,14 +14287,14 @@
         <v>17</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E19" s="32"/>
       <c r="F19" s="32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G19" s="33"/>
       <c r="H19" s="43"/>
@@ -14300,7 +14320,7 @@
     </row>
     <row r="20" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>0</v>
@@ -14318,10 +14338,10 @@
         <v>64</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H20" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I20" s="20"/>
       <c r="J20" s="20"/>
@@ -14343,27 +14363,31 @@
       <c r="Z20" s="20"/>
       <c r="AA20" s="20"/>
     </row>
-    <row r="21" spans="1:27" ht="102" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" ht="136" x14ac:dyDescent="0.2">
       <c r="A21" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B21" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D21" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="F21" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="F21" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="G21" s="28"/>
-      <c r="H21" s="41"/>
+      <c r="G21" s="52" t="s">
+        <v>300</v>
+      </c>
+      <c r="H21" s="53" t="s">
+        <v>299</v>
+      </c>
       <c r="I21" s="20"/>
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
@@ -14386,7 +14410,7 @@
     </row>
     <row r="22" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B22" s="26" t="s">
         <v>19</v>
@@ -14395,11 +14419,11 @@
         <v>63</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E22" s="27"/>
       <c r="F22" s="29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G22" s="28"/>
       <c r="H22" s="41"/>
@@ -14425,7 +14449,7 @@
     </row>
     <row r="23" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B23" s="26" t="s">
         <v>20</v>
@@ -14434,11 +14458,11 @@
         <v>63</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E23" s="27"/>
       <c r="F23" s="27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G23" s="28"/>
       <c r="H23" s="41"/>
@@ -14464,7 +14488,7 @@
     </row>
     <row r="24" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B24" s="26" t="s">
         <v>21</v>
@@ -14473,11 +14497,11 @@
         <v>63</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E24" s="27"/>
       <c r="F24" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G24" s="28"/>
       <c r="H24" s="41"/>
@@ -14503,7 +14527,7 @@
     </row>
     <row r="25" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B25" s="26" t="s">
         <v>22</v>
@@ -14512,11 +14536,11 @@
         <v>63</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E25" s="27"/>
       <c r="F25" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G25" s="28"/>
       <c r="H25" s="41"/>
@@ -14542,7 +14566,7 @@
     </row>
     <row r="26" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B26" s="26" t="s">
         <v>23</v>
@@ -14551,11 +14575,11 @@
         <v>63</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E26" s="27"/>
       <c r="F26" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G26" s="28"/>
       <c r="H26" s="41"/>
@@ -14581,7 +14605,7 @@
     </row>
     <row r="27" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B27" s="26" t="s">
         <v>24</v>
@@ -14590,13 +14614,13 @@
         <v>63</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E27" s="27"/>
       <c r="F27" s="27"/>
       <c r="G27" s="28"/>
       <c r="H27" s="41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I27" s="20"/>
       <c r="J27" s="20"/>
@@ -14620,7 +14644,7 @@
     </row>
     <row r="28" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B28" s="26" t="s">
         <v>25</v>
@@ -14629,13 +14653,13 @@
         <v>63</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E28" s="27"/>
       <c r="F28" s="27"/>
       <c r="G28" s="28"/>
       <c r="H28" s="41" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I28" s="20"/>
       <c r="J28" s="20"/>
@@ -14659,7 +14683,7 @@
     </row>
     <row r="29" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B29" s="26" t="s">
         <v>26</v>
@@ -14668,19 +14692,19 @@
         <v>63</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E29" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="F29" s="29" t="s">
         <v>234</v>
       </c>
-      <c r="F29" s="29" t="s">
+      <c r="G29" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="H29" s="41" t="s">
         <v>235</v>
-      </c>
-      <c r="G29" s="28" t="s">
-        <v>249</v>
-      </c>
-      <c r="H29" s="41" t="s">
-        <v>236</v>
       </c>
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
@@ -14704,7 +14728,7 @@
     </row>
     <row r="30" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B30" s="26" t="s">
         <v>27</v>
@@ -14713,19 +14737,19 @@
         <v>63</v>
       </c>
       <c r="D30" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="E30" s="27" t="s">
         <v>238</v>
       </c>
-      <c r="E30" s="27" t="s">
+      <c r="F30" s="27" t="s">
         <v>239</v>
       </c>
-      <c r="F30" s="27" t="s">
+      <c r="G30" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="H30" s="41" t="s">
         <v>240</v>
-      </c>
-      <c r="G30" s="28" t="s">
-        <v>250</v>
-      </c>
-      <c r="H30" s="41" t="s">
-        <v>241</v>
       </c>
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
@@ -14749,7 +14773,7 @@
     </row>
     <row r="31" spans="1:27" ht="154" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B31" s="31" t="s">
         <v>28</v>
@@ -14758,19 +14782,19 @@
         <v>63</v>
       </c>
       <c r="D31" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="E31" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="F31" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="F31" s="32" t="s">
-        <v>131</v>
-      </c>
       <c r="G31" s="33" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H31" s="43" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I31" s="20"/>
       <c r="J31" s="20"/>
@@ -14794,7 +14818,7 @@
     </row>
     <row r="32" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A32" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B32" s="22" t="s">
         <v>0</v>
@@ -14812,10 +14836,10 @@
         <v>64</v>
       </c>
       <c r="G32" s="24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H32" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
@@ -14839,7 +14863,7 @@
     </row>
     <row r="33" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A33" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B33" s="26" t="s">
         <v>30</v>
@@ -14848,16 +14872,16 @@
         <v>63</v>
       </c>
       <c r="D33" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="E33" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="E33" s="27" t="s">
+      <c r="F33" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="F33" s="27" t="s">
-        <v>136</v>
-      </c>
       <c r="G33" s="49" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H33" s="41"/>
       <c r="I33" s="20"/>
@@ -14882,22 +14906,22 @@
     </row>
     <row r="34" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B34" s="26" t="s">
         <v>31</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D34" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="E34" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="E34" s="27" t="s">
+      <c r="F34" s="27" t="s">
         <v>138</v>
-      </c>
-      <c r="F34" s="27" t="s">
-        <v>139</v>
       </c>
       <c r="G34" s="28"/>
       <c r="H34" s="41"/>
@@ -14923,7 +14947,7 @@
     </row>
     <row r="35" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B35" s="26" t="s">
         <v>32</v>
@@ -14932,11 +14956,11 @@
         <v>63</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E35" s="27"/>
       <c r="F35" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G35" s="28"/>
       <c r="H35" s="41"/>
@@ -14962,22 +14986,22 @@
     </row>
     <row r="36" spans="1:27" ht="119" x14ac:dyDescent="0.2">
       <c r="A36" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B36" s="26" t="s">
         <v>33</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D36" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="E36" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="E36" s="27" t="s">
+      <c r="F36" s="27" t="s">
         <v>143</v>
-      </c>
-      <c r="F36" s="27" t="s">
-        <v>144</v>
       </c>
       <c r="G36" s="28"/>
       <c r="H36" s="41"/>
@@ -15003,22 +15027,22 @@
     </row>
     <row r="37" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A37" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B37" s="26" t="s">
         <v>34</v>
       </c>
       <c r="C37" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="D37" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="D37" s="27" t="s">
+      <c r="E37" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="E37" s="27" t="s">
+      <c r="F37" s="27" t="s">
         <v>147</v>
-      </c>
-      <c r="F37" s="27" t="s">
-        <v>148</v>
       </c>
       <c r="G37" s="28"/>
       <c r="H37" s="41"/>
@@ -15044,22 +15068,22 @@
     </row>
     <row r="38" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A38" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B38" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D38" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="E38" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="E38" s="27" t="s">
+      <c r="F38" s="27" t="s">
         <v>150</v>
-      </c>
-      <c r="F38" s="27" t="s">
-        <v>151</v>
       </c>
       <c r="G38" s="28"/>
       <c r="H38" s="41"/>
@@ -15085,22 +15109,22 @@
     </row>
     <row r="39" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B39" s="26" t="s">
         <v>36</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D39" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="E39" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="E39" s="27" t="s">
+      <c r="F39" s="27" t="s">
         <v>153</v>
-      </c>
-      <c r="F39" s="27" t="s">
-        <v>154</v>
       </c>
       <c r="G39" s="28"/>
       <c r="H39" s="41"/>
@@ -15126,22 +15150,22 @@
     </row>
     <row r="40" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A40" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B40" s="26" t="s">
         <v>37</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D40" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="E40" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="E40" s="27" t="s">
+      <c r="F40" s="27" t="s">
         <v>156</v>
-      </c>
-      <c r="F40" s="27" t="s">
-        <v>157</v>
       </c>
       <c r="G40" s="28"/>
       <c r="H40" s="41"/>
@@ -15167,22 +15191,22 @@
     </row>
     <row r="41" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A41" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B41" s="26" t="s">
         <v>38</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D41" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="E41" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="E41" s="27" t="s">
+      <c r="F41" s="27" t="s">
         <v>159</v>
-      </c>
-      <c r="F41" s="27" t="s">
-        <v>160</v>
       </c>
       <c r="G41" s="28"/>
       <c r="H41" s="41"/>
@@ -15208,22 +15232,22 @@
     </row>
     <row r="42" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A42" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B42" s="26" t="s">
         <v>39</v>
       </c>
       <c r="C42" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D42" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="E42" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="E42" s="27" t="s">
+      <c r="F42" s="27" t="s">
         <v>162</v>
-      </c>
-      <c r="F42" s="27" t="s">
-        <v>163</v>
       </c>
       <c r="G42" s="28"/>
       <c r="H42" s="41"/>
@@ -15249,22 +15273,22 @@
     </row>
     <row r="43" spans="1:27" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B43" s="31" t="s">
         <v>40</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D43" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="E43" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="E43" s="32" t="s">
+      <c r="F43" s="32" t="s">
         <v>165</v>
-      </c>
-      <c r="F43" s="32" t="s">
-        <v>166</v>
       </c>
       <c r="G43" s="33"/>
       <c r="H43" s="43"/>
@@ -15290,7 +15314,7 @@
     </row>
     <row r="44" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A44" s="21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B44" s="22" t="s">
         <v>0</v>
@@ -15308,10 +15332,10 @@
         <v>64</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H44" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I44" s="20"/>
       <c r="J44" s="20"/>
@@ -15335,10 +15359,10 @@
     </row>
     <row r="45" spans="1:27" ht="205" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="30" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C45" s="31" t="s">
         <v>64</v>
@@ -15353,10 +15377,10 @@
         <v>64</v>
       </c>
       <c r="G45" s="50" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H45" s="43" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I45" s="20"/>
       <c r="J45" s="20"/>
@@ -15380,10 +15404,10 @@
     </row>
     <row r="46" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B46" s="22" t="s">
         <v>167</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>168</v>
       </c>
       <c r="C46" s="35" t="s">
         <v>63</v>
@@ -15398,10 +15422,10 @@
         <v>64</v>
       </c>
       <c r="G46" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="H46" s="40" t="s">
         <v>169</v>
-      </c>
-      <c r="H46" s="40" t="s">
-        <v>170</v>
       </c>
       <c r="I46" s="20"/>
       <c r="J46" s="20"/>
@@ -15425,10 +15449,10 @@
     </row>
     <row r="47" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A47" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="B47" s="22" t="s">
         <v>171</v>
-      </c>
-      <c r="B47" s="22" t="s">
-        <v>172</v>
       </c>
       <c r="C47" s="22" t="s">
         <v>63</v>
@@ -15443,10 +15467,10 @@
         <v>64</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H47" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
@@ -15470,25 +15494,25 @@
     </row>
     <row r="48" spans="1:27" ht="119" x14ac:dyDescent="0.2">
       <c r="A48" s="36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C48" s="26" t="s">
         <v>63</v>
       </c>
       <c r="D48" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="E48" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="E48" s="27" t="s">
+      <c r="F48" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="F48" s="27" t="s">
+      <c r="G48" s="28" t="s">
         <v>176</v>
-      </c>
-      <c r="G48" s="28" t="s">
-        <v>177</v>
       </c>
       <c r="H48" s="41">
         <v>486</v>
@@ -15515,7 +15539,7 @@
     </row>
     <row r="49" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A49" s="36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B49" s="26" t="s">
         <v>42</v>
@@ -15524,15 +15548,15 @@
         <v>63</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E49" s="27"/>
       <c r="F49" s="27"/>
       <c r="G49" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="H49" s="41" t="s">
         <v>179</v>
-      </c>
-      <c r="H49" s="41" t="s">
-        <v>180</v>
       </c>
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
@@ -15556,26 +15580,26 @@
     </row>
     <row r="50" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A50" s="36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B50" s="26" t="s">
         <v>43</v>
       </c>
       <c r="C50" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E50" s="27"/>
       <c r="F50" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G50" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="H50" s="41" t="s">
         <v>202</v>
-      </c>
-      <c r="H50" s="41" t="s">
-        <v>203</v>
       </c>
       <c r="I50" s="20"/>
       <c r="J50" s="20"/>
@@ -15599,7 +15623,7 @@
     </row>
     <row r="51" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A51" s="36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B51" s="26" t="s">
         <v>44</v>
@@ -15608,14 +15632,14 @@
         <v>63</v>
       </c>
       <c r="D51" s="27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E51" s="27"/>
       <c r="F51" s="27" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G51" s="48" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H51" s="41"/>
       <c r="I51" s="20"/>
@@ -15640,20 +15664,20 @@
     </row>
     <row r="52" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B52" s="26" t="s">
         <v>45</v>
       </c>
       <c r="C52" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="D52" s="27" t="s">
         <v>185</v>
-      </c>
-      <c r="D52" s="27" t="s">
-        <v>186</v>
       </c>
       <c r="E52" s="27"/>
       <c r="F52" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G52" s="28"/>
       <c r="H52" s="41"/>
@@ -15679,20 +15703,20 @@
     </row>
     <row r="53" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B53" s="26" t="s">
         <v>46</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E53" s="27"/>
       <c r="F53" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G53" s="28"/>
       <c r="H53" s="41"/>
@@ -15718,20 +15742,20 @@
     </row>
     <row r="54" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B54" s="26" t="s">
         <v>47</v>
       </c>
       <c r="C54" s="26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D54" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E54" s="27"/>
       <c r="F54" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G54" s="28"/>
       <c r="H54" s="41"/>
@@ -15757,20 +15781,20 @@
     </row>
     <row r="55" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B55" s="26" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E55" s="27"/>
       <c r="F55" s="27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G55" s="28"/>
       <c r="H55" s="41"/>
@@ -15796,20 +15820,20 @@
     </row>
     <row r="56" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" s="36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B56" s="26" t="s">
         <v>49</v>
       </c>
       <c r="C56" s="26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E56" s="27"/>
       <c r="F56" s="27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G56" s="28"/>
       <c r="H56" s="41"/>
@@ -15835,20 +15859,20 @@
     </row>
     <row r="57" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" s="36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B57" s="26" t="s">
         <v>50</v>
       </c>
       <c r="C57" s="26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D57" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E57" s="27"/>
       <c r="F57" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G57" s="28"/>
       <c r="H57" s="41"/>
@@ -15874,23 +15898,23 @@
     </row>
     <row r="58" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A58" s="36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B58" s="26" t="s">
         <v>51</v>
       </c>
       <c r="C58" s="26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D58" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E58" s="27"/>
       <c r="F58" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="G58" s="28" t="s">
         <v>199</v>
-      </c>
-      <c r="G58" s="28" t="s">
-        <v>200</v>
       </c>
       <c r="H58" s="41"/>
       <c r="I58" s="20"/>
@@ -15915,13 +15939,13 @@
     </row>
     <row r="59" spans="1:27" ht="103" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B59" s="31" t="s">
         <v>52</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D59" s="31" t="s">
         <v>64</v>
@@ -15933,7 +15957,7 @@
         <v>64</v>
       </c>
       <c r="G59" s="33" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H59" s="43" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Restore note on adding molbio/bioinf to samplingProtocol + add seq_meth
IPT warns about wrong format when sop is fed free text. And sop is 
currently only shown in dynamicProperties (JSON) so should be kept short 
anyway
</commit_message>
<xml_diff>
--- a/molmod/static/downloads/SBDI-ASV-template.xlsx
+++ b/molmod/static/downloads/SBDI-ASV-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/molmod/static/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0BE70B-9676-4B49-B4A9-308A0E5F02C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C2FA5C-E98C-9C46-AA60-0C56BFF18DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10780" yWindow="8720" windowWidth="38000" windowHeight="14600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7360" yWindow="9760" windowWidth="38000" windowHeight="14600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="guide" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">guide!$A$1:$AA$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">guide!$A$1:$AA$60</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="302">
   <si>
     <t>event_id_alias</t>
   </si>
@@ -250,9 +250,6 @@
   </si>
   <si>
     <t>'UV light trap', 'mist net', 'bottom trawl', 'ad hoc observation', 'point count', 'Penguins from space: faecal stains reveal the location of emperor penguin colonies, https://doi.org/10.1111/j.1466-8238.2009.00467.x', 'Takats et al. 2001. Guidelines for Nocturnal Owl Monitoring in North America. Beaverhill Bird Observatory and Bird Studies Canada, Edmonton, Alberta. 32 pp.', 'http://www.bsc-eoc.org/download/Owl.pdf'</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.3389/fmicb.2016.00679</t>
   </si>
   <si>
     <t xml:space="preserve">A numeric value for a measurement of the size (time duration, length, area, or volume) of a sample in a sampling event. </t>
@@ -941,14 +938,16 @@
     <t>Use this, simplified, version of emof if you only want to submit measurementType, measurementUnit and measurementValue for some contextual variable, i.e. no additional metadata regarding these. Preferably use variable names and units listed in a relevant GCS Checklist, see https://www.ebi.ac.uk/ena/browser/checklists. Add a single field for every measured variable, and a single row for every event with measured variables(s).</t>
   </si>
   <si>
-    <t>DNA extraction, PCR, sequencing: https://doi.org/10.3389/fmicb.2016.00679
-Sequence processing/denoising: https://nf-co.re/ampliseq</t>
+    <t>Include your method for taking the material sample, as well as subsequent molecular lab and bioinformatics steps, e.g. sequencing and denoising procedures.</t>
   </si>
   <si>
-    <t>We suggest that you describe your method for taking the material sample here, and document subsequent molecular lab and bioinformatics steps under 'sop' in sheet 'mixs'. If you refer to a published paper or protocol, however, this may include all methods, of course.</t>
+    <t>seq_meth</t>
   </si>
   <si>
-    <t>We suggest that you describe your molecular lab and bioinformatics methods here, and document the method used for taking the material sample under 'samplingProtocol' in sheet 'event'. If you refer to a published paper or protocol, however, this may include all methods, of course.</t>
+    <t>Illumina HiSeq 1500'</t>
+  </si>
+  <si>
+    <t>Sequencing method used</t>
   </si>
 </sst>
 </file>
@@ -959,18 +958,11 @@
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1275,139 +1267,148 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1739,16 +1740,16 @@
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>208</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>209</v>
       </c>
       <c r="E2" s="6">
         <v>5414</v>
@@ -1760,10 +1761,10 @@
         <v>13.791</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q2" s="5">
         <v>3</v>
@@ -1774,16 +1775,16 @@
     </row>
     <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E3" s="6">
         <v>37676</v>
@@ -1795,10 +1796,10 @@
         <v>14.813000000000001</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Q3" s="5">
         <v>3</v>
@@ -1820,16 +1821,16 @@
     </row>
     <row r="4" spans="1:30" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E4" s="6">
         <v>41973</v>
@@ -1841,10 +1842,10 @@
         <v>16.649999999999999</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Q4" s="5">
         <v>3</v>
@@ -5163,7 +5164,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:V9">
     <sortCondition ref="A3:A9"/>
   </sortState>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -5233,107 +5234,107 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>212</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>214</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>212</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>214</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>212</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F4" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>214</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6315,7 +6316,7 @@
     <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -6376,10 +6377,10 @@
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5">
@@ -6387,7 +6388,7 @@
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -6398,38 +6399,38 @@
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D3" s="5">
         <v>7.23</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D4" s="5">
         <v>6.97</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5">
@@ -6437,21 +6438,21 @@
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D6" s="5">
         <v>17.399999999999999</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -6462,16 +6463,16 @@
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D7" s="5">
         <v>16.899999999999999</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -9633,15 +9634,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B2" s="5">
         <v>7.25</v>
@@ -9652,7 +9653,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B3" s="5">
         <v>7.23</v>
@@ -9663,7 +9664,7 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B4" s="5">
         <v>6.97</v>
@@ -12683,39 +12684,39 @@
         <v>52</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>257</v>
-      </c>
       <c r="I2" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M2" s="5">
         <v>2235</v>
@@ -12729,28 +12730,28 @@
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="D3" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>263</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>264</v>
       </c>
       <c r="M3" s="5">
         <v>1033</v>
@@ -12764,22 +12765,22 @@
     </row>
     <row r="4" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>266</v>
-      </c>
       <c r="D4" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>255</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>256</v>
       </c>
       <c r="M4" s="5">
         <v>795</v>
@@ -12793,28 +12794,28 @@
     </row>
     <row r="5" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="D5" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>272</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>273</v>
       </c>
       <c r="M5" s="5">
         <v>134</v>
@@ -12828,28 +12829,28 @@
     </row>
     <row r="6" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="D6" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>275</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>276</v>
       </c>
       <c r="M6" s="5">
         <v>572</v>
@@ -12863,28 +12864,28 @@
     </row>
     <row r="7" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>278</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>272</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>273</v>
       </c>
       <c r="M7" s="5">
         <v>47</v>
@@ -12898,31 +12899,31 @@
     </row>
     <row r="8" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="D8" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="H8" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>284</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>285</v>
       </c>
       <c r="M8" s="5">
         <v>40</v>
@@ -12936,28 +12937,28 @@
     </row>
     <row r="9" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="D9" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>287</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>288</v>
       </c>
       <c r="M9" s="5">
         <v>99</v>
@@ -12971,25 +12972,25 @@
     </row>
     <row r="10" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>290</v>
-      </c>
       <c r="D10" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="H10" s="5" t="s">
         <v>262</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>263</v>
       </c>
       <c r="M10" s="5">
         <v>312</v>
@@ -13003,28 +13004,28 @@
     </row>
     <row r="11" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="D11" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>292</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>293</v>
       </c>
       <c r="M11" s="5">
         <v>147</v>
@@ -13512,12 +13513,12 @@
   <sheetPr>
     <tabColor rgb="FFD6E3BC"/>
   </sheetPr>
-  <dimension ref="A1:AA1002"/>
+  <dimension ref="A1:AA1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13599,10 +13600,10 @@
         <v>64</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H2" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>
@@ -13642,10 +13643,10 @@
         <v>67</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
@@ -13681,16 +13682,16 @@
         <v>68</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F4" s="27" t="s">
         <v>69</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H4" s="46" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
@@ -13729,12 +13730,10 @@
       <c r="F5" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="G5" s="53" t="s">
-        <v>300</v>
-      </c>
-      <c r="H5" s="47" t="s">
-        <v>72</v>
-      </c>
+      <c r="G5" s="52" t="s">
+        <v>298</v>
+      </c>
+      <c r="H5" s="47"/>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
@@ -13766,14 +13765,14 @@
         <v>63</v>
       </c>
       <c r="D6" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="27" t="s">
         <v>73</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>74</v>
       </c>
       <c r="F6" s="27"/>
       <c r="G6" s="49" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H6" s="41">
         <v>80698</v>
@@ -13806,20 +13805,20 @@
         <v>5</v>
       </c>
       <c r="C7" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>75</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>76</v>
       </c>
       <c r="E7" s="27"/>
       <c r="F7" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="49" t="s">
+        <v>294</v>
+      </c>
+      <c r="H7" s="42" t="s">
         <v>77</v>
-      </c>
-      <c r="G7" s="49" t="s">
-        <v>295</v>
-      </c>
-      <c r="H7" s="42" t="s">
-        <v>78</v>
       </c>
       <c r="I7" s="20"/>
       <c r="J7" s="20"/>
@@ -13852,11 +13851,11 @@
         <v>63</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E8" s="27"/>
       <c r="F8" s="27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G8" s="28"/>
       <c r="H8" s="41"/>
@@ -13891,11 +13890,11 @@
         <v>63</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E9" s="27"/>
       <c r="F9" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G9" s="28"/>
       <c r="H9" s="41"/>
@@ -13930,19 +13929,19 @@
         <v>63</v>
       </c>
       <c r="D10" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="F10" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="G10" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="H10" s="41" t="s">
         <v>86</v>
-      </c>
-      <c r="H10" s="41" t="s">
-        <v>87</v>
       </c>
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
@@ -13972,14 +13971,14 @@
         <v>9</v>
       </c>
       <c r="C11" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="27" t="s">
         <v>88</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>89</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G11" s="28"/>
       <c r="H11" s="41"/>
@@ -14011,22 +14010,22 @@
         <v>10</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D12" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="F12" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="F12" s="27" t="s">
-        <v>93</v>
-      </c>
       <c r="G12" s="49" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H12" s="41" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I12" s="20"/>
       <c r="J12" s="20"/>
@@ -14056,16 +14055,16 @@
         <v>11</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D13" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="F13" s="29" t="s">
         <v>95</v>
-      </c>
-      <c r="F13" s="29" t="s">
-        <v>96</v>
       </c>
       <c r="G13" s="28"/>
       <c r="H13" s="41"/>
@@ -14097,16 +14096,16 @@
         <v>12</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D14" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="F14" s="29" t="s">
         <v>98</v>
-      </c>
-      <c r="F14" s="29" t="s">
-        <v>99</v>
       </c>
       <c r="G14" s="28"/>
       <c r="H14" s="41"/>
@@ -14138,14 +14137,14 @@
         <v>13</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E15" s="27"/>
       <c r="F15" s="29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G15" s="28"/>
       <c r="H15" s="41"/>
@@ -14177,14 +14176,14 @@
         <v>14</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E16" s="27"/>
       <c r="F16" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G16" s="28"/>
       <c r="H16" s="41"/>
@@ -14216,14 +14215,14 @@
         <v>15</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E17" s="27"/>
       <c r="F17" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="41"/>
@@ -14255,14 +14254,14 @@
         <v>16</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E18" s="27"/>
       <c r="F18" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G18" s="28"/>
       <c r="H18" s="41"/>
@@ -14294,14 +14293,14 @@
         <v>17</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E19" s="32"/>
       <c r="F19" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G19" s="33"/>
       <c r="H19" s="43"/>
@@ -14327,7 +14326,7 @@
     </row>
     <row r="20" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>0</v>
@@ -14345,10 +14344,10 @@
         <v>64</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H20" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I20" s="20"/>
       <c r="J20" s="20"/>
@@ -14370,31 +14369,27 @@
       <c r="Z20" s="20"/>
       <c r="AA20" s="20"/>
     </row>
-    <row r="21" spans="1:27" ht="136" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A21" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B21" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D21" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E21" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="F21" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="F21" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="G21" s="53" t="s">
-        <v>301</v>
-      </c>
-      <c r="H21" s="52" t="s">
-        <v>299</v>
-      </c>
+      <c r="G21" s="28"/>
+      <c r="H21" s="41"/>
       <c r="I21" s="20"/>
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
@@ -14417,7 +14412,7 @@
     </row>
     <row r="22" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B22" s="26" t="s">
         <v>19</v>
@@ -14426,11 +14421,11 @@
         <v>63</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E22" s="27"/>
       <c r="F22" s="29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G22" s="28"/>
       <c r="H22" s="41"/>
@@ -14456,7 +14451,7 @@
     </row>
     <row r="23" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B23" s="26" t="s">
         <v>20</v>
@@ -14465,11 +14460,11 @@
         <v>63</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E23" s="27"/>
       <c r="F23" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G23" s="28"/>
       <c r="H23" s="41"/>
@@ -14495,7 +14490,7 @@
     </row>
     <row r="24" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B24" s="26" t="s">
         <v>21</v>
@@ -14504,11 +14499,11 @@
         <v>63</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E24" s="27"/>
       <c r="F24" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G24" s="28"/>
       <c r="H24" s="41"/>
@@ -14533,21 +14528,21 @@
       <c r="AA24" s="20"/>
     </row>
     <row r="25" spans="1:27" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="26" t="s">
+      <c r="A25" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="53" t="s">
+        <v>299</v>
+      </c>
+      <c r="C25" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="27" t="s">
-        <v>120</v>
+      <c r="D25" s="55" t="s">
+        <v>301</v>
       </c>
       <c r="E25" s="27"/>
-      <c r="F25" s="27" t="s">
-        <v>121</v>
+      <c r="F25" s="56" t="s">
+        <v>300</v>
       </c>
       <c r="G25" s="28"/>
       <c r="H25" s="41"/>
@@ -14573,20 +14568,20 @@
     </row>
     <row r="26" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C26" s="26" t="s">
         <v>63</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E26" s="27"/>
       <c r="F26" s="27" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G26" s="28"/>
       <c r="H26" s="41"/>
@@ -14610,25 +14605,25 @@
       <c r="Z26" s="20"/>
       <c r="AA26" s="20"/>
     </row>
-    <row r="27" spans="1:27" ht="34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" s="26" t="s">
         <v>63</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
+      <c r="F27" s="27" t="s">
+        <v>122</v>
+      </c>
       <c r="G27" s="28"/>
-      <c r="H27" s="41" t="s">
-        <v>125</v>
-      </c>
+      <c r="H27" s="41"/>
       <c r="I27" s="20"/>
       <c r="J27" s="20"/>
       <c r="K27" s="20"/>
@@ -14651,22 +14646,22 @@
     </row>
     <row r="28" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="26" t="s">
         <v>63</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E28" s="27"/>
       <c r="F28" s="27"/>
       <c r="G28" s="28"/>
       <c r="H28" s="41" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I28" s="20"/>
       <c r="J28" s="20"/>
@@ -14688,30 +14683,24 @@
       <c r="Z28" s="20"/>
       <c r="AA28" s="20"/>
     </row>
-    <row r="29" spans="1:27" ht="204" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C29" s="26" t="s">
         <v>63</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="E29" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="F29" s="29" t="s">
-        <v>234</v>
-      </c>
-      <c r="G29" s="28" t="s">
-        <v>248</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="28"/>
       <c r="H29" s="41" t="s">
-        <v>235</v>
+        <v>126</v>
       </c>
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
@@ -14735,28 +14724,28 @@
     </row>
     <row r="30" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C30" s="26" t="s">
         <v>63</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>238</v>
-      </c>
-      <c r="F30" s="27" t="s">
-        <v>239</v>
+        <v>232</v>
+      </c>
+      <c r="F30" s="29" t="s">
+        <v>233</v>
       </c>
       <c r="G30" s="28" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H30" s="41" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
@@ -14778,30 +14767,30 @@
       <c r="Z30" s="20"/>
       <c r="AA30" s="20"/>
     </row>
-    <row r="31" spans="1:27" ht="154" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="B31" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="31" t="s">
+    <row r="31" spans="1:27" ht="204" x14ac:dyDescent="0.2">
+      <c r="A31" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="E31" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="F31" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="G31" s="33" t="s">
-        <v>250</v>
-      </c>
-      <c r="H31" s="43" t="s">
-        <v>241</v>
+      <c r="D31" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="F31" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="G31" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="H31" s="41" t="s">
+        <v>239</v>
       </c>
       <c r="I31" s="20"/>
       <c r="J31" s="20"/>
@@ -14823,30 +14812,30 @@
       <c r="Z31" s="20"/>
       <c r="AA31" s="20"/>
     </row>
-    <row r="32" spans="1:27" ht="68" x14ac:dyDescent="0.2">
-      <c r="A32" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="E32" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="F32" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="G32" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="H32" s="40" t="s">
-        <v>205</v>
+    <row r="32" spans="1:27" ht="154" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="G32" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="H32" s="43" t="s">
+        <v>240</v>
       </c>
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
@@ -14868,29 +14857,31 @@
       <c r="Z32" s="20"/>
       <c r="AA32" s="20"/>
     </row>
-    <row r="33" spans="1:27" ht="204" x14ac:dyDescent="0.2">
-      <c r="A33" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="B33" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="E33" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="F33" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="G33" s="49" t="s">
-        <v>297</v>
-      </c>
-      <c r="H33" s="41"/>
+    <row r="33" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+      <c r="A33" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="E33" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="G33" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H33" s="40" t="s">
+        <v>204</v>
+      </c>
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
       <c r="K33" s="20"/>
@@ -14911,26 +14902,28 @@
       <c r="Z33" s="20"/>
       <c r="AA33" s="20"/>
     </row>
-    <row r="34" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A34" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="B34" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D34" s="27" t="s">
-        <v>136</v>
-      </c>
       <c r="E34" s="27" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F34" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="G34" s="28"/>
+        <v>134</v>
+      </c>
+      <c r="G34" s="49" t="s">
+        <v>296</v>
+      </c>
       <c r="H34" s="41"/>
       <c r="I34" s="20"/>
       <c r="J34" s="20"/>
@@ -14952,22 +14945,24 @@
       <c r="Z34" s="20"/>
       <c r="AA34" s="20"/>
     </row>
-    <row r="35" spans="1:27" ht="34" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="E35" s="27"/>
+        <v>135</v>
+      </c>
+      <c r="E35" s="27" t="s">
+        <v>136</v>
+      </c>
       <c r="F35" s="27" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G35" s="28"/>
       <c r="H35" s="41"/>
@@ -14991,24 +14986,22 @@
       <c r="Z35" s="20"/>
       <c r="AA35" s="20"/>
     </row>
-    <row r="36" spans="1:27" ht="119" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="E36" s="27" t="s">
-        <v>142</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="E36" s="27"/>
       <c r="F36" s="27" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G36" s="28"/>
       <c r="H36" s="41"/>
@@ -15032,24 +15025,24 @@
       <c r="Z36" s="20"/>
       <c r="AA36" s="20"/>
     </row>
-    <row r="37" spans="1:27" ht="85" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" ht="119" x14ac:dyDescent="0.2">
       <c r="A37" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>144</v>
+        <v>74</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F37" s="27" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G37" s="28"/>
       <c r="H37" s="41"/>
@@ -15073,24 +15066,24 @@
       <c r="Z37" s="20"/>
       <c r="AA37" s="20"/>
     </row>
-    <row r="38" spans="1:27" ht="102" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A38" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>75</v>
+        <v>143</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F38" s="27" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G38" s="28"/>
       <c r="H38" s="41"/>
@@ -15114,24 +15107,24 @@
       <c r="Z38" s="20"/>
       <c r="AA38" s="20"/>
     </row>
-    <row r="39" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A39" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E39" s="27" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F39" s="27" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G39" s="28"/>
       <c r="H39" s="41"/>
@@ -15155,24 +15148,24 @@
       <c r="Z39" s="20"/>
       <c r="AA39" s="20"/>
     </row>
-    <row r="40" spans="1:27" ht="102" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F40" s="27" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G40" s="28"/>
       <c r="H40" s="41"/>
@@ -15196,24 +15189,24 @@
       <c r="Z40" s="20"/>
       <c r="AA40" s="20"/>
     </row>
-    <row r="41" spans="1:27" ht="85" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A41" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E41" s="27" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F41" s="27" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G41" s="28"/>
       <c r="H41" s="41"/>
@@ -15237,24 +15230,24 @@
       <c r="Z41" s="20"/>
       <c r="AA41" s="20"/>
     </row>
-    <row r="42" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A42" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C42" s="26" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F42" s="27" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G42" s="28"/>
       <c r="H42" s="41"/>
@@ -15278,27 +15271,27 @@
       <c r="Z42" s="20"/>
       <c r="AA42" s="20"/>
     </row>
-    <row r="43" spans="1:27" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="B43" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C43" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="D43" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="E43" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="F43" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="G43" s="33"/>
-      <c r="H43" s="43"/>
+    <row r="43" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+      <c r="A43" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="E43" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="F43" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="G43" s="28"/>
+      <c r="H43" s="41"/>
       <c r="I43" s="20"/>
       <c r="J43" s="20"/>
       <c r="K43" s="20"/>
@@ -15319,31 +15312,27 @@
       <c r="Z43" s="20"/>
       <c r="AA43" s="20"/>
     </row>
-    <row r="44" spans="1:27" ht="68" x14ac:dyDescent="0.2">
-      <c r="A44" s="21" t="s">
-        <v>226</v>
-      </c>
-      <c r="B44" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="D44" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="E44" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="F44" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="G44" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="H44" s="40" t="s">
-        <v>205</v>
-      </c>
+    <row r="44" spans="1:27" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="B44" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="E44" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="F44" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="G44" s="33"/>
+      <c r="H44" s="43"/>
       <c r="I44" s="20"/>
       <c r="J44" s="20"/>
       <c r="K44" s="20"/>
@@ -15364,30 +15353,30 @@
       <c r="Z44" s="20"/>
       <c r="AA44" s="20"/>
     </row>
-    <row r="45" spans="1:27" ht="205" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="30" t="s">
-        <v>228</v>
-      </c>
-      <c r="B45" s="31" t="s">
-        <v>227</v>
-      </c>
-      <c r="C45" s="31" t="s">
+    <row r="45" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+      <c r="A45" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="D45" s="38" t="s">
+      <c r="D45" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="38" t="s">
+      <c r="E45" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="F45" s="38" t="s">
+      <c r="F45" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="G45" s="50" t="s">
-        <v>298</v>
-      </c>
-      <c r="H45" s="43" t="s">
-        <v>245</v>
+      <c r="G45" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H45" s="40" t="s">
+        <v>204</v>
       </c>
       <c r="I45" s="20"/>
       <c r="J45" s="20"/>
@@ -15409,30 +15398,30 @@
       <c r="Z45" s="20"/>
       <c r="AA45" s="20"/>
     </row>
-    <row r="46" spans="1:27" ht="51" x14ac:dyDescent="0.2">
-      <c r="A46" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="C46" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="D46" s="35" t="s">
+    <row r="46" spans="1:27" ht="205" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="B46" s="31" t="s">
+        <v>226</v>
+      </c>
+      <c r="C46" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="E46" s="35" t="s">
+      <c r="D46" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="F46" s="35" t="s">
+      <c r="E46" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="G46" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="H46" s="40" t="s">
-        <v>169</v>
+      <c r="F46" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="G46" s="50" t="s">
+        <v>297</v>
+      </c>
+      <c r="H46" s="43" t="s">
+        <v>244</v>
       </c>
       <c r="I46" s="20"/>
       <c r="J46" s="20"/>
@@ -15454,30 +15443,30 @@
       <c r="Z46" s="20"/>
       <c r="AA46" s="20"/>
     </row>
-    <row r="47" spans="1:27" ht="68" x14ac:dyDescent="0.2">
-      <c r="A47" s="36" t="s">
-        <v>170</v>
+    <row r="47" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+      <c r="A47" s="21" t="s">
+        <v>165</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="C47" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="C47" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="D47" s="23" t="s">
+      <c r="D47" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="E47" s="23" t="s">
+      <c r="E47" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="F47" s="23" t="s">
+      <c r="F47" s="35" t="s">
         <v>64</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>247</v>
+        <v>167</v>
       </c>
       <c r="H47" s="40" t="s">
-        <v>205</v>
+        <v>168</v>
       </c>
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
@@ -15499,30 +15488,30 @@
       <c r="Z47" s="20"/>
       <c r="AA47" s="20"/>
     </row>
-    <row r="48" spans="1:27" ht="119" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A48" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="B48" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="B48" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D48" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="E48" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="F48" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="G48" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="H48" s="41">
-        <v>486</v>
+      <c r="D48" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E48" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F48" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G48" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H48" s="40" t="s">
+        <v>204</v>
       </c>
       <c r="I48" s="20"/>
       <c r="J48" s="20"/>
@@ -15544,26 +15533,30 @@
       <c r="Z48" s="20"/>
       <c r="AA48" s="20"/>
     </row>
-    <row r="49" spans="1:27" ht="204" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:27" ht="119" x14ac:dyDescent="0.2">
       <c r="A49" s="36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>42</v>
+        <v>171</v>
       </c>
       <c r="C49" s="26" t="s">
         <v>63</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>177</v>
-      </c>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
+        <v>172</v>
+      </c>
+      <c r="E49" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="F49" s="27" t="s">
+        <v>174</v>
+      </c>
       <c r="G49" s="28" t="s">
-        <v>178</v>
-      </c>
-      <c r="H49" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
+      </c>
+      <c r="H49" s="41">
+        <v>486</v>
       </c>
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
@@ -15585,28 +15578,26 @@
       <c r="Z49" s="20"/>
       <c r="AA49" s="20"/>
     </row>
-    <row r="50" spans="1:27" ht="102" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A50" s="36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C50" s="26" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E50" s="27"/>
-      <c r="F50" s="27" t="s">
-        <v>181</v>
-      </c>
+      <c r="F50" s="27"/>
       <c r="G50" s="28" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="H50" s="41" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="I50" s="20"/>
       <c r="J50" s="20"/>
@@ -15628,27 +15619,29 @@
       <c r="Z50" s="20"/>
       <c r="AA50" s="20"/>
     </row>
-    <row r="51" spans="1:27" ht="85" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A51" s="36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="D51" s="27" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E51" s="27"/>
       <c r="F51" s="27" t="s">
-        <v>183</v>
-      </c>
-      <c r="G51" s="48" t="s">
-        <v>246</v>
-      </c>
-      <c r="H51" s="41"/>
+        <v>180</v>
+      </c>
+      <c r="G51" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="H51" s="41" t="s">
+        <v>201</v>
+      </c>
       <c r="I51" s="20"/>
       <c r="J51" s="20"/>
       <c r="K51" s="20"/>
@@ -15669,24 +15662,26 @@
       <c r="Z51" s="20"/>
       <c r="AA51" s="20"/>
     </row>
-    <row r="52" spans="1:27" ht="34" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A52" s="36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C52" s="26" t="s">
-        <v>184</v>
+        <v>63</v>
       </c>
       <c r="D52" s="27" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E52" s="27"/>
       <c r="F52" s="27" t="s">
-        <v>186</v>
-      </c>
-      <c r="G52" s="28"/>
+        <v>182</v>
+      </c>
+      <c r="G52" s="48" t="s">
+        <v>245</v>
+      </c>
       <c r="H52" s="41"/>
       <c r="I52" s="20"/>
       <c r="J52" s="20"/>
@@ -15710,20 +15705,20 @@
     </row>
     <row r="53" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C53" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="D53" s="27" t="s">
         <v>184</v>
-      </c>
-      <c r="D53" s="27" t="s">
-        <v>187</v>
       </c>
       <c r="E53" s="27"/>
       <c r="F53" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G53" s="28"/>
       <c r="H53" s="41"/>
@@ -15749,20 +15744,20 @@
     </row>
     <row r="54" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C54" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D54" s="27" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E54" s="27"/>
       <c r="F54" s="27" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G54" s="28"/>
       <c r="H54" s="41"/>
@@ -15788,20 +15783,20 @@
     </row>
     <row r="55" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C55" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E55" s="27"/>
       <c r="F55" s="27" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G55" s="28"/>
       <c r="H55" s="41"/>
@@ -15827,20 +15822,20 @@
     </row>
     <row r="56" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" s="36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C56" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E56" s="27"/>
       <c r="F56" s="27" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G56" s="28"/>
       <c r="H56" s="41"/>
@@ -15866,20 +15861,20 @@
     </row>
     <row r="57" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" s="36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C57" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D57" s="27" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E57" s="27"/>
       <c r="F57" s="27" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G57" s="28"/>
       <c r="H57" s="41"/>
@@ -15903,26 +15898,24 @@
       <c r="Z57" s="20"/>
       <c r="AA57" s="20"/>
     </row>
-    <row r="58" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C58" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D58" s="27" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E58" s="27"/>
       <c r="F58" s="27" t="s">
-        <v>198</v>
-      </c>
-      <c r="G58" s="28" t="s">
-        <v>199</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="G58" s="28"/>
       <c r="H58" s="41"/>
       <c r="I58" s="20"/>
       <c r="J58" s="20"/>
@@ -15944,31 +15937,27 @@
       <c r="Z58" s="20"/>
       <c r="AA58" s="20"/>
     </row>
-    <row r="59" spans="1:27" ht="103" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="31" t="s">
-        <v>170</v>
-      </c>
-      <c r="B59" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="C59" s="31" t="s">
-        <v>184</v>
-      </c>
-      <c r="D59" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="E59" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="F59" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="G59" s="33" t="s">
-        <v>200</v>
-      </c>
-      <c r="H59" s="43" t="s">
-        <v>53</v>
-      </c>
+    <row r="59" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+      <c r="A59" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C59" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="D59" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="E59" s="27"/>
+      <c r="F59" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="G59" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="H59" s="41"/>
       <c r="I59" s="20"/>
       <c r="J59" s="20"/>
       <c r="K59" s="20"/>
@@ -15989,34 +15978,50 @@
       <c r="Z59" s="20"/>
       <c r="AA59" s="20"/>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A60" s="15"/>
-      <c r="B60" s="15"/>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="15"/>
-      <c r="F60" s="15"/>
-      <c r="G60" s="15"/>
-      <c r="H60" s="44"/>
-      <c r="I60" s="15"/>
-      <c r="J60" s="15"/>
-      <c r="K60" s="15"/>
-      <c r="L60" s="15"/>
-      <c r="M60" s="15"/>
-      <c r="N60" s="15"/>
-      <c r="O60" s="15"/>
-      <c r="P60" s="15"/>
-      <c r="Q60" s="15"/>
-      <c r="R60" s="15"/>
-      <c r="S60" s="15"/>
-      <c r="T60" s="15"/>
-      <c r="U60" s="15"/>
-      <c r="V60" s="15"/>
-      <c r="W60" s="15"/>
-      <c r="X60" s="15"/>
-      <c r="Y60" s="15"/>
-      <c r="Z60" s="15"/>
-      <c r="AA60" s="15"/>
+    <row r="60" spans="1:27" ht="103" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="B60" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C60" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="D60" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="E60" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F60" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="G60" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="H60" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="I60" s="20"/>
+      <c r="J60" s="20"/>
+      <c r="K60" s="20"/>
+      <c r="L60" s="20"/>
+      <c r="M60" s="20"/>
+      <c r="N60" s="20"/>
+      <c r="O60" s="20"/>
+      <c r="P60" s="20"/>
+      <c r="Q60" s="20"/>
+      <c r="R60" s="20"/>
+      <c r="S60" s="20"/>
+      <c r="T60" s="20"/>
+      <c r="U60" s="20"/>
+      <c r="V60" s="20"/>
+      <c r="W60" s="20"/>
+      <c r="X60" s="20"/>
+      <c r="Y60" s="20"/>
+      <c r="Z60" s="20"/>
+      <c r="AA60" s="20"/>
     </row>
     <row r="61" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A61" s="15"/>
@@ -43336,6 +43341,35 @@
       <c r="Z1002" s="15"/>
       <c r="AA1002" s="15"/>
     </row>
+    <row r="1003" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A1003" s="15"/>
+      <c r="B1003" s="15"/>
+      <c r="C1003" s="15"/>
+      <c r="D1003" s="15"/>
+      <c r="E1003" s="15"/>
+      <c r="F1003" s="15"/>
+      <c r="G1003" s="15"/>
+      <c r="H1003" s="44"/>
+      <c r="I1003" s="15"/>
+      <c r="J1003" s="15"/>
+      <c r="K1003" s="15"/>
+      <c r="L1003" s="15"/>
+      <c r="M1003" s="15"/>
+      <c r="N1003" s="15"/>
+      <c r="O1003" s="15"/>
+      <c r="P1003" s="15"/>
+      <c r="Q1003" s="15"/>
+      <c r="R1003" s="15"/>
+      <c r="S1003" s="15"/>
+      <c r="T1003" s="15"/>
+      <c r="U1003" s="15"/>
+      <c r="V1003" s="15"/>
+      <c r="W1003" s="15"/>
+      <c r="X1003" s="15"/>
+      <c r="Y1003" s="15"/>
+      <c r="Z1003" s="15"/>
+      <c r="AA1003" s="15"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="G1:H1">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="[ needs">
@@ -43352,9 +43386,6 @@
       <formula>NOT(ISERROR(SEARCH(("[none"),(G1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="H5" r:id="rId1" xr:uid="{D8864EDD-96F5-E04C-A9F9-BD9394ADB81C}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>

<commit_message>
Add seq_meth and denoising_appr fields
</commit_message>
<xml_diff>
--- a/molmod/static/downloads/SBDI-ASV-template.xlsx
+++ b/molmod/static/downloads/SBDI-ASV-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/molmod/static/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C2FA5C-E98C-9C46-AA60-0C56BFF18DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC50E4DD-D0DB-9149-86C0-7B8CADA1780F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7360" yWindow="9760" windowWidth="38000" windowHeight="14600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <sheet name="guide" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">guide!$A$1:$AA$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">guide!$A$1:$AA$61</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="305">
   <si>
     <t>event_id_alias</t>
   </si>
@@ -944,10 +944,19 @@
     <t>seq_meth</t>
   </si>
   <si>
-    <t>Illumina HiSeq 1500'</t>
+    <t>Sequencing method used</t>
   </si>
   <si>
-    <t>Sequencing method used</t>
+    <t>denoising_appr</t>
+  </si>
+  <si>
+    <t>Approach for denoising reads into Amplicon Sequence Variants (ASVs).</t>
+  </si>
+  <si>
+    <t>DADA2</t>
+  </si>
+  <si>
+    <t>'Illumina HiSeq 1500'</t>
   </si>
 </sst>
 </file>
@@ -958,11 +967,18 @@
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1267,146 +1283,155 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -5164,7 +5189,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:V9">
     <sortCondition ref="A3:A9"/>
   </sortState>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -6316,7 +6341,7 @@
     <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -13513,12 +13538,12 @@
   <sheetPr>
     <tabColor rgb="FFD6E3BC"/>
   </sheetPr>
-  <dimension ref="A1:AA1003"/>
+  <dimension ref="A1:AA1004"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14538,11 +14563,11 @@
         <v>63</v>
       </c>
       <c r="D25" s="55" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E25" s="27"/>
-      <c r="F25" s="56" t="s">
-        <v>300</v>
+      <c r="F25" s="59" t="s">
+        <v>304</v>
       </c>
       <c r="G25" s="28"/>
       <c r="H25" s="41"/>
@@ -14722,30 +14747,30 @@
       <c r="Z29" s="20"/>
       <c r="AA29" s="20"/>
     </row>
-    <row r="30" spans="1:27" ht="204" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="B30" s="26" t="s">
-        <v>26</v>
+      <c r="B30" s="56" t="s">
+        <v>301</v>
       </c>
       <c r="C30" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="E30" s="27" t="s">
-        <v>232</v>
-      </c>
-      <c r="F30" s="29" t="s">
-        <v>233</v>
-      </c>
-      <c r="G30" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="H30" s="41" t="s">
-        <v>234</v>
+      <c r="D30" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="G30" s="57" t="s">
+        <v>302</v>
+      </c>
+      <c r="H30" s="58" t="s">
+        <v>303</v>
       </c>
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
@@ -14772,25 +14797,25 @@
         <v>110</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C31" s="26" t="s">
         <v>63</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>237</v>
-      </c>
-      <c r="F31" s="27" t="s">
-        <v>238</v>
+        <v>232</v>
+      </c>
+      <c r="F31" s="29" t="s">
+        <v>233</v>
       </c>
       <c r="G31" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H31" s="41" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="I31" s="20"/>
       <c r="J31" s="20"/>
@@ -14812,30 +14837,30 @@
       <c r="Z31" s="20"/>
       <c r="AA31" s="20"/>
     </row>
-    <row r="32" spans="1:27" ht="154" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
+    <row r="32" spans="1:27" ht="204" x14ac:dyDescent="0.2">
+      <c r="A32" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="B32" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="31" t="s">
+      <c r="B32" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="32" t="s">
-        <v>127</v>
-      </c>
-      <c r="E32" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="F32" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="G32" s="33" t="s">
-        <v>249</v>
-      </c>
-      <c r="H32" s="43" t="s">
-        <v>240</v>
+      <c r="D32" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="E32" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="F32" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="G32" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="H32" s="41" t="s">
+        <v>239</v>
       </c>
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
@@ -14857,30 +14882,30 @@
       <c r="Z32" s="20"/>
       <c r="AA32" s="20"/>
     </row>
-    <row r="33" spans="1:27" ht="68" x14ac:dyDescent="0.2">
-      <c r="A33" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="B33" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="D33" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="E33" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="F33" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="G33" s="24" t="s">
-        <v>246</v>
-      </c>
-      <c r="H33" s="40" t="s">
-        <v>204</v>
+    <row r="33" spans="1:27" ht="154" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="G33" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="H33" s="43" t="s">
+        <v>240</v>
       </c>
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
@@ -14902,29 +14927,31 @@
       <c r="Z33" s="20"/>
       <c r="AA33" s="20"/>
     </row>
-    <row r="34" spans="1:27" ht="204" x14ac:dyDescent="0.2">
-      <c r="A34" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="B34" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="E34" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="F34" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="G34" s="49" t="s">
-        <v>296</v>
-      </c>
-      <c r="H34" s="41"/>
+    <row r="34" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+      <c r="A34" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="F34" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="G34" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H34" s="40" t="s">
+        <v>204</v>
+      </c>
       <c r="I34" s="20"/>
       <c r="J34" s="20"/>
       <c r="K34" s="20"/>
@@ -14945,26 +14972,28 @@
       <c r="Z34" s="20"/>
       <c r="AA34" s="20"/>
     </row>
-    <row r="35" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A35" s="25" t="s">
         <v>131</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F35" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="G35" s="28"/>
+        <v>134</v>
+      </c>
+      <c r="G35" s="49" t="s">
+        <v>296</v>
+      </c>
       <c r="H35" s="41"/>
       <c r="I35" s="20"/>
       <c r="J35" s="20"/>
@@ -14986,22 +15015,24 @@
       <c r="Z35" s="20"/>
       <c r="AA35" s="20"/>
     </row>
-    <row r="36" spans="1:27" ht="34" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" s="25" t="s">
         <v>131</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="E36" s="27"/>
+        <v>135</v>
+      </c>
+      <c r="E36" s="27" t="s">
+        <v>136</v>
+      </c>
       <c r="F36" s="27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G36" s="28"/>
       <c r="H36" s="41"/>
@@ -15025,24 +15056,22 @@
       <c r="Z36" s="20"/>
       <c r="AA36" s="20"/>
     </row>
-    <row r="37" spans="1:27" ht="119" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="25" t="s">
         <v>131</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="E37" s="27" t="s">
-        <v>141</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="E37" s="27"/>
       <c r="F37" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G37" s="28"/>
       <c r="H37" s="41"/>
@@ -15066,24 +15095,24 @@
       <c r="Z37" s="20"/>
       <c r="AA37" s="20"/>
     </row>
-    <row r="38" spans="1:27" ht="85" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27" ht="119" x14ac:dyDescent="0.2">
       <c r="A38" s="25" t="s">
         <v>131</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>143</v>
+        <v>74</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F38" s="27" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G38" s="28"/>
       <c r="H38" s="41"/>
@@ -15107,24 +15136,24 @@
       <c r="Z38" s="20"/>
       <c r="AA38" s="20"/>
     </row>
-    <row r="39" spans="1:27" ht="102" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A39" s="25" t="s">
         <v>131</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>74</v>
+        <v>143</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E39" s="27" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F39" s="27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G39" s="28"/>
       <c r="H39" s="41"/>
@@ -15148,24 +15177,24 @@
       <c r="Z39" s="20"/>
       <c r="AA39" s="20"/>
     </row>
-    <row r="40" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A40" s="25" t="s">
         <v>131</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C40" s="26" t="s">
         <v>74</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F40" s="27" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G40" s="28"/>
       <c r="H40" s="41"/>
@@ -15189,24 +15218,24 @@
       <c r="Z40" s="20"/>
       <c r="AA40" s="20"/>
     </row>
-    <row r="41" spans="1:27" ht="102" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="25" t="s">
         <v>131</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C41" s="26" t="s">
         <v>74</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E41" s="27" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F41" s="27" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G41" s="28"/>
       <c r="H41" s="41"/>
@@ -15230,24 +15259,24 @@
       <c r="Z41" s="20"/>
       <c r="AA41" s="20"/>
     </row>
-    <row r="42" spans="1:27" ht="85" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A42" s="25" t="s">
         <v>131</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C42" s="26" t="s">
         <v>74</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F42" s="27" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G42" s="28"/>
       <c r="H42" s="41"/>
@@ -15271,24 +15300,24 @@
       <c r="Z42" s="20"/>
       <c r="AA42" s="20"/>
     </row>
-    <row r="43" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A43" s="25" t="s">
         <v>131</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E43" s="27" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F43" s="27" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G43" s="28"/>
       <c r="H43" s="41"/>
@@ -15312,27 +15341,27 @@
       <c r="Z43" s="20"/>
       <c r="AA43" s="20"/>
     </row>
-    <row r="44" spans="1:27" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="30" t="s">
+    <row r="44" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+      <c r="A44" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="B44" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C44" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="D44" s="32" t="s">
-        <v>162</v>
-      </c>
-      <c r="E44" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="F44" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="G44" s="33"/>
-      <c r="H44" s="43"/>
+      <c r="B44" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="E44" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="F44" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="G44" s="28"/>
+      <c r="H44" s="41"/>
       <c r="I44" s="20"/>
       <c r="J44" s="20"/>
       <c r="K44" s="20"/>
@@ -15353,31 +15382,27 @@
       <c r="Z44" s="20"/>
       <c r="AA44" s="20"/>
     </row>
-    <row r="45" spans="1:27" ht="68" x14ac:dyDescent="0.2">
-      <c r="A45" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="B45" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="D45" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="E45" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="F45" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="G45" s="24" t="s">
-        <v>246</v>
-      </c>
-      <c r="H45" s="40" t="s">
-        <v>204</v>
-      </c>
+    <row r="45" spans="1:27" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="B45" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="D45" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="E45" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="F45" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="G45" s="33"/>
+      <c r="H45" s="43"/>
       <c r="I45" s="20"/>
       <c r="J45" s="20"/>
       <c r="K45" s="20"/>
@@ -15398,30 +15423,30 @@
       <c r="Z45" s="20"/>
       <c r="AA45" s="20"/>
     </row>
-    <row r="46" spans="1:27" ht="205" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
-        <v>227</v>
-      </c>
-      <c r="B46" s="31" t="s">
-        <v>226</v>
-      </c>
-      <c r="C46" s="31" t="s">
+    <row r="46" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+      <c r="A46" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="D46" s="38" t="s">
+      <c r="D46" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="E46" s="38" t="s">
+      <c r="E46" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="F46" s="38" t="s">
+      <c r="F46" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="G46" s="50" t="s">
-        <v>297</v>
-      </c>
-      <c r="H46" s="43" t="s">
-        <v>244</v>
+      <c r="G46" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H46" s="40" t="s">
+        <v>204</v>
       </c>
       <c r="I46" s="20"/>
       <c r="J46" s="20"/>
@@ -15443,30 +15468,30 @@
       <c r="Z46" s="20"/>
       <c r="AA46" s="20"/>
     </row>
-    <row r="47" spans="1:27" ht="51" x14ac:dyDescent="0.2">
-      <c r="A47" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="B47" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="C47" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="D47" s="35" t="s">
+    <row r="47" spans="1:27" ht="205" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="B47" s="31" t="s">
+        <v>226</v>
+      </c>
+      <c r="C47" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="E47" s="35" t="s">
+      <c r="D47" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="F47" s="35" t="s">
+      <c r="E47" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="G47" s="24" t="s">
-        <v>167</v>
-      </c>
-      <c r="H47" s="40" t="s">
-        <v>168</v>
+      <c r="F47" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="G47" s="50" t="s">
+        <v>297</v>
+      </c>
+      <c r="H47" s="43" t="s">
+        <v>244</v>
       </c>
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
@@ -15488,30 +15513,30 @@
       <c r="Z47" s="20"/>
       <c r="AA47" s="20"/>
     </row>
-    <row r="48" spans="1:27" ht="68" x14ac:dyDescent="0.2">
-      <c r="A48" s="36" t="s">
-        <v>169</v>
+    <row r="48" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+      <c r="A48" s="21" t="s">
+        <v>165</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="C48" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="C48" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="D48" s="23" t="s">
+      <c r="D48" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="E48" s="23" t="s">
+      <c r="E48" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="F48" s="23" t="s">
+      <c r="F48" s="35" t="s">
         <v>64</v>
       </c>
       <c r="G48" s="24" t="s">
-        <v>246</v>
+        <v>167</v>
       </c>
       <c r="H48" s="40" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="I48" s="20"/>
       <c r="J48" s="20"/>
@@ -15533,30 +15558,30 @@
       <c r="Z48" s="20"/>
       <c r="AA48" s="20"/>
     </row>
-    <row r="49" spans="1:27" ht="119" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A49" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="B49" s="26" t="s">
-        <v>171</v>
-      </c>
-      <c r="C49" s="26" t="s">
+      <c r="B49" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="C49" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D49" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="E49" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="F49" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="G49" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H49" s="41">
-        <v>486</v>
+      <c r="D49" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E49" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F49" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G49" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H49" s="40" t="s">
+        <v>204</v>
       </c>
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
@@ -15578,26 +15603,30 @@
       <c r="Z49" s="20"/>
       <c r="AA49" s="20"/>
     </row>
-    <row r="50" spans="1:27" ht="204" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:27" ht="119" x14ac:dyDescent="0.2">
       <c r="A50" s="36" t="s">
         <v>169</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>42</v>
+        <v>171</v>
       </c>
       <c r="C50" s="26" t="s">
         <v>63</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
+        <v>172</v>
+      </c>
+      <c r="E50" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="F50" s="27" t="s">
+        <v>174</v>
+      </c>
       <c r="G50" s="28" t="s">
-        <v>177</v>
-      </c>
-      <c r="H50" s="41" t="s">
-        <v>178</v>
+        <v>175</v>
+      </c>
+      <c r="H50" s="41">
+        <v>486</v>
       </c>
       <c r="I50" s="20"/>
       <c r="J50" s="20"/>
@@ -15619,28 +15648,26 @@
       <c r="Z50" s="20"/>
       <c r="AA50" s="20"/>
     </row>
-    <row r="51" spans="1:27" ht="102" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A51" s="36" t="s">
         <v>169</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D51" s="27" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E51" s="27"/>
-      <c r="F51" s="27" t="s">
-        <v>180</v>
-      </c>
+      <c r="F51" s="27"/>
       <c r="G51" s="28" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="H51" s="41" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
       <c r="I51" s="20"/>
       <c r="J51" s="20"/>
@@ -15662,27 +15689,29 @@
       <c r="Z51" s="20"/>
       <c r="AA51" s="20"/>
     </row>
-    <row r="52" spans="1:27" ht="85" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A52" s="36" t="s">
         <v>169</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C52" s="26" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="D52" s="27" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E52" s="27"/>
       <c r="F52" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="G52" s="48" t="s">
-        <v>245</v>
-      </c>
-      <c r="H52" s="41"/>
+        <v>180</v>
+      </c>
+      <c r="G52" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="H52" s="41" t="s">
+        <v>201</v>
+      </c>
       <c r="I52" s="20"/>
       <c r="J52" s="20"/>
       <c r="K52" s="20"/>
@@ -15703,24 +15732,26 @@
       <c r="Z52" s="20"/>
       <c r="AA52" s="20"/>
     </row>
-    <row r="53" spans="1:27" ht="34" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A53" s="36" t="s">
         <v>169</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>183</v>
+        <v>63</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E53" s="27"/>
       <c r="F53" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="G53" s="28"/>
+        <v>182</v>
+      </c>
+      <c r="G53" s="48" t="s">
+        <v>245</v>
+      </c>
       <c r="H53" s="41"/>
       <c r="I53" s="20"/>
       <c r="J53" s="20"/>
@@ -15747,17 +15778,17 @@
         <v>169</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C54" s="26" t="s">
         <v>183</v>
       </c>
       <c r="D54" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E54" s="27"/>
       <c r="F54" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G54" s="28"/>
       <c r="H54" s="41"/>
@@ -15786,17 +15817,17 @@
         <v>169</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C55" s="26" t="s">
         <v>183</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E55" s="27"/>
       <c r="F55" s="27" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G55" s="28"/>
       <c r="H55" s="41"/>
@@ -15825,17 +15856,17 @@
         <v>169</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C56" s="26" t="s">
         <v>183</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E56" s="27"/>
       <c r="F56" s="27" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G56" s="28"/>
       <c r="H56" s="41"/>
@@ -15864,17 +15895,17 @@
         <v>169</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C57" s="26" t="s">
         <v>183</v>
       </c>
       <c r="D57" s="27" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E57" s="27"/>
       <c r="F57" s="27" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G57" s="28"/>
       <c r="H57" s="41"/>
@@ -15903,17 +15934,17 @@
         <v>169</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C58" s="26" t="s">
         <v>183</v>
       </c>
       <c r="D58" s="27" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E58" s="27"/>
       <c r="F58" s="27" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G58" s="28"/>
       <c r="H58" s="41"/>
@@ -15937,26 +15968,24 @@
       <c r="Z58" s="20"/>
       <c r="AA58" s="20"/>
     </row>
-    <row r="59" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" s="36" t="s">
         <v>169</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C59" s="26" t="s">
         <v>183</v>
       </c>
       <c r="D59" s="27" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E59" s="27"/>
       <c r="F59" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="G59" s="28" t="s">
-        <v>198</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="G59" s="28"/>
       <c r="H59" s="41"/>
       <c r="I59" s="20"/>
       <c r="J59" s="20"/>
@@ -15978,31 +16007,27 @@
       <c r="Z59" s="20"/>
       <c r="AA59" s="20"/>
     </row>
-    <row r="60" spans="1:27" ht="103" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="31" t="s">
+    <row r="60" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+      <c r="A60" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="B60" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="C60" s="31" t="s">
+      <c r="B60" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C60" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="D60" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="E60" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="F60" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="G60" s="33" t="s">
-        <v>199</v>
-      </c>
-      <c r="H60" s="43" t="s">
-        <v>53</v>
-      </c>
+      <c r="D60" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="E60" s="27"/>
+      <c r="F60" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="G60" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="H60" s="41"/>
       <c r="I60" s="20"/>
       <c r="J60" s="20"/>
       <c r="K60" s="20"/>
@@ -16023,34 +16048,50 @@
       <c r="Z60" s="20"/>
       <c r="AA60" s="20"/>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A61" s="15"/>
-      <c r="B61" s="15"/>
-      <c r="C61" s="15"/>
-      <c r="D61" s="15"/>
-      <c r="E61" s="15"/>
-      <c r="F61" s="15"/>
-      <c r="G61" s="15"/>
-      <c r="H61" s="44"/>
-      <c r="I61" s="15"/>
-      <c r="J61" s="15"/>
-      <c r="K61" s="15"/>
-      <c r="L61" s="15"/>
-      <c r="M61" s="15"/>
-      <c r="N61" s="15"/>
-      <c r="O61" s="15"/>
-      <c r="P61" s="15"/>
-      <c r="Q61" s="15"/>
-      <c r="R61" s="15"/>
-      <c r="S61" s="15"/>
-      <c r="T61" s="15"/>
-      <c r="U61" s="15"/>
-      <c r="V61" s="15"/>
-      <c r="W61" s="15"/>
-      <c r="X61" s="15"/>
-      <c r="Y61" s="15"/>
-      <c r="Z61" s="15"/>
-      <c r="AA61" s="15"/>
+    <row r="61" spans="1:27" ht="103" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="B61" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C61" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="D61" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="E61" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F61" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="G61" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="H61" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="I61" s="20"/>
+      <c r="J61" s="20"/>
+      <c r="K61" s="20"/>
+      <c r="L61" s="20"/>
+      <c r="M61" s="20"/>
+      <c r="N61" s="20"/>
+      <c r="O61" s="20"/>
+      <c r="P61" s="20"/>
+      <c r="Q61" s="20"/>
+      <c r="R61" s="20"/>
+      <c r="S61" s="20"/>
+      <c r="T61" s="20"/>
+      <c r="U61" s="20"/>
+      <c r="V61" s="20"/>
+      <c r="W61" s="20"/>
+      <c r="X61" s="20"/>
+      <c r="Y61" s="20"/>
+      <c r="Z61" s="20"/>
+      <c r="AA61" s="20"/>
     </row>
     <row r="62" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A62" s="15"/>
@@ -43370,6 +43411,35 @@
       <c r="Z1003" s="15"/>
       <c r="AA1003" s="15"/>
     </row>
+    <row r="1004" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A1004" s="15"/>
+      <c r="B1004" s="15"/>
+      <c r="C1004" s="15"/>
+      <c r="D1004" s="15"/>
+      <c r="E1004" s="15"/>
+      <c r="F1004" s="15"/>
+      <c r="G1004" s="15"/>
+      <c r="H1004" s="44"/>
+      <c r="I1004" s="15"/>
+      <c r="J1004" s="15"/>
+      <c r="K1004" s="15"/>
+      <c r="L1004" s="15"/>
+      <c r="M1004" s="15"/>
+      <c r="N1004" s="15"/>
+      <c r="O1004" s="15"/>
+      <c r="P1004" s="15"/>
+      <c r="Q1004" s="15"/>
+      <c r="R1004" s="15"/>
+      <c r="S1004" s="15"/>
+      <c r="T1004" s="15"/>
+      <c r="U1004" s="15"/>
+      <c r="V1004" s="15"/>
+      <c r="W1004" s="15"/>
+      <c r="X1004" s="15"/>
+      <c r="Y1004" s="15"/>
+      <c r="Z1004" s="15"/>
+      <c r="AA1004" s="15"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="G1:H1">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="[ needs">

</xml_diff>

<commit_message>
Open import template in guide tab
</commit_message>
<xml_diff>
--- a/molmod/static/downloads/SBDI-ASV-template.xlsx
+++ b/molmod/static/downloads/SBDI-ASV-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/molmod/static/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C891F6B-25FB-C44A-AAC3-C69A3691B114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FA3F2F-DBE6-9B46-8AD4-A6936F4EDDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7360" yWindow="9760" windowWidth="38000" windowHeight="14600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7360" yWindow="9760" windowWidth="38000" windowHeight="14600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event" sheetId="1" r:id="rId1"/>
@@ -704,9 +704,6 @@
     <t>temperature (°C)</t>
   </si>
   <si>
-    <t>emof-simple (A simplified version of emof, used by ASV portal only)</t>
-  </si>
-  <si>
     <t>[measurementType] ([measurementUnit])</t>
   </si>
   <si>
@@ -961,6 +958,9 @@
   <si>
     <t>Illumina MiSeq</t>
   </si>
+  <si>
+    <t>emof-simple (a simplified version of emof, used by ASV portal only)</t>
+  </si>
 </sst>
 </file>
 
@@ -970,11 +970,18 @@
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1293,160 +1300,163 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1779,7 +1789,7 @@
         <v>199</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>202</v>
@@ -1814,7 +1824,7 @@
         <v>198</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>201</v>
@@ -1860,7 +1870,7 @@
         <v>197</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>200</v>
@@ -5200,7 +5210,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:V9">
     <sortCondition ref="A3:A9"/>
   </sortState>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -5210,7 +5220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N977"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -5247,7 +5257,7 @@
         <v>21</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>22</v>
@@ -5262,7 +5272,7 @@
         <v>25</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>26</v>
@@ -5288,7 +5298,7 @@
         <v>29</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>207</v>
@@ -5303,7 +5313,7 @@
         <v>123</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>211</v>
@@ -5329,7 +5339,7 @@
         <v>29</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>207</v>
@@ -5344,7 +5354,7 @@
         <v>123</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>211</v>
@@ -5370,7 +5380,7 @@
         <v>29</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>207</v>
@@ -5385,7 +5395,7 @@
         <v>123</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>211</v>
@@ -6371,7 +6381,7 @@
     <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -12750,28 +12760,28 @@
     </row>
     <row r="2" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>251</v>
-      </c>
       <c r="I2" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M2" s="5">
         <v>2235</v>
@@ -12785,28 +12795,28 @@
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="D3" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>257</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>258</v>
       </c>
       <c r="M3" s="5">
         <v>1033</v>
@@ -12820,22 +12830,22 @@
     </row>
     <row r="4" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>260</v>
-      </c>
       <c r="D4" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>249</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>250</v>
       </c>
       <c r="M4" s="5">
         <v>795</v>
@@ -12849,28 +12859,28 @@
     </row>
     <row r="5" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="D5" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="M5" s="5">
         <v>134</v>
@@ -12884,28 +12894,28 @@
     </row>
     <row r="6" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="D6" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>269</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>270</v>
       </c>
       <c r="M6" s="5">
         <v>572</v>
@@ -12919,28 +12929,28 @@
     </row>
     <row r="7" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>272</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="M7" s="5">
         <v>47</v>
@@ -12954,31 +12964,31 @@
     </row>
     <row r="8" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="D8" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="H8" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>278</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>279</v>
       </c>
       <c r="M8" s="5">
         <v>40</v>
@@ -12992,28 +13002,28 @@
     </row>
     <row r="9" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="D9" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>281</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>282</v>
       </c>
       <c r="M9" s="5">
         <v>99</v>
@@ -13027,25 +13037,25 @@
     </row>
     <row r="10" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>284</v>
-      </c>
       <c r="D10" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="H10" s="5" t="s">
         <v>256</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>257</v>
       </c>
       <c r="M10" s="5">
         <v>312</v>
@@ -13059,28 +13069,28 @@
     </row>
     <row r="11" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="D11" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>286</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>287</v>
       </c>
       <c r="M11" s="5">
         <v>147</v>
@@ -13570,8 +13580,8 @@
   </sheetPr>
   <dimension ref="A1:AA1004"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
     </sheetView>
@@ -13637,7 +13647,7 @@
     </row>
     <row r="2" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="54" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>0</v>
@@ -13655,7 +13665,7 @@
         <v>63</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H2" s="35" t="s">
         <v>199</v>
@@ -13698,10 +13708,10 @@
         <v>66</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H3" s="36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I3" s="19"/>
       <c r="J3" s="19"/>
@@ -13737,13 +13747,13 @@
         <v>67</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>68</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H4" s="41" t="s">
         <v>202</v>
@@ -13786,7 +13796,7 @@
         <v>70</v>
       </c>
       <c r="G5" s="47" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H5" s="42"/>
       <c r="I5" s="19"/>
@@ -13827,7 +13837,7 @@
       </c>
       <c r="F6" s="24"/>
       <c r="G6" s="44" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H6" s="36">
         <v>80698</v>
@@ -13870,7 +13880,7 @@
         <v>75</v>
       </c>
       <c r="G7" s="44" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H7" s="37" t="s">
         <v>76</v>
@@ -14077,10 +14087,10 @@
         <v>91</v>
       </c>
       <c r="G12" s="44" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H12" s="36" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
@@ -14381,7 +14391,7 @@
     </row>
     <row r="20" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="54" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B20" s="23" t="s">
         <v>0</v>
@@ -14399,7 +14409,7 @@
         <v>63</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H20" s="35" t="s">
         <v>199</v>
@@ -14426,7 +14436,7 @@
     </row>
     <row r="21" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A21" s="54" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B21" s="23" t="s">
         <v>18</v>
@@ -14467,7 +14477,7 @@
     </row>
     <row r="22" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="54" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B22" s="23" t="s">
         <v>19</v>
@@ -14506,7 +14516,7 @@
     </row>
     <row r="23" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="54" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B23" s="23" t="s">
         <v>20</v>
@@ -14545,7 +14555,7 @@
     </row>
     <row r="24" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="54" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B24" s="23" t="s">
         <v>21</v>
@@ -14584,20 +14594,20 @@
     </row>
     <row r="25" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="54" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B25" s="48" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C25" s="48" t="s">
         <v>62</v>
       </c>
       <c r="D25" s="49" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E25" s="24"/>
       <c r="F25" s="53" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G25" s="25"/>
       <c r="H25" s="36"/>
@@ -14623,7 +14633,7 @@
     </row>
     <row r="26" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="54" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B26" s="23" t="s">
         <v>22</v>
@@ -14662,7 +14672,7 @@
     </row>
     <row r="27" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="54" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B27" s="23" t="s">
         <v>23</v>
@@ -14701,7 +14711,7 @@
     </row>
     <row r="28" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="54" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B28" s="23" t="s">
         <v>24</v>
@@ -14740,7 +14750,7 @@
     </row>
     <row r="29" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="54" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B29" s="23" t="s">
         <v>25</v>
@@ -14779,10 +14789,10 @@
     </row>
     <row r="30" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="54" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B30" s="50" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C30" s="23" t="s">
         <v>62</v>
@@ -14797,10 +14807,10 @@
         <v>63</v>
       </c>
       <c r="G30" s="51" t="s">
+        <v>296</v>
+      </c>
+      <c r="H30" s="52" t="s">
         <v>297</v>
-      </c>
-      <c r="H30" s="52" t="s">
-        <v>298</v>
       </c>
       <c r="I30" s="19"/>
       <c r="J30" s="19"/>
@@ -14824,7 +14834,7 @@
     </row>
     <row r="31" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A31" s="54" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B31" s="23" t="s">
         <v>26</v>
@@ -14833,19 +14843,19 @@
         <v>62</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E31" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="F31" s="26" t="s">
         <v>227</v>
       </c>
-      <c r="F31" s="26" t="s">
+      <c r="G31" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="H31" s="36" t="s">
         <v>228</v>
-      </c>
-      <c r="G31" s="25" t="s">
-        <v>242</v>
-      </c>
-      <c r="H31" s="36" t="s">
-        <v>229</v>
       </c>
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
@@ -14869,7 +14879,7 @@
     </row>
     <row r="32" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A32" s="54" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B32" s="23" t="s">
         <v>27</v>
@@ -14878,19 +14888,19 @@
         <v>62</v>
       </c>
       <c r="D32" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="E32" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="E32" s="24" t="s">
+      <c r="F32" s="24" t="s">
         <v>232</v>
       </c>
-      <c r="F32" s="24" t="s">
+      <c r="G32" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="H32" s="36" t="s">
         <v>233</v>
-      </c>
-      <c r="G32" s="25" t="s">
-        <v>243</v>
-      </c>
-      <c r="H32" s="36" t="s">
-        <v>234</v>
       </c>
       <c r="I32" s="19"/>
       <c r="J32" s="19"/>
@@ -14914,7 +14924,7 @@
     </row>
     <row r="33" spans="1:27" ht="154" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="57" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B33" s="27" t="s">
         <v>28</v>
@@ -14932,10 +14942,10 @@
         <v>126</v>
       </c>
       <c r="G33" s="29" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H33" s="38" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I33" s="19"/>
       <c r="J33" s="19"/>
@@ -14959,7 +14969,7 @@
     </row>
     <row r="34" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A34" s="54" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B34" s="20" t="s">
         <v>0</v>
@@ -14977,7 +14987,7 @@
         <v>63</v>
       </c>
       <c r="G34" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H34" s="35" t="s">
         <v>199</v>
@@ -15022,7 +15032,7 @@
         <v>130</v>
       </c>
       <c r="G35" s="44" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H35" s="36"/>
       <c r="I35" s="19"/>
@@ -15454,8 +15464,8 @@
       <c r="AA45" s="19"/>
     </row>
     <row r="46" spans="1:27" ht="68" x14ac:dyDescent="0.2">
-      <c r="A46" s="54" t="s">
-        <v>220</v>
+      <c r="A46" s="61" t="s">
+        <v>305</v>
       </c>
       <c r="B46" s="20" t="s">
         <v>0</v>
@@ -15473,7 +15483,7 @@
         <v>63</v>
       </c>
       <c r="G46" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H46" s="35" t="s">
         <v>199</v>
@@ -15500,10 +15510,10 @@
     </row>
     <row r="47" spans="1:27" ht="205" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="57" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C47" s="27" t="s">
         <v>63</v>
@@ -15518,10 +15528,10 @@
         <v>63</v>
       </c>
       <c r="G47" s="45" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H47" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I47" s="19"/>
       <c r="J47" s="19"/>
@@ -15545,7 +15555,7 @@
     </row>
     <row r="48" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A48" s="54" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B48" s="20" t="s">
         <v>161</v>
@@ -15608,7 +15618,7 @@
         <v>63</v>
       </c>
       <c r="G49" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H49" s="35" t="s">
         <v>199</v>
@@ -15780,7 +15790,7 @@
         <v>177</v>
       </c>
       <c r="G53" s="43" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H53" s="36"/>
       <c r="I53" s="19"/>

</xml_diff>

<commit_message>
Remove old indata field sample_size_value/sampleSizeValue
</commit_message>
<xml_diff>
--- a/molmod/static/downloads/SBDI-ASV-template.xlsx
+++ b/molmod/static/downloads/SBDI-ASV-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/molmod/static/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FA3F2F-DBE6-9B46-8AD4-A6936F4EDDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC011D0-9A19-0C49-AB1E-FFBA13D112B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7360" yWindow="9760" windowWidth="38000" windowHeight="14600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <sheet name="guide" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">guide!$A$1:$AA$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">guide!$A$1:$AA$60</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="302">
   <si>
     <t>event_id_alias</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>samplingProtocol</t>
-  </si>
-  <si>
-    <t>sampleSizeValue</t>
   </si>
   <si>
     <t>locationID</t>
@@ -247,12 +244,6 @@
   </si>
   <si>
     <t>'UV light trap', 'mist net', 'bottom trawl', 'ad hoc observation', 'point count', 'Penguins from space: faecal stains reveal the location of emperor penguin colonies, https://doi.org/10.1111/j.1466-8238.2009.00467.x', 'Takats et al. 2001. Guidelines for Nocturnal Owl Monitoring in North America. Beaverhill Bird Observatory and Bird Studies Canada, Edmonton, Alberta. 32 pp.', 'http://www.bsc-eoc.org/download/Owl.pdf'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A numeric value for a measurement of the size (time duration, length, area, or volume) of a sample in a sampling event. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">	A sampleSizeValue must have a corresponding sampleSizeUnit.</t>
   </si>
   <si>
     <t>Optional</t>
@@ -909,9 +900,6 @@
   </si>
   <si>
     <t>Use e.g. for Station ID:Name in Stationsregistret.</t>
-  </si>
-  <si>
-    <t>Total number of (target gene) reads counted per sample.</t>
   </si>
   <si>
     <t>Use this full version of emof to report contextual data if you, in addition to measurementType, measurementUnit and measurementValue, also want to refer to some controlled vocabulary or system for e.g. variables, units and values etc. Otherwise, you can also see emof-simpler below. Preferably use variable names and units listed in a relevant GCS Checklist, see https://www.ebi.ac.uk/ena/browser/checklists.</t>
@@ -1701,29 +1689,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD991"/>
+  <dimension ref="A1:AC991"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="14.140625" style="6" customWidth="1"/>
     <col min="3" max="3" width="17" style="6" customWidth="1"/>
-    <col min="4" max="8" width="14.140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="23.28515625" style="6" customWidth="1"/>
-    <col min="11" max="14" width="14.140625" style="6" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" style="6" customWidth="1"/>
-    <col min="16" max="16" width="21.42578125" style="6" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" style="6" customWidth="1"/>
-    <col min="18" max="18" width="19" style="6" customWidth="1"/>
-    <col min="19" max="26" width="11.28515625" style="6" customWidth="1"/>
-    <col min="27" max="16384" width="11.28515625" style="6"/>
+    <col min="4" max="7" width="14.140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" style="6" customWidth="1"/>
+    <col min="10" max="13" width="14.140625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" style="6" customWidth="1"/>
+    <col min="15" max="15" width="21.42578125" style="6" customWidth="1"/>
+    <col min="16" max="16" width="18.5703125" style="6" customWidth="1"/>
+    <col min="17" max="17" width="19" style="6" customWidth="1"/>
+    <col min="18" max="25" width="11.28515625" style="6" customWidth="1"/>
+    <col min="26" max="16384" width="11.28515625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1775,84 +1763,76 @@
       <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="R1" s="5"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
       <c r="U1" s="5"/>
       <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-    </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>202</v>
-      </c>
       <c r="D2" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E2" s="6">
-        <v>5414</v>
+        <v>200</v>
+      </c>
+      <c r="F2" s="5">
+        <v>55.185000000000002</v>
       </c>
       <c r="G2" s="5">
-        <v>55.185000000000002</v>
-      </c>
-      <c r="H2" s="5">
         <v>13.791</v>
       </c>
-      <c r="I2" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>213</v>
+      <c r="H2" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="P2" s="5">
+        <v>3</v>
       </c>
       <c r="Q2" s="5">
         <v>3</v>
       </c>
-      <c r="R2" s="5">
+    </row>
+    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="F3" s="5">
+        <v>55.433999999999997</v>
+      </c>
+      <c r="G3" s="5">
+        <v>14.813000000000001</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="P3" s="5">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E3" s="6">
-        <v>37676</v>
-      </c>
-      <c r="G3" s="5">
-        <v>55.433999999999997</v>
-      </c>
-      <c r="H3" s="5">
-        <v>14.813000000000001</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>212</v>
       </c>
       <c r="Q3" s="5">
         <v>3</v>
       </c>
-      <c r="R3" s="5">
-        <v>3</v>
-      </c>
+      <c r="S3" s="5"/>
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
@@ -1863,42 +1843,39 @@
       <c r="AA3" s="5"/>
       <c r="AB3" s="5"/>
       <c r="AC3" s="5"/>
-      <c r="AD3" s="5"/>
-    </row>
-    <row r="4" spans="1:30" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E4" s="6">
-        <v>41973</v>
+      <c r="F4" s="5">
+        <v>56.031999999999996</v>
       </c>
       <c r="G4" s="5">
-        <v>56.031999999999996</v>
-      </c>
-      <c r="H4" s="5">
         <v>16.649999999999999</v>
       </c>
-      <c r="I4" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>212</v>
+      <c r="H4" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="P4" s="5">
+        <v>3</v>
       </c>
       <c r="Q4" s="5">
         <v>3</v>
       </c>
-      <c r="R4" s="5">
-        <v>3</v>
-      </c>
+      <c r="S4" s="5"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
@@ -1909,9 +1886,9 @@
       <c r="AA4" s="5"/>
       <c r="AB4" s="5"/>
       <c r="AC4" s="5"/>
-      <c r="AD4" s="5"/>
-    </row>
-    <row r="5" spans="1:30" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="S5" s="5"/>
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
@@ -1922,9 +1899,9 @@
       <c r="AA5" s="5"/>
       <c r="AB5" s="5"/>
       <c r="AC5" s="5"/>
-      <c r="AD5" s="5"/>
-    </row>
-    <row r="6" spans="1:30" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="S6" s="5"/>
       <c r="T6" s="5"/>
       <c r="U6" s="5"/>
       <c r="V6" s="5"/>
@@ -1935,9 +1912,9 @@
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
       <c r="AC6" s="5"/>
-      <c r="AD6" s="5"/>
-    </row>
-    <row r="7" spans="1:30" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="S7" s="5"/>
       <c r="T7" s="5"/>
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
@@ -1948,9 +1925,9 @@
       <c r="AA7" s="5"/>
       <c r="AB7" s="5"/>
       <c r="AC7" s="5"/>
-      <c r="AD7" s="5"/>
-    </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S8" s="5"/>
       <c r="T8" s="5"/>
       <c r="U8" s="5"/>
       <c r="V8" s="5"/>
@@ -1961,9 +1938,9 @@
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
       <c r="AC8" s="5"/>
-      <c r="AD8" s="5"/>
-    </row>
-    <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S9" s="5"/>
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
       <c r="V9" s="5"/>
@@ -1974,407 +1951,385 @@
       <c r="AA9" s="5"/>
       <c r="AB9" s="5"/>
       <c r="AC9" s="5"/>
-      <c r="AD9" s="5"/>
-    </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="7"/>
     </row>
-    <row r="13" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="7"/>
     </row>
-    <row r="14" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
-      <c r="H14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="9"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
+      <c r="J14" s="8"/>
       <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-    </row>
-    <row r="15" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="10"/>
       <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="H15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="J15" s="5"/>
       <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="13"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-    </row>
-    <row r="16" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="10"/>
       <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="H16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="J16" s="5"/>
       <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="14"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-    </row>
-    <row r="17" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="10"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="H17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="J17" s="5"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="14"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-    </row>
-    <row r="18" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="10"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="H18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="14"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-    </row>
-    <row r="19" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="10"/>
       <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="H19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="J19" s="5"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="14"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-    </row>
-    <row r="20" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="10"/>
       <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="H20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="J20" s="5"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="14"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-    </row>
-    <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="10"/>
       <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="H21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="14"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-    </row>
-    <row r="22" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="10"/>
       <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="H22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="14"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-    </row>
-    <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="10"/>
       <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="H23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="J23" s="5"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="14"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="5"/>
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-    </row>
-    <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="10"/>
       <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="H24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="14"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="5"/>
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-    </row>
-    <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="10"/>
       <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="H25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="J25" s="5"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="14"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-    </row>
-    <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="10"/>
       <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="H26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="J26" s="5"/>
       <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="14"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="5"/>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
-    </row>
-    <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="10"/>
       <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="H27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="J27" s="5"/>
       <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="14"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="5"/>
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
-    </row>
-    <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="10"/>
       <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="H28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="J28" s="5"/>
       <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="14"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="5"/>
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
-      <c r="Q28" s="5"/>
-    </row>
-    <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="10"/>
       <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="H29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="14"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="5"/>
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-    </row>
-    <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="10"/>
       <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="H30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="J30" s="5"/>
       <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="14"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
-    </row>
-    <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="10"/>
       <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="H31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="J31" s="5"/>
       <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="14"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
-    </row>
-    <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="10"/>
       <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="H32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="J32" s="5"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="14"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="5"/>
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-    </row>
-    <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="10"/>
       <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="H33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="12"/>
-      <c r="N33" s="14"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
-    </row>
-    <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="10"/>
       <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="H34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="J34" s="5"/>
       <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="14"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="5"/>
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
-      <c r="Q34" s="5"/>
-    </row>
-    <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="10"/>
       <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="H35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="J35" s="5"/>
       <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="14"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="5"/>
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
-      <c r="Q35" s="5"/>
-    </row>
-    <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="7"/>
     </row>
-    <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C37" s="7"/>
     </row>
-    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C38" s="7"/>
     </row>
-    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C39" s="7"/>
     </row>
-    <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="7"/>
     </row>
-    <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="7"/>
     </row>
-    <row r="42" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C42" s="7"/>
     </row>
-    <row r="43" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C43" s="7"/>
     </row>
-    <row r="44" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C44" s="7"/>
     </row>
-    <row r="45" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C45" s="7"/>
     </row>
-    <row r="46" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C46" s="7"/>
     </row>
-    <row r="47" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C47" s="7"/>
     </row>
-    <row r="48" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C48" s="7"/>
     </row>
     <row r="49" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5207,7 +5162,7 @@
       <c r="C991" s="7"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:V9">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:U9">
     <sortCondition ref="A3:A9"/>
   </sortState>
   <phoneticPr fontId="9" type="noConversion"/>
@@ -5245,166 +5200,166 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="I2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="I3" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="I4" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6407,45 +6362,45 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5">
@@ -6453,7 +6408,7 @@
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -6464,38 +6419,38 @@
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D3" s="5">
         <v>7.23</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D4" s="5">
         <v>6.97</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5">
@@ -6503,21 +6458,21 @@
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="6" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D6" s="5">
         <v>17.399999999999999</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -6528,16 +6483,16 @@
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D7" s="5">
         <v>16.899999999999999</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -9699,15 +9654,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B2" s="5">
         <v>7.25</v>
@@ -9718,7 +9673,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B3" s="5">
         <v>7.23</v>
@@ -9729,7 +9684,7 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B4" s="5">
         <v>6.97</v>
@@ -12713,75 +12668,75 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="M1" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>250</v>
-      </c>
       <c r="I2" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="M2" s="5">
         <v>2235</v>
@@ -12795,28 +12750,28 @@
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>257</v>
       </c>
       <c r="M3" s="5">
         <v>1033</v>
@@ -12830,22 +12785,22 @@
     </row>
     <row r="4" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>246</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>249</v>
       </c>
       <c r="M4" s="5">
         <v>795</v>
@@ -12859,28 +12814,28 @@
     </row>
     <row r="5" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>263</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>266</v>
       </c>
       <c r="M5" s="5">
         <v>134</v>
@@ -12894,28 +12849,28 @@
     </row>
     <row r="6" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>256</v>
-      </c>
       <c r="I6" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="M6" s="5">
         <v>572</v>
@@ -12929,28 +12884,28 @@
     </row>
     <row r="7" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>263</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>266</v>
       </c>
       <c r="M7" s="5">
         <v>47</v>
@@ -12964,31 +12919,31 @@
     </row>
     <row r="8" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="H8" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>275</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>278</v>
       </c>
       <c r="M8" s="5">
         <v>40</v>
@@ -13002,28 +12957,28 @@
     </row>
     <row r="9" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="M9" s="5">
         <v>99</v>
@@ -13037,25 +12992,25 @@
     </row>
     <row r="10" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>253</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>256</v>
       </c>
       <c r="M10" s="5">
         <v>312</v>
@@ -13069,28 +13024,28 @@
     </row>
     <row r="11" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E11" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>265</v>
-      </c>
       <c r="I11" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="M11" s="5">
         <v>147</v>
@@ -13578,12 +13533,12 @@
   <sheetPr>
     <tabColor rgb="FFD6E3BC"/>
   </sheetPr>
-  <dimension ref="A1:AA1004"/>
+  <dimension ref="A1:AA1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13602,28 +13557,28 @@
   <sheetData>
     <row r="1" spans="1:27" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="H1" s="34" t="s">
         <v>60</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>61</v>
       </c>
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
@@ -13647,28 +13602,28 @@
     </row>
     <row r="2" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="54" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="21" t="s">
-        <v>63</v>
-      </c>
       <c r="E2" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I2" s="19"/>
       <c r="J2" s="19"/>
@@ -13692,26 +13647,26 @@
     </row>
     <row r="3" spans="1:27" ht="136" x14ac:dyDescent="0.2">
       <c r="A3" s="56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E3" s="24"/>
       <c r="F3" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="H3" s="36" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I3" s="19"/>
       <c r="J3" s="19"/>
@@ -13735,28 +13690,28 @@
     </row>
     <row r="4" spans="1:27" ht="306" x14ac:dyDescent="0.2">
       <c r="A4" s="56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="23" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F4" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="24" t="s">
-        <v>224</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>68</v>
-      </c>
       <c r="G4" s="25" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H4" s="41" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
@@ -13780,23 +13735,23 @@
     </row>
     <row r="5" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A5" s="56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E5" s="24"/>
       <c r="F5" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G5" s="47" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="H5" s="42"/>
       <c r="I5" s="19"/>
@@ -13819,28 +13774,28 @@
       <c r="Z5" s="19"/>
       <c r="AA5" s="19"/>
     </row>
-    <row r="6" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="24"/>
+      <c r="F6" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="24"/>
       <c r="G6" s="44" t="s">
-        <v>289</v>
-      </c>
-      <c r="H6" s="36">
-        <v>80698</v>
+        <v>285</v>
+      </c>
+      <c r="H6" s="37" t="s">
+        <v>73</v>
       </c>
       <c r="I6" s="19"/>
       <c r="J6" s="19"/>
@@ -13862,15 +13817,15 @@
       <c r="Z6" s="19"/>
       <c r="AA6" s="19"/>
     </row>
-    <row r="7" spans="1:27" ht="85" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="119" x14ac:dyDescent="0.2">
       <c r="A7" s="56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>74</v>
@@ -13879,12 +13834,8 @@
       <c r="F7" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="G7" s="44" t="s">
-        <v>288</v>
-      </c>
-      <c r="H7" s="37" t="s">
-        <v>76</v>
-      </c>
+      <c r="G7" s="25"/>
+      <c r="H7" s="36"/>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
@@ -13905,22 +13856,22 @@
       <c r="Z7" s="19"/>
       <c r="AA7" s="19"/>
     </row>
-    <row r="8" spans="1:27" ht="119" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="136" x14ac:dyDescent="0.2">
       <c r="A8" s="56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E8" s="24"/>
       <c r="F8" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G8" s="25"/>
       <c r="H8" s="36"/>
@@ -13944,25 +13895,31 @@
       <c r="Z8" s="19"/>
       <c r="AA8" s="19"/>
     </row>
-    <row r="9" spans="1:27" ht="136" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="119" x14ac:dyDescent="0.2">
       <c r="A9" s="56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="24"/>
       <c r="F9" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="G9" s="25"/>
-      <c r="H9" s="36"/>
+      <c r="G9" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>82</v>
+      </c>
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
@@ -13983,31 +13940,25 @@
       <c r="Z9" s="19"/>
       <c r="AA9" s="19"/>
     </row>
-    <row r="10" spans="1:27" ht="119" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" ht="153" x14ac:dyDescent="0.2">
       <c r="A10" s="56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>82</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="E10" s="24"/>
       <c r="F10" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="G10" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H10" s="36" t="s">
         <v>85</v>
       </c>
+      <c r="G10" s="25"/>
+      <c r="H10" s="36"/>
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
@@ -14028,25 +13979,31 @@
       <c r="Z10" s="19"/>
       <c r="AA10" s="19"/>
     </row>
-    <row r="11" spans="1:27" ht="153" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="119" x14ac:dyDescent="0.2">
       <c r="A11" s="56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="E11" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="24"/>
       <c r="F11" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="25"/>
-      <c r="H11" s="36"/>
+      <c r="G11" s="44" t="s">
+        <v>284</v>
+      </c>
+      <c r="H11" s="36" t="s">
+        <v>232</v>
+      </c>
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
@@ -14067,15 +14024,15 @@
       <c r="Z11" s="19"/>
       <c r="AA11" s="19"/>
     </row>
-    <row r="12" spans="1:27" ht="119" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" s="23" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>89</v>
@@ -14083,15 +14040,11 @@
       <c r="E12" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="G12" s="44" t="s">
-        <v>287</v>
-      </c>
-      <c r="H12" s="36" t="s">
-        <v>235</v>
-      </c>
+      <c r="G12" s="25"/>
+      <c r="H12" s="36"/>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
@@ -14112,15 +14065,15 @@
       <c r="Z12" s="19"/>
       <c r="AA12" s="19"/>
     </row>
-    <row r="13" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" s="23" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>92</v>
@@ -14153,24 +14106,22 @@
       <c r="Z13" s="19"/>
       <c r="AA13" s="19"/>
     </row>
-    <row r="14" spans="1:27" ht="102" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="23" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D14" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="24"/>
+      <c r="F14" s="26" t="s">
         <v>96</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>97</v>
       </c>
       <c r="G14" s="25"/>
       <c r="H14" s="36"/>
@@ -14194,22 +14145,22 @@
       <c r="Z14" s="19"/>
       <c r="AA14" s="19"/>
     </row>
-    <row r="15" spans="1:27" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="23" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="D15" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24" t="s">
         <v>98</v>
-      </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="26" t="s">
-        <v>99</v>
       </c>
       <c r="G15" s="25"/>
       <c r="H15" s="36"/>
@@ -14235,20 +14186,20 @@
     </row>
     <row r="16" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" s="23" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D16" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="24"/>
+      <c r="F16" s="26" t="s">
         <v>100</v>
-      </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24" t="s">
-        <v>101</v>
       </c>
       <c r="G16" s="25"/>
       <c r="H16" s="36"/>
@@ -14272,22 +14223,22 @@
       <c r="Z16" s="19"/>
       <c r="AA16" s="19"/>
     </row>
-    <row r="17" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E17" s="24"/>
       <c r="F17" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G17" s="25"/>
       <c r="H17" s="36"/>
@@ -14311,25 +14262,25 @@
       <c r="Z17" s="19"/>
       <c r="AA17" s="19"/>
     </row>
-    <row r="18" spans="1:27" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="56" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="23" t="s">
+    <row r="18" spans="1:27" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="D18" s="24" t="s">
+      <c r="C18" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="G18" s="25"/>
-      <c r="H18" s="36"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="38"/>
       <c r="I18" s="19"/>
       <c r="J18" s="19"/>
       <c r="K18" s="19"/>
@@ -14350,25 +14301,31 @@
       <c r="Z18" s="19"/>
       <c r="AA18" s="19"/>
     </row>
-    <row r="19" spans="1:27" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="57" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="G19" s="29"/>
-      <c r="H19" s="38"/>
+    <row r="19" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+      <c r="A19" s="54" t="s">
+        <v>296</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="H19" s="35" t="s">
+        <v>196</v>
+      </c>
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
       <c r="K19" s="19"/>
@@ -14389,31 +14346,27 @@
       <c r="Z19" s="19"/>
       <c r="AA19" s="19"/>
     </row>
-    <row r="20" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A20" s="54" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="H20" s="35" t="s">
-        <v>199</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" s="25"/>
+      <c r="H20" s="36"/>
       <c r="I20" s="19"/>
       <c r="J20" s="19"/>
       <c r="K20" s="19"/>
@@ -14434,24 +14387,22 @@
       <c r="Z20" s="19"/>
       <c r="AA20" s="19"/>
     </row>
-    <row r="21" spans="1:27" ht="102" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="54" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B21" s="23" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D21" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="E21" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="F21" s="24" t="s">
-        <v>110</v>
+      <c r="E21" s="24"/>
+      <c r="F21" s="26" t="s">
+        <v>201</v>
       </c>
       <c r="G21" s="25"/>
       <c r="H21" s="36"/>
@@ -14475,22 +14426,22 @@
       <c r="Z21" s="19"/>
       <c r="AA21" s="19"/>
     </row>
-    <row r="22" spans="1:27" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="54" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B22" s="23" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E22" s="24"/>
-      <c r="F22" s="26" t="s">
-        <v>204</v>
+      <c r="F22" s="24" t="s">
+        <v>110</v>
       </c>
       <c r="G22" s="25"/>
       <c r="H22" s="36"/>
@@ -14514,22 +14465,22 @@
       <c r="Z22" s="19"/>
       <c r="AA22" s="19"/>
     </row>
-    <row r="23" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A23" s="54" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B23" s="23" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G23" s="25"/>
       <c r="H23" s="36"/>
@@ -14553,22 +14504,22 @@
       <c r="Z23" s="19"/>
       <c r="AA23" s="19"/>
     </row>
-    <row r="24" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="54" t="s">
-        <v>299</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>114</v>
+        <v>295</v>
+      </c>
+      <c r="B24" s="48" t="s">
+        <v>289</v>
+      </c>
+      <c r="C24" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="49" t="s">
+        <v>290</v>
       </c>
       <c r="E24" s="24"/>
-      <c r="F24" s="24" t="s">
-        <v>115</v>
+      <c r="F24" s="53" t="s">
+        <v>294</v>
       </c>
       <c r="G24" s="25"/>
       <c r="H24" s="36"/>
@@ -14594,20 +14545,20 @@
     </row>
     <row r="25" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="54" t="s">
-        <v>299</v>
-      </c>
-      <c r="B25" s="48" t="s">
-        <v>293</v>
-      </c>
-      <c r="C25" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="49" t="s">
-        <v>294</v>
+        <v>295</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>113</v>
       </c>
       <c r="E25" s="24"/>
-      <c r="F25" s="53" t="s">
-        <v>298</v>
+      <c r="F25" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="G25" s="25"/>
       <c r="H25" s="36"/>
@@ -14633,20 +14584,20 @@
     </row>
     <row r="26" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="54" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B26" s="23" t="s">
         <v>22</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E26" s="24"/>
       <c r="F26" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G26" s="25"/>
       <c r="H26" s="36"/>
@@ -14670,25 +14621,25 @@
       <c r="Z26" s="19"/>
       <c r="AA26" s="19"/>
     </row>
-    <row r="27" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="54" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B27" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D27" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="G27" s="25"/>
-      <c r="H27" s="36"/>
       <c r="I27" s="19"/>
       <c r="J27" s="19"/>
       <c r="K27" s="19"/>
@@ -14711,22 +14662,22 @@
     </row>
     <row r="28" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="54" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B28" s="23" t="s">
         <v>24</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E28" s="24"/>
       <c r="F28" s="24"/>
       <c r="G28" s="25"/>
       <c r="H28" s="36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I28" s="19"/>
       <c r="J28" s="19"/>
@@ -14750,22 +14701,28 @@
     </row>
     <row r="29" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="54" t="s">
-        <v>299</v>
-      </c>
-      <c r="B29" s="23" t="s">
-        <v>25</v>
+        <v>295</v>
+      </c>
+      <c r="B29" s="50" t="s">
+        <v>291</v>
       </c>
       <c r="C29" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="36" t="s">
-        <v>123</v>
+      <c r="E29" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="G29" s="51" t="s">
+        <v>292</v>
+      </c>
+      <c r="H29" s="52" t="s">
+        <v>293</v>
       </c>
       <c r="I29" s="19"/>
       <c r="J29" s="19"/>
@@ -14787,30 +14744,30 @@
       <c r="Z29" s="19"/>
       <c r="AA29" s="19"/>
     </row>
-    <row r="30" spans="1:27" ht="34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A30" s="54" t="s">
-        <v>299</v>
-      </c>
-      <c r="B30" s="50" t="s">
         <v>295</v>
       </c>
+      <c r="B30" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="C30" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="F30" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G30" s="51" t="s">
-        <v>296</v>
-      </c>
-      <c r="H30" s="52" t="s">
-        <v>297</v>
+        <v>61</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="F30" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="H30" s="36" t="s">
+        <v>225</v>
       </c>
       <c r="I30" s="19"/>
       <c r="J30" s="19"/>
@@ -14834,28 +14791,28 @@
     </row>
     <row r="31" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A31" s="54" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B31" s="23" t="s">
         <v>26</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D31" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="F31" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="E31" s="24" t="s">
-        <v>226</v>
-      </c>
-      <c r="F31" s="26" t="s">
-        <v>227</v>
-      </c>
       <c r="G31" s="25" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H31" s="36" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
@@ -14877,30 +14834,30 @@
       <c r="Z31" s="19"/>
       <c r="AA31" s="19"/>
     </row>
-    <row r="32" spans="1:27" ht="204" x14ac:dyDescent="0.2">
-      <c r="A32" s="54" t="s">
-        <v>299</v>
-      </c>
-      <c r="B32" s="23" t="s">
+    <row r="32" spans="1:27" ht="154" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="57" t="s">
+        <v>295</v>
+      </c>
+      <c r="B32" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D32" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="E32" s="24" t="s">
+      <c r="C32" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="F32" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G32" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="H32" s="38" t="s">
         <v>231</v>
-      </c>
-      <c r="F32" s="24" t="s">
-        <v>232</v>
-      </c>
-      <c r="G32" s="25" t="s">
-        <v>242</v>
-      </c>
-      <c r="H32" s="36" t="s">
-        <v>233</v>
       </c>
       <c r="I32" s="19"/>
       <c r="J32" s="19"/>
@@ -14922,30 +14879,30 @@
       <c r="Z32" s="19"/>
       <c r="AA32" s="19"/>
     </row>
-    <row r="33" spans="1:27" ht="154" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="57" t="s">
-        <v>299</v>
-      </c>
-      <c r="B33" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="27" t="s">
+    <row r="33" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+      <c r="A33" s="54" t="s">
+        <v>297</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="E33" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="F33" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="G33" s="29" t="s">
-        <v>243</v>
-      </c>
-      <c r="H33" s="38" t="s">
-        <v>234</v>
+      <c r="D33" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="G33" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="H33" s="35" t="s">
+        <v>196</v>
       </c>
       <c r="I33" s="19"/>
       <c r="J33" s="19"/>
@@ -14967,31 +14924,29 @@
       <c r="Z33" s="19"/>
       <c r="AA33" s="19"/>
     </row>
-    <row r="34" spans="1:27" ht="68" x14ac:dyDescent="0.2">
-      <c r="A34" s="54" t="s">
-        <v>301</v>
-      </c>
-      <c r="B34" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="E34" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="F34" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="G34" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="H34" s="35" t="s">
-        <v>199</v>
-      </c>
+    <row r="34" spans="1:27" ht="204" x14ac:dyDescent="0.2">
+      <c r="A34" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="E34" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="F34" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="G34" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="H34" s="36"/>
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
       <c r="K34" s="19"/>
@@ -15012,15 +14967,15 @@
       <c r="Z34" s="19"/>
       <c r="AA34" s="19"/>
     </row>
-    <row r="35" spans="1:27" ht="204" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="56" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B35" s="23" t="s">
         <v>30</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D35" s="24" t="s">
         <v>128</v>
@@ -15031,9 +14986,7 @@
       <c r="F35" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="G35" s="44" t="s">
-        <v>290</v>
-      </c>
+      <c r="G35" s="25"/>
       <c r="H35" s="36"/>
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
@@ -15055,24 +15008,22 @@
       <c r="Z35" s="19"/>
       <c r="AA35" s="19"/>
     </row>
-    <row r="36" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="56" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B36" s="23" t="s">
         <v>31</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D36" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="E36" s="24" t="s">
+      <c r="E36" s="24"/>
+      <c r="F36" s="24" t="s">
         <v>132</v>
-      </c>
-      <c r="F36" s="24" t="s">
-        <v>133</v>
       </c>
       <c r="G36" s="25"/>
       <c r="H36" s="36"/>
@@ -15096,20 +15047,22 @@
       <c r="Z36" s="19"/>
       <c r="AA36" s="19"/>
     </row>
-    <row r="37" spans="1:27" ht="34" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" ht="119" x14ac:dyDescent="0.2">
       <c r="A37" s="56" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B37" s="23" t="s">
         <v>32</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D37" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="E37" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="E37" s="24"/>
       <c r="F37" s="24" t="s">
         <v>135</v>
       </c>
@@ -15135,24 +15088,24 @@
       <c r="Z37" s="19"/>
       <c r="AA37" s="19"/>
     </row>
-    <row r="38" spans="1:27" ht="119" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A38" s="56" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B38" s="23" t="s">
         <v>33</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>73</v>
+        <v>136</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G38" s="25"/>
       <c r="H38" s="36"/>
@@ -15176,15 +15129,15 @@
       <c r="Z38" s="19"/>
       <c r="AA38" s="19"/>
     </row>
-    <row r="39" spans="1:27" ht="85" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A39" s="56" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B39" s="23" t="s">
         <v>34</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>139</v>
+        <v>70</v>
       </c>
       <c r="D39" s="24" t="s">
         <v>140</v>
@@ -15217,15 +15170,15 @@
       <c r="Z39" s="19"/>
       <c r="AA39" s="19"/>
     </row>
-    <row r="40" spans="1:27" ht="102" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="56" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B40" s="23" t="s">
         <v>35</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D40" s="24" t="s">
         <v>143</v>
@@ -15258,15 +15211,15 @@
       <c r="Z40" s="19"/>
       <c r="AA40" s="19"/>
     </row>
-    <row r="41" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A41" s="56" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B41" s="23" t="s">
         <v>36</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D41" s="24" t="s">
         <v>146</v>
@@ -15299,15 +15252,15 @@
       <c r="Z41" s="19"/>
       <c r="AA41" s="19"/>
     </row>
-    <row r="42" spans="1:27" ht="102" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A42" s="56" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B42" s="23" t="s">
         <v>37</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D42" s="24" t="s">
         <v>149</v>
@@ -15340,15 +15293,15 @@
       <c r="Z42" s="19"/>
       <c r="AA42" s="19"/>
     </row>
-    <row r="43" spans="1:27" ht="85" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A43" s="56" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B43" s="23" t="s">
         <v>38</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="D43" s="24" t="s">
         <v>152</v>
@@ -15381,27 +15334,27 @@
       <c r="Z43" s="19"/>
       <c r="AA43" s="19"/>
     </row>
-    <row r="44" spans="1:27" ht="68" x14ac:dyDescent="0.2">
-      <c r="A44" s="56" t="s">
-        <v>127</v>
-      </c>
-      <c r="B44" s="23" t="s">
+    <row r="44" spans="1:27" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="B44" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D44" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="E44" s="24" t="s">
+      <c r="E44" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="F44" s="24" t="s">
+      <c r="F44" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="G44" s="25"/>
-      <c r="H44" s="36"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="38"/>
       <c r="I44" s="19"/>
       <c r="J44" s="19"/>
       <c r="K44" s="19"/>
@@ -15422,27 +15375,31 @@
       <c r="Z44" s="19"/>
       <c r="AA44" s="19"/>
     </row>
-    <row r="45" spans="1:27" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="57" t="s">
-        <v>127</v>
-      </c>
-      <c r="B45" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="C45" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D45" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="E45" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="F45" s="28" t="s">
-        <v>160</v>
-      </c>
-      <c r="G45" s="29"/>
-      <c r="H45" s="38"/>
+    <row r="45" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+      <c r="A45" s="61" t="s">
+        <v>301</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D45" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F45" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="G45" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="H45" s="35" t="s">
+        <v>196</v>
+      </c>
       <c r="I45" s="19"/>
       <c r="J45" s="19"/>
       <c r="K45" s="19"/>
@@ -15463,30 +15420,30 @@
       <c r="Z45" s="19"/>
       <c r="AA45" s="19"/>
     </row>
-    <row r="46" spans="1:27" ht="68" x14ac:dyDescent="0.2">
-      <c r="A46" s="61" t="s">
-        <v>305</v>
-      </c>
-      <c r="B46" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C46" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="D46" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="E46" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="F46" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="G46" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="H46" s="35" t="s">
-        <v>199</v>
+    <row r="46" spans="1:27" ht="205" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="57" t="s">
+        <v>218</v>
+      </c>
+      <c r="B46" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D46" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="E46" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="F46" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="G46" s="45" t="s">
+        <v>287</v>
+      </c>
+      <c r="H46" s="38" t="s">
+        <v>235</v>
       </c>
       <c r="I46" s="19"/>
       <c r="J46" s="19"/>
@@ -15508,30 +15465,30 @@
       <c r="Z46" s="19"/>
       <c r="AA46" s="19"/>
     </row>
-    <row r="47" spans="1:27" ht="205" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="57" t="s">
-        <v>221</v>
-      </c>
-      <c r="B47" s="27" t="s">
-        <v>220</v>
-      </c>
-      <c r="C47" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="D47" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="E47" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="F47" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="G47" s="45" t="s">
-        <v>291</v>
-      </c>
-      <c r="H47" s="38" t="s">
-        <v>238</v>
+    <row r="47" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+      <c r="A47" s="54" t="s">
+        <v>299</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C47" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E47" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F47" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="G47" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="H47" s="35" t="s">
+        <v>160</v>
       </c>
       <c r="I47" s="19"/>
       <c r="J47" s="19"/>
@@ -15554,29 +15511,29 @@
       <c r="AA47" s="19"/>
     </row>
     <row r="48" spans="1:27" ht="68" x14ac:dyDescent="0.2">
-      <c r="A48" s="54" t="s">
-        <v>303</v>
+      <c r="A48" s="58" t="s">
+        <v>161</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="C48" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D48" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="E48" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="F48" s="31" t="s">
-        <v>63</v>
+      <c r="E48" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F48" s="21" t="s">
+        <v>62</v>
       </c>
       <c r="G48" s="22" t="s">
-        <v>162</v>
+        <v>237</v>
       </c>
       <c r="H48" s="35" t="s">
-        <v>163</v>
+        <v>196</v>
       </c>
       <c r="I48" s="19"/>
       <c r="J48" s="19"/>
@@ -15598,30 +15555,30 @@
       <c r="Z48" s="19"/>
       <c r="AA48" s="19"/>
     </row>
-    <row r="49" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:27" ht="119" x14ac:dyDescent="0.2">
       <c r="A49" s="58" t="s">
+        <v>161</v>
+      </c>
+      <c r="B49" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="C49" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="B49" s="20" t="s">
+      <c r="E49" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="C49" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="D49" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="E49" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="F49" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="G49" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="H49" s="35" t="s">
-        <v>199</v>
+      <c r="F49" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="G49" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="H49" s="36">
+        <v>486</v>
       </c>
       <c r="I49" s="19"/>
       <c r="J49" s="19"/>
@@ -15643,30 +15600,26 @@
       <c r="Z49" s="19"/>
       <c r="AA49" s="19"/>
     </row>
-    <row r="50" spans="1:27" ht="119" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A50" s="58" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>166</v>
+        <v>41</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>167</v>
-      </c>
-      <c r="E50" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="F50" s="24" t="s">
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="G50" s="25" t="s">
+      <c r="H50" s="36" t="s">
         <v>170</v>
-      </c>
-      <c r="H50" s="36">
-        <v>486</v>
       </c>
       <c r="I50" s="19"/>
       <c r="J50" s="19"/>
@@ -15688,26 +15641,28 @@
       <c r="Z50" s="19"/>
       <c r="AA50" s="19"/>
     </row>
-    <row r="51" spans="1:27" ht="204" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A51" s="58" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B51" s="23" t="s">
         <v>42</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D51" s="24" t="s">
         <v>171</v>
       </c>
       <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
+      <c r="F51" s="24" t="s">
+        <v>172</v>
+      </c>
       <c r="G51" s="25" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="H51" s="36" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="I51" s="19"/>
       <c r="J51" s="19"/>
@@ -15729,29 +15684,27 @@
       <c r="Z51" s="19"/>
       <c r="AA51" s="19"/>
     </row>
-    <row r="52" spans="1:27" ht="102" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A52" s="58" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B52" s="23" t="s">
         <v>43</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E52" s="24"/>
       <c r="F52" s="24" t="s">
-        <v>175</v>
-      </c>
-      <c r="G52" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="H52" s="36" t="s">
-        <v>196</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="G52" s="43" t="s">
+        <v>236</v>
+      </c>
+      <c r="H52" s="36"/>
       <c r="I52" s="19"/>
       <c r="J52" s="19"/>
       <c r="K52" s="19"/>
@@ -15772,15 +15725,15 @@
       <c r="Z52" s="19"/>
       <c r="AA52" s="19"/>
     </row>
-    <row r="53" spans="1:27" ht="85" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="58" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B53" s="23" t="s">
         <v>44</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>62</v>
+        <v>175</v>
       </c>
       <c r="D53" s="24" t="s">
         <v>176</v>
@@ -15789,9 +15742,7 @@
       <c r="F53" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="G53" s="43" t="s">
-        <v>239</v>
-      </c>
+      <c r="G53" s="25"/>
       <c r="H53" s="36"/>
       <c r="I53" s="19"/>
       <c r="J53" s="19"/>
@@ -15815,20 +15766,20 @@
     </row>
     <row r="54" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="58" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B54" s="23" t="s">
         <v>45</v>
       </c>
       <c r="C54" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="D54" s="24" t="s">
         <v>178</v>
-      </c>
-      <c r="D54" s="24" t="s">
-        <v>179</v>
       </c>
       <c r="E54" s="24"/>
       <c r="F54" s="24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G54" s="25"/>
       <c r="H54" s="36"/>
@@ -15854,20 +15805,20 @@
     </row>
     <row r="55" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="58" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B55" s="23" t="s">
         <v>46</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D55" s="24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E55" s="24"/>
       <c r="F55" s="24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G55" s="25"/>
       <c r="H55" s="36"/>
@@ -15893,20 +15844,20 @@
     </row>
     <row r="56" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" s="58" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B56" s="23" t="s">
         <v>47</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D56" s="24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E56" s="24"/>
       <c r="F56" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G56" s="25"/>
       <c r="H56" s="36"/>
@@ -15932,20 +15883,20 @@
     </row>
     <row r="57" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" s="58" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B57" s="23" t="s">
         <v>48</v>
       </c>
       <c r="C57" s="23" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E57" s="24"/>
       <c r="F57" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G57" s="25"/>
       <c r="H57" s="36"/>
@@ -15971,20 +15922,20 @@
     </row>
     <row r="58" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="58" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B58" s="23" t="s">
         <v>49</v>
       </c>
       <c r="C58" s="23" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D58" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E58" s="24"/>
       <c r="F58" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G58" s="25"/>
       <c r="H58" s="36"/>
@@ -16008,24 +15959,26 @@
       <c r="Z58" s="19"/>
       <c r="AA58" s="19"/>
     </row>
-    <row r="59" spans="1:27" ht="34" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A59" s="58" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B59" s="23" t="s">
         <v>50</v>
       </c>
       <c r="C59" s="23" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D59" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E59" s="24"/>
       <c r="F59" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="G59" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="G59" s="25"/>
       <c r="H59" s="36"/>
       <c r="I59" s="19"/>
       <c r="J59" s="19"/>
@@ -16047,27 +16000,31 @@
       <c r="Z59" s="19"/>
       <c r="AA59" s="19"/>
     </row>
-    <row r="60" spans="1:27" ht="68" x14ac:dyDescent="0.2">
-      <c r="A60" s="58" t="s">
-        <v>164</v>
-      </c>
-      <c r="B60" s="23" t="s">
+    <row r="60" spans="1:27" ht="103" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="59" t="s">
+        <v>161</v>
+      </c>
+      <c r="B60" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C60" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="D60" s="24" t="s">
+      <c r="C60" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="D60" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="E60" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F60" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="G60" s="29" t="s">
         <v>191</v>
       </c>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="G60" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="H60" s="36"/>
+      <c r="H60" s="38" t="s">
+        <v>52</v>
+      </c>
       <c r="I60" s="19"/>
       <c r="J60" s="19"/>
       <c r="K60" s="19"/>
@@ -16088,50 +16045,34 @@
       <c r="Z60" s="19"/>
       <c r="AA60" s="19"/>
     </row>
-    <row r="61" spans="1:27" ht="103" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="59" t="s">
-        <v>164</v>
-      </c>
-      <c r="B61" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="C61" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="D61" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="E61" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="F61" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="G61" s="29" t="s">
-        <v>194</v>
-      </c>
-      <c r="H61" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="I61" s="19"/>
-      <c r="J61" s="19"/>
-      <c r="K61" s="19"/>
-      <c r="L61" s="19"/>
-      <c r="M61" s="19"/>
-      <c r="N61" s="19"/>
-      <c r="O61" s="19"/>
-      <c r="P61" s="19"/>
-      <c r="Q61" s="19"/>
-      <c r="R61" s="19"/>
-      <c r="S61" s="19"/>
-      <c r="T61" s="19"/>
-      <c r="U61" s="19"/>
-      <c r="V61" s="19"/>
-      <c r="W61" s="19"/>
-      <c r="X61" s="19"/>
-      <c r="Y61" s="19"/>
-      <c r="Z61" s="19"/>
-      <c r="AA61" s="19"/>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A61" s="60"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="39"/>
+      <c r="I61" s="15"/>
+      <c r="J61" s="15"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="15"/>
+      <c r="M61" s="15"/>
+      <c r="N61" s="15"/>
+      <c r="O61" s="15"/>
+      <c r="P61" s="15"/>
+      <c r="Q61" s="15"/>
+      <c r="R61" s="15"/>
+      <c r="S61" s="15"/>
+      <c r="T61" s="15"/>
+      <c r="U61" s="15"/>
+      <c r="V61" s="15"/>
+      <c r="W61" s="15"/>
+      <c r="X61" s="15"/>
+      <c r="Y61" s="15"/>
+      <c r="Z61" s="15"/>
+      <c r="AA61" s="15"/>
     </row>
     <row r="62" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A62" s="60"/>
@@ -43451,35 +43392,6 @@
       <c r="Z1003" s="15"/>
       <c r="AA1003" s="15"/>
     </row>
-    <row r="1004" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A1004" s="60"/>
-      <c r="B1004" s="15"/>
-      <c r="C1004" s="15"/>
-      <c r="D1004" s="15"/>
-      <c r="E1004" s="15"/>
-      <c r="F1004" s="15"/>
-      <c r="G1004" s="15"/>
-      <c r="H1004" s="39"/>
-      <c r="I1004" s="15"/>
-      <c r="J1004" s="15"/>
-      <c r="K1004" s="15"/>
-      <c r="L1004" s="15"/>
-      <c r="M1004" s="15"/>
-      <c r="N1004" s="15"/>
-      <c r="O1004" s="15"/>
-      <c r="P1004" s="15"/>
-      <c r="Q1004" s="15"/>
-      <c r="R1004" s="15"/>
-      <c r="S1004" s="15"/>
-      <c r="T1004" s="15"/>
-      <c r="U1004" s="15"/>
-      <c r="V1004" s="15"/>
-      <c r="W1004" s="15"/>
-      <c r="X1004" s="15"/>
-      <c r="Y1004" s="15"/>
-      <c r="Z1004" s="15"/>
-      <c r="AA1004" s="15"/>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="G1:H1">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="[ needs">

</xml_diff>

<commit_message>
Clarify explanation for associatedSequences
</commit_message>
<xml_diff>
--- a/molmod/static/downloads/SBDI-ASV-template.xlsx
+++ b/molmod/static/downloads/SBDI-ASV-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/molmod/static/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4133DA-58C3-334B-819B-80537F53BDC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A8412A-7CFB-AF4B-9354-35EA54FABE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14540" yWindow="1380" windowWidth="36360" windowHeight="18940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3400" yWindow="1820" windowWidth="36360" windowHeight="18940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event" sheetId="1" r:id="rId1"/>
@@ -929,9 +929,6 @@
     <t>https://www.ebi.ac.uk/ena/browser/view/ERR1202039</t>
   </si>
   <si>
-    <t>Use this for linking to processed/denoised sequences and associated metadata, preferably in an ENA Run page. Optionally, also add link(s) to associated genome sequence(s), e.g. if you have acquired both ASV and genome sequences from a single individal.</t>
-  </si>
-  <si>
     <t>https://www.ncbi.nlm.nih.gov/biosample/15224856
 https://www.ebi.ac.uk/ena/browser/view/SAMEA3724543
 urn:uuid:a964805b-33c2-439a-beaa-6379ebbfcd03</t>
@@ -1038,6 +1035,9 @@
   <si>
     <t>KTH-2013-Baltic-16S</t>
   </si>
+  <si>
+    <t>Use this for linking to raw sequence read files and associated metadata, preferably in an ENA Run page. Optionally, also add a link to associated genome sequence(s), e.g. if you have acquired both ASV and genome sequences from a single individal (i.e. when you have barcoding rather than metabarcoding data). If so, separate entries with a pipe (|) character.</t>
+  </si>
 </sst>
 </file>
 
@@ -1047,11 +1047,18 @@
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1226,117 +1233,120 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2"/>
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2"/>
-    <xf numFmtId="164" fontId="1" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1617,19 +1627,19 @@
   <sheetData>
     <row r="1" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -1638,13 +1648,13 @@
         <v>41</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>302</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>1</v>
@@ -1698,13 +1708,13 @@
         <v>188</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>290</v>
@@ -1742,13 +1752,13 @@
         <v>187</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="17" t="s">
@@ -1796,13 +1806,13 @@
         <v>186</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="17" t="s">
@@ -5190,7 +5200,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:Z9">
     <sortCondition ref="A3:A9"/>
   </sortState>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{693BAF2D-BDDF-0F46-A91B-2426EEB1769B}"/>
     <hyperlink ref="G3" r:id="rId2" xr:uid="{50F9EBAB-90C1-0945-B3A5-D73BA3A7019E}"/>
@@ -5230,7 +5240,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>16</v>
@@ -5277,7 +5287,7 @@
         <v>188</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>193</v>
@@ -5321,7 +5331,7 @@
         <v>187</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>193</v>
@@ -5365,7 +5375,7 @@
         <v>186</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>193</v>
@@ -6378,7 +6388,7 @@
     <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{1F017430-2DBD-FF43-A14B-BC9311C9C887}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{7E4AB1A7-0ABB-7E41-9808-8A99834CE20A}"/>
@@ -6404,7 +6414,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>28</v>
@@ -9694,7 +9704,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>206</v>
@@ -13576,9 +13586,9 @@
   <dimension ref="A1:AA1011"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13643,17 +13653,17 @@
         <v>61</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C2" s="35" t="s">
         <v>59</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E2" s="36"/>
       <c r="F2" s="36" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G2" s="33" t="s">
         <v>225</v>
@@ -13685,21 +13695,21 @@
         <v>61</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C3" s="31" t="s">
         <v>59</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E3" s="30"/>
       <c r="F3" s="30" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G3" s="29"/>
       <c r="H3" s="28" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J3" s="27"/>
       <c r="K3" s="27"/>
@@ -13725,21 +13735,21 @@
         <v>61</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C4" s="31" t="s">
         <v>80</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="30" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G4" s="29"/>
       <c r="H4" s="28" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I4" s="44"/>
       <c r="J4" s="44"/>
@@ -13766,25 +13776,25 @@
         <v>61</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>80</v>
       </c>
       <c r="D5" s="30" t="s">
+        <v>310</v>
+      </c>
+      <c r="E5" s="30" t="s">
         <v>311</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="F5" s="30" t="s">
         <v>312</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="G5" s="29" t="s">
         <v>313</v>
       </c>
-      <c r="G5" s="29" t="s">
-        <v>314</v>
-      </c>
       <c r="H5" s="28" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I5" s="44"/>
       <c r="J5" s="44"/>
@@ -13811,17 +13821,17 @@
         <v>61</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C6" s="31" t="s">
         <v>67</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E6" s="30"/>
       <c r="F6" s="30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G6" s="29"/>
       <c r="H6" s="28"/>
@@ -13860,7 +13870,7 @@
       </c>
       <c r="E7" s="30"/>
       <c r="F7" s="30" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G7" s="29" t="s">
         <v>210</v>
@@ -13888,7 +13898,7 @@
       <c r="Z7" s="27"/>
       <c r="AA7" s="27"/>
     </row>
-    <row r="8" spans="1:27" ht="136" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="153" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
         <v>61</v>
       </c>
@@ -13905,8 +13915,8 @@
       <c r="F8" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="G8" s="29" t="s">
-        <v>295</v>
+      <c r="G8" s="49" t="s">
+        <v>330</v>
       </c>
       <c r="H8" s="28" t="s">
         <v>289</v>
@@ -13936,17 +13946,17 @@
         <v>61</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>67</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E9" s="30"/>
       <c r="F9" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G9" s="29"/>
       <c r="H9" s="28"/>
@@ -13975,17 +13985,17 @@
         <v>61</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>67</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G10" s="29"/>
       <c r="H10" s="28"/>
@@ -14014,19 +14024,19 @@
         <v>61</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>67</v>
       </c>
       <c r="D11" s="30" t="s">
+        <v>316</v>
+      </c>
+      <c r="E11" s="30" t="s">
         <v>317</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="F11" s="30" t="s">
         <v>318</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>319</v>
       </c>
       <c r="G11" s="29"/>
       <c r="H11" s="28"/>
@@ -14668,17 +14678,17 @@
         <v>283</v>
       </c>
       <c r="B27" s="35" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C27" s="35" t="s">
         <v>59</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E27" s="36"/>
       <c r="F27" s="36" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G27" s="33" t="s">
         <v>225</v>
@@ -15240,20 +15250,20 @@
     </row>
     <row r="41" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A41" s="34" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B41" s="35" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C41" s="35" t="s">
         <v>59</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E41" s="36"/>
       <c r="F41" s="36" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G41" s="33" t="s">
         <v>225</v>
@@ -15737,17 +15747,17 @@
         <v>286</v>
       </c>
       <c r="B53" s="35" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C53" s="35" t="s">
         <v>59</v>
       </c>
       <c r="D53" s="36" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E53" s="36"/>
       <c r="F53" s="36" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G53" s="33" t="s">
         <v>225</v>
@@ -15870,17 +15880,17 @@
         <v>157</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C56" s="31" t="s">
         <v>59</v>
       </c>
       <c r="D56" s="30" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E56" s="30"/>
       <c r="F56" s="30" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G56" s="29" t="s">
         <v>225</v>

</xml_diff>

<commit_message>
Restore associatedSequences field at occurrrence level
UU researchers requested the option of adding links to sequences 
published elsewhere, for specific ASVs (in addition to links raw data 
sequences given at event level). We will merge inputs at event & 
occurrence level in IPT view, where applicable
</commit_message>
<xml_diff>
--- a/molmod/static/downloads/SBDI-ASV-template.xlsx
+++ b/molmod/static/downloads/SBDI-ASV-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/molmod/static/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A8412A-7CFB-AF4B-9354-35EA54FABE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0790D4D9-0FCE-594F-A387-B2723D172837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="1820" windowWidth="36360" windowHeight="18940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9220" yWindow="7560" windowWidth="36360" windowHeight="18940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="guide" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">guide!$A$1:$AA$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">guide!$A$1:$AA$67</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="333">
   <si>
     <t>materialSampleID</t>
   </si>
@@ -1036,7 +1036,13 @@
     <t>KTH-2013-Baltic-16S</t>
   </si>
   <si>
-    <t>Use this for linking to raw sequence read files and associated metadata, preferably in an ENA Run page. Optionally, also add a link to associated genome sequence(s), e.g. if you have acquired both ASV and genome sequences from a single individal (i.e. when you have barcoding rather than metabarcoding data). If so, separate entries with a pipe (|) character.</t>
+    <t>Use this for linking to raw sequence read files and associated metadata, preferably in an ENA Run page.</t>
+  </si>
+  <si>
+    <t>https://plutof.ut.ee/#/sequence/view/2846870</t>
+  </si>
+  <si>
+    <t>Note that the associatedSequences field is mainly used in the event tab for (mandatory) links to raw sequence reads associated with a specific sample (see above). In the asv-table tab, you can (optionally) use it for adding links to sequences published elsewhere, for specific ASVs.</t>
   </si>
 </sst>
 </file>
@@ -1237,7 +1243,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1347,6 +1353,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1597,7 +1609,7 @@
   <dimension ref="A1:AH991"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12703,23 +12715,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N472"/>
+  <dimension ref="A1:O472"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.140625" style="5" customWidth="1"/>
     <col min="2" max="2" width="13.140625" style="5" customWidth="1"/>
-    <col min="3" max="12" width="12.140625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" style="5" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" style="5" customWidth="1"/>
-    <col min="15" max="16384" width="11.28515625" style="5"/>
+    <col min="3" max="3" width="19.42578125" style="5" customWidth="1"/>
+    <col min="4" max="13" width="12.140625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" style="5" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="5" customWidth="1"/>
+    <col min="16" max="16384" width="11.28515625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -12727,391 +12740,394 @@
         <v>40</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>229</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>234</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>235</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="L2" s="4">
+      <c r="I2" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="M2" s="4">
         <v>2235</v>
       </c>
-      <c r="M2" s="4">
+      <c r="N2" s="4">
         <v>16165</v>
       </c>
-      <c r="N2" s="4">
+      <c r="O2" s="4">
         <v>12855</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>236</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="L3" s="4">
+      <c r="M3" s="4">
         <v>1033</v>
       </c>
-      <c r="M3" s="4">
+      <c r="N3" s="4">
         <v>6836</v>
       </c>
-      <c r="N3" s="4">
+      <c r="O3" s="4">
         <v>12742</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>243</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="L4" s="4">
+      <c r="M4" s="4">
         <v>795</v>
       </c>
-      <c r="M4" s="4">
+      <c r="N4" s="4">
         <v>4941</v>
       </c>
-      <c r="N4" s="4">
+      <c r="O4" s="4">
         <v>3666</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>245</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="L5" s="4">
+      <c r="M5" s="4">
         <v>134</v>
       </c>
-      <c r="M5" s="4">
+      <c r="N5" s="4">
         <v>1187</v>
       </c>
-      <c r="N5" s="4">
+      <c r="O5" s="4">
         <v>2307</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>252</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="L6" s="4">
+      <c r="M6" s="4">
         <v>572</v>
       </c>
-      <c r="M6" s="4">
+      <c r="N6" s="4">
         <v>2827</v>
       </c>
-      <c r="N6" s="4">
+      <c r="O6" s="4">
         <v>1513</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>255</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="L7" s="4">
+      <c r="M7" s="4">
         <v>47</v>
       </c>
-      <c r="M7" s="4">
+      <c r="N7" s="4">
         <v>464</v>
       </c>
-      <c r="N7" s="4">
+      <c r="O7" s="4">
         <v>617</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>257</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="L8" s="4">
+      <c r="M8" s="4">
         <v>40</v>
       </c>
-      <c r="M8" s="4">
+      <c r="N8" s="4">
         <v>494</v>
       </c>
-      <c r="N8" s="4">
+      <c r="O8" s="4">
         <v>839</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>264</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="I9" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="L9" s="4">
+      <c r="M9" s="4">
         <v>99</v>
       </c>
-      <c r="M9" s="4">
+      <c r="N9" s="4">
         <v>1641</v>
       </c>
-      <c r="N9" s="4">
+      <c r="O9" s="4">
         <v>2961</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>267</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="L10" s="4">
+      <c r="M10" s="4">
         <v>312</v>
       </c>
-      <c r="M10" s="4">
+      <c r="N10" s="4">
         <v>1685</v>
       </c>
-      <c r="N10" s="4">
+      <c r="O10" s="4">
         <v>1689</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>269</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="L11" s="4">
+      <c r="M11" s="4">
         <v>147</v>
       </c>
-      <c r="M11" s="4">
+      <c r="N11" s="4">
         <v>1436</v>
       </c>
-      <c r="N11" s="4">
+      <c r="O11" s="4">
         <v>2784</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13583,12 +13599,12 @@
   <sheetPr>
     <tabColor rgb="FFD6E3BC"/>
   </sheetPr>
-  <dimension ref="A1:AA1011"/>
+  <dimension ref="A1:AA1012"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13898,7 +13914,7 @@
       <c r="Z7" s="27"/>
       <c r="AA7" s="27"/>
     </row>
-    <row r="8" spans="1:27" ht="153" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="136" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
         <v>61</v>
       </c>
@@ -16004,27 +16020,25 @@
       <c r="Z58" s="27"/>
       <c r="AA58" s="27"/>
     </row>
-    <row r="59" spans="1:27" ht="85" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:27" ht="136" x14ac:dyDescent="0.2">
       <c r="A59" s="31" t="s">
         <v>157</v>
       </c>
       <c r="B59" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C59" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="D59" s="30" t="s">
-        <v>167</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C59" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="D59" s="30"/>
       <c r="E59" s="30"/>
-      <c r="F59" s="30" t="s">
-        <v>168</v>
-      </c>
-      <c r="G59" s="29" t="s">
-        <v>224</v>
-      </c>
-      <c r="H59" s="28"/>
+      <c r="F59" s="30"/>
+      <c r="G59" s="49" t="s">
+        <v>332</v>
+      </c>
+      <c r="H59" s="51" t="s">
+        <v>331</v>
+      </c>
       <c r="I59" s="27"/>
       <c r="J59" s="27"/>
       <c r="K59" s="27"/>
@@ -16045,24 +16059,26 @@
       <c r="Z59" s="27"/>
       <c r="AA59" s="27"/>
     </row>
-    <row r="60" spans="1:27" ht="34" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A60" s="31" t="s">
         <v>157</v>
       </c>
       <c r="B60" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C60" s="31" t="s">
-        <v>169</v>
+        <v>59</v>
       </c>
       <c r="D60" s="30" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E60" s="30"/>
       <c r="F60" s="30" t="s">
-        <v>171</v>
-      </c>
-      <c r="G60" s="29"/>
+        <v>168</v>
+      </c>
+      <c r="G60" s="29" t="s">
+        <v>224</v>
+      </c>
       <c r="H60" s="28"/>
       <c r="I60" s="27"/>
       <c r="J60" s="27"/>
@@ -16089,17 +16105,17 @@
         <v>157</v>
       </c>
       <c r="B61" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C61" s="31" t="s">
         <v>169</v>
       </c>
       <c r="D61" s="30" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E61" s="30"/>
       <c r="F61" s="30" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G61" s="29"/>
       <c r="H61" s="28"/>
@@ -16128,17 +16144,17 @@
         <v>157</v>
       </c>
       <c r="B62" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C62" s="31" t="s">
         <v>169</v>
       </c>
       <c r="D62" s="30" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E62" s="30"/>
       <c r="F62" s="30" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G62" s="29"/>
       <c r="H62" s="28"/>
@@ -16167,17 +16183,17 @@
         <v>157</v>
       </c>
       <c r="B63" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C63" s="31" t="s">
         <v>169</v>
       </c>
       <c r="D63" s="30" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E63" s="30"/>
       <c r="F63" s="30" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G63" s="29"/>
       <c r="H63" s="28"/>
@@ -16206,17 +16222,17 @@
         <v>157</v>
       </c>
       <c r="B64" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C64" s="31" t="s">
         <v>169</v>
       </c>
       <c r="D64" s="30" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E64" s="30"/>
       <c r="F64" s="30" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G64" s="29"/>
       <c r="H64" s="28"/>
@@ -16245,17 +16261,17 @@
         <v>157</v>
       </c>
       <c r="B65" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C65" s="31" t="s">
         <v>169</v>
       </c>
       <c r="D65" s="30" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E65" s="30"/>
       <c r="F65" s="30" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G65" s="29"/>
       <c r="H65" s="28"/>
@@ -16279,26 +16295,24 @@
       <c r="Z65" s="27"/>
       <c r="AA65" s="27"/>
     </row>
-    <row r="66" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" s="31" t="s">
         <v>157</v>
       </c>
       <c r="B66" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C66" s="31" t="s">
         <v>169</v>
       </c>
       <c r="D66" s="30" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E66" s="30"/>
       <c r="F66" s="30" t="s">
-        <v>183</v>
-      </c>
-      <c r="G66" s="29" t="s">
-        <v>184</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="G66" s="29"/>
       <c r="H66" s="28"/>
       <c r="I66" s="27"/>
       <c r="J66" s="27"/>
@@ -16320,60 +16334,72 @@
       <c r="Z66" s="27"/>
       <c r="AA66" s="27"/>
     </row>
-    <row r="67" spans="1:27" ht="103" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="26" t="s">
+    <row r="67" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+      <c r="A67" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="B67" s="26" t="s">
+      <c r="B67" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C67" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="D67" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="E67" s="30"/>
+      <c r="F67" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="G67" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="H67" s="28"/>
+      <c r="I67" s="27"/>
+      <c r="J67" s="27"/>
+      <c r="K67" s="27"/>
+      <c r="L67" s="27"/>
+      <c r="M67" s="27"/>
+      <c r="N67" s="27"/>
+      <c r="O67" s="27"/>
+      <c r="P67" s="27"/>
+      <c r="Q67" s="27"/>
+      <c r="R67" s="27"/>
+      <c r="S67" s="27"/>
+      <c r="T67" s="27"/>
+      <c r="U67" s="27"/>
+      <c r="V67" s="27"/>
+      <c r="W67" s="27"/>
+      <c r="X67" s="27"/>
+      <c r="Y67" s="27"/>
+      <c r="Z67" s="27"/>
+      <c r="AA67" s="27"/>
+    </row>
+    <row r="68" spans="1:27" ht="103" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="B68" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="C67" s="26" t="s">
+      <c r="C68" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="D67" s="26" t="s">
+      <c r="D68" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="E67" s="25" t="s">
+      <c r="E68" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="F67" s="25" t="s">
+      <c r="F68" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="G67" s="24" t="s">
+      <c r="G68" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="H67" s="23" t="s">
+      <c r="H68" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="I67" s="21"/>
-      <c r="J67" s="21"/>
-      <c r="K67" s="21"/>
-      <c r="L67" s="21"/>
-      <c r="M67" s="21"/>
-      <c r="N67" s="21"/>
-      <c r="O67" s="21"/>
-      <c r="P67" s="21"/>
-      <c r="Q67" s="21"/>
-      <c r="R67" s="21"/>
-      <c r="S67" s="21"/>
-      <c r="T67" s="21"/>
-      <c r="U67" s="21"/>
-      <c r="V67" s="21"/>
-      <c r="W67" s="21"/>
-      <c r="X67" s="21"/>
-      <c r="Y67" s="21"/>
-      <c r="Z67" s="21"/>
-      <c r="AA67" s="21"/>
-    </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A68" s="21"/>
-      <c r="B68" s="21"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="21"/>
-      <c r="E68" s="21"/>
-      <c r="F68" s="21"/>
-      <c r="G68" s="21"/>
-      <c r="H68" s="22"/>
       <c r="I68" s="21"/>
       <c r="J68" s="21"/>
       <c r="K68" s="21"/>
@@ -43692,9 +43718,38 @@
       <c r="F1010" s="21"/>
       <c r="G1010" s="21"/>
       <c r="H1010" s="22"/>
+      <c r="I1010" s="21"/>
+      <c r="J1010" s="21"/>
+      <c r="K1010" s="21"/>
+      <c r="L1010" s="21"/>
+      <c r="M1010" s="21"/>
+      <c r="N1010" s="21"/>
+      <c r="O1010" s="21"/>
+      <c r="P1010" s="21"/>
+      <c r="Q1010" s="21"/>
+      <c r="R1010" s="21"/>
+      <c r="S1010" s="21"/>
+      <c r="T1010" s="21"/>
+      <c r="U1010" s="21"/>
+      <c r="V1010" s="21"/>
+      <c r="W1010" s="21"/>
+      <c r="X1010" s="21"/>
+      <c r="Y1010" s="21"/>
+      <c r="Z1010" s="21"/>
+      <c r="AA1010" s="21"/>
     </row>
     <row r="1011" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A1011" s="21"/>
       <c r="B1011" s="21"/>
+      <c r="C1011" s="21"/>
+      <c r="D1011" s="21"/>
+      <c r="E1011" s="21"/>
+      <c r="F1011" s="21"/>
+      <c r="G1011" s="21"/>
+      <c r="H1011" s="22"/>
+    </row>
+    <row r="1012" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B1012" s="21"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:H1">
@@ -43712,6 +43767,9 @@
       <formula>NOT(ISERROR(SEARCH(("[none"),(G1))))</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="H59" r:id="rId1" location="/sequence/view/2846870" xr:uid="{4B790C9F-30C5-074B-889B-AF01508D65E9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>

<commit_message>
Add ampliseq-ref to samplingProtocol and in template
</commit_message>
<xml_diff>
--- a/molmod/static/downloads/SBDI-ASV-template.xlsx
+++ b/molmod/static/downloads/SBDI-ASV-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/molmod/static/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0790D4D9-0FCE-594F-A387-B2723D172837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CA4445-5AFA-1645-B5B7-1E93A0200AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9220" yWindow="7560" windowWidth="36360" windowHeight="18940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9060" yWindow="1940" windowWidth="36360" windowHeight="18940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">guide!$A$1:$AA$67</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataSignature="AMtx7mh33fER1yIp3D1vEqs8lBeXGWFROw=="/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="335">
   <si>
     <t>materialSampleID</t>
   </si>
@@ -620,9 +620,6 @@
     <t>2013-07-13T07:08</t>
   </si>
   <si>
-    <t>200–500 mL seawater were filtered onto 0.22 μm pore-size mixed cellulose ester membrane filters; https://doi.org/10.3389/fmicb.2016.00679</t>
-  </si>
-  <si>
     <t>16S rRNA</t>
   </si>
   <si>
@@ -1009,9 +1006,6 @@
     <t>SBDI-ASV-KTH-2013-Baltic-16S</t>
   </si>
   <si>
-    <t>https://doi.org/10.3389/fmicb.2016.00679</t>
-  </si>
-  <si>
     <t>eventID</t>
   </si>
   <si>
@@ -1044,6 +1038,18 @@
   <si>
     <t>Note that the associatedSequences field is mainly used in the event tab for (mandatory) links to raw sequence reads associated with a specific sample (see above). In the asv-table tab, you can (optionally) use it for adding links to sequences published elsewhere, for specific ASVs.</t>
   </si>
+  <si>
+    <t>[See SBDI note in yellow section]</t>
+  </si>
+  <si>
+    <t>[See SBDI example in yellow section]</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3389/fmicb.2016.00679. Sequence processing was not conducted as in the journal publication, but by using the https://nf-co.re/ampliseq pipeline in which the denoising (ASV reconstruction) step was conducted with DADA2.</t>
+  </si>
+  <si>
+    <t>https://nf-co.re/ampliseq</t>
+  </si>
 </sst>
 </file>
 
@@ -1053,11 +1059,25 @@
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1239,125 +1259,128 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2"/>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2"/>
-    <xf numFmtId="164" fontId="2" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1608,8 +1631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH991"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:J1"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1639,19 +1662,19 @@
   <sheetData>
     <row r="1" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -1660,13 +1683,13 @@
         <v>41</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>301</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>1</v>
@@ -1720,25 +1743,25 @@
         <v>188</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="L2" s="13" t="s">
-        <v>192</v>
+      <c r="L2" s="16" t="s">
+        <v>333</v>
       </c>
       <c r="N2" s="4">
         <v>55.185000000000002</v>
@@ -1750,7 +1773,7 @@
         <v>79</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="X2" s="4">
         <v>3</v>
@@ -1764,26 +1787,26 @@
         <v>187</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="L3" s="13" t="s">
-        <v>192</v>
+      <c r="L3" s="16" t="s">
+        <v>333</v>
       </c>
       <c r="N3" s="4">
         <v>55.433999999999997</v>
@@ -1795,7 +1818,7 @@
         <v>79</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="X3" s="4">
         <v>3</v>
@@ -1818,26 +1841,26 @@
         <v>186</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="L4" s="13" t="s">
-        <v>192</v>
+      <c r="L4" s="16" t="s">
+        <v>333</v>
       </c>
       <c r="N4" s="4">
         <v>56.031999999999996</v>
@@ -1849,7 +1872,7 @@
         <v>79</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="X4" s="4">
         <v>3</v>
@@ -5212,7 +5235,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:Z9">
     <sortCondition ref="A3:A9"/>
   </sortState>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{693BAF2D-BDDF-0F46-A91B-2426EEB1769B}"/>
     <hyperlink ref="G3" r:id="rId2" xr:uid="{50F9EBAB-90C1-0945-B3A5-D73BA3A7019E}"/>
@@ -5230,12 +5253,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N977"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39" style="5" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" style="5" customWidth="1"/>
     <col min="4" max="4" width="22" style="5" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" style="5" customWidth="1"/>
@@ -5252,7 +5277,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>16</v>
@@ -5267,7 +5292,7 @@
         <v>19</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>20</v>
@@ -5282,7 +5307,7 @@
         <v>23</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>24</v>
@@ -5299,25 +5324,25 @@
         <v>188</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>194</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>195</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>196</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>115</v>
@@ -5326,16 +5351,16 @@
         <v>117</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5343,25 +5368,25 @@
         <v>187</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>194</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>27</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G3" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>195</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>196</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>115</v>
@@ -5370,16 +5395,16 @@
         <v>117</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5387,25 +5412,25 @@
         <v>186</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>194</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>27</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G4" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>195</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>196</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>115</v>
@@ -5414,16 +5439,16 @@
         <v>117</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6400,12 +6425,7 @@
     <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{1F017430-2DBD-FF43-A14B-BC9311C9C887}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{7E4AB1A7-0ABB-7E41-9808-8A99834CE20A}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{2ECFF2AE-1207-CE4E-AF6F-C184998F606E}"/>
-  </hyperlinks>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -6426,7 +6446,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>28</v>
@@ -6467,7 +6487,7 @@
         <v>188</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4">
@@ -6475,7 +6495,7 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -6489,13 +6509,13 @@
         <v>187</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D3" s="4">
         <v>7.23</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6503,13 +6523,13 @@
         <v>186</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D4" s="4">
         <v>6.97</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6517,7 +6537,7 @@
         <v>188</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4">
@@ -6525,7 +6545,7 @@
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6533,13 +6553,13 @@
         <v>187</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D6" s="4">
         <v>17.399999999999999</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -6553,13 +6573,13 @@
         <v>186</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D7" s="4">
         <v>16.899999999999999</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -9716,13 +9736,13 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12781,28 +12801,28 @@
     </row>
     <row r="2" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>235</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M2" s="4">
         <v>2235</v>
@@ -12816,28 +12836,28 @@
     </row>
     <row r="3" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="D3" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>241</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>242</v>
       </c>
       <c r="M3" s="4">
         <v>1033</v>
@@ -12851,22 +12871,22 @@
     </row>
     <row r="4" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>244</v>
-      </c>
       <c r="D4" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>233</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>234</v>
       </c>
       <c r="M4" s="4">
         <v>795</v>
@@ -12880,28 +12900,28 @@
     </row>
     <row r="5" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="D5" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>250</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>251</v>
       </c>
       <c r="M5" s="4">
         <v>134</v>
@@ -12915,28 +12935,28 @@
     </row>
     <row r="6" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="D6" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>253</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>254</v>
       </c>
       <c r="M6" s="4">
         <v>572</v>
@@ -12950,28 +12970,28 @@
     </row>
     <row r="7" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>256</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>250</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>251</v>
       </c>
       <c r="M7" s="4">
         <v>47</v>
@@ -12985,31 +13005,31 @@
     </row>
     <row r="8" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="D8" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>262</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>263</v>
       </c>
       <c r="M8" s="4">
         <v>40</v>
@@ -13023,28 +13043,28 @@
     </row>
     <row r="9" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="D9" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>265</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>266</v>
       </c>
       <c r="M9" s="4">
         <v>99</v>
@@ -13058,25 +13078,25 @@
     </row>
     <row r="10" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>268</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>240</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>241</v>
       </c>
       <c r="M10" s="4">
         <v>312</v>
@@ -13090,28 +13110,28 @@
     </row>
     <row r="11" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="D11" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>270</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>271</v>
       </c>
       <c r="M11" s="4">
         <v>147</v>
@@ -13602,9 +13622,9 @@
   <dimension ref="A1:AA1012"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="H59" sqref="H59"/>
+      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13622,26 +13642,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48" t="s">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="45" t="s">
         <v>58</v>
       </c>
       <c r="I1" s="27"/>
@@ -13669,20 +13689,20 @@
         <v>61</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C2" s="35" t="s">
         <v>59</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E2" s="36"/>
       <c r="F2" s="36" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H2" s="32" t="s">
         <v>188</v>
@@ -13711,21 +13731,21 @@
         <v>61</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C3" s="31" t="s">
         <v>59</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E3" s="30"/>
       <c r="F3" s="30" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G3" s="29"/>
       <c r="H3" s="28" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="J3" s="27"/>
       <c r="K3" s="27"/>
@@ -13751,24 +13771,24 @@
         <v>61</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C4" s="31" t="s">
         <v>80</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G4" s="29"/>
       <c r="H4" s="28" t="s">
-        <v>299</v>
-      </c>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
+        <v>298</v>
+      </c>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
       <c r="K4" s="27"/>
       <c r="L4" s="27"/>
       <c r="M4" s="27"/>
@@ -13792,28 +13812,28 @@
         <v>61</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>80</v>
       </c>
       <c r="D5" s="30" t="s">
+        <v>309</v>
+      </c>
+      <c r="E5" s="30" t="s">
         <v>310</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="F5" s="30" t="s">
         <v>311</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="G5" s="29" t="s">
         <v>312</v>
       </c>
-      <c r="G5" s="29" t="s">
-        <v>313</v>
-      </c>
       <c r="H5" s="28" t="s">
-        <v>303</v>
-      </c>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
+        <v>302</v>
+      </c>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
       <c r="K5" s="27"/>
       <c r="L5" s="27"/>
       <c r="M5" s="27"/>
@@ -13837,22 +13857,22 @@
         <v>61</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C6" s="31" t="s">
         <v>67</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E6" s="30"/>
       <c r="F6" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G6" s="29"/>
       <c r="H6" s="28"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
       <c r="K6" s="27"/>
       <c r="L6" s="27"/>
       <c r="M6" s="27"/>
@@ -13886,16 +13906,16 @@
       </c>
       <c r="E7" s="30"/>
       <c r="F7" s="30" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>290</v>
-      </c>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
+        <v>289</v>
+      </c>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
       <c r="K7" s="27"/>
       <c r="L7" s="27"/>
       <c r="M7" s="27"/>
@@ -13925,20 +13945,20 @@
         <v>59</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E8" s="30"/>
       <c r="F8" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="G8" s="49" t="s">
-        <v>330</v>
+      <c r="G8" s="48" t="s">
+        <v>328</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>289</v>
-      </c>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
+        <v>288</v>
+      </c>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
       <c r="K8" s="27"/>
       <c r="L8" s="27"/>
       <c r="M8" s="27"/>
@@ -13962,22 +13982,22 @@
         <v>61</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>67</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E9" s="30"/>
       <c r="F9" s="30" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G9" s="29"/>
       <c r="H9" s="28"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
       <c r="K9" s="27"/>
       <c r="L9" s="27"/>
       <c r="M9" s="27"/>
@@ -14001,22 +14021,22 @@
         <v>61</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>67</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="30" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G10" s="29"/>
       <c r="H10" s="28"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
       <c r="K10" s="27"/>
       <c r="L10" s="27"/>
       <c r="M10" s="27"/>
@@ -14040,24 +14060,24 @@
         <v>61</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>67</v>
       </c>
       <c r="D11" s="30" t="s">
+        <v>315</v>
+      </c>
+      <c r="E11" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="F11" s="30" t="s">
         <v>317</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>318</v>
       </c>
       <c r="G11" s="29"/>
       <c r="H11" s="28"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
       <c r="K11" s="27"/>
       <c r="L11" s="27"/>
       <c r="M11" s="27"/>
@@ -14090,19 +14110,19 @@
         <v>63</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F12" s="30" t="s">
         <v>64</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>212</v>
-      </c>
-      <c r="H12" s="45" t="s">
+        <v>211</v>
+      </c>
+      <c r="H12" s="44" t="s">
         <v>191</v>
       </c>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
       <c r="K12" s="27"/>
       <c r="L12" s="27"/>
       <c r="M12" s="27"/>
@@ -14139,9 +14159,11 @@
         <v>66</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>276</v>
-      </c>
-      <c r="H13" s="43"/>
+        <v>275</v>
+      </c>
+      <c r="H13" s="52" t="s">
+        <v>333</v>
+      </c>
       <c r="I13" s="27"/>
       <c r="J13" s="27"/>
       <c r="K13" s="27"/>
@@ -14180,7 +14202,7 @@
         <v>69</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H14" s="42" t="s">
         <v>70</v>
@@ -14387,10 +14409,10 @@
         <v>85</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H19" s="28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I19" s="27"/>
       <c r="J19" s="27"/>
@@ -14691,23 +14713,23 @@
     </row>
     <row r="27" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A27" s="35" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B27" s="35" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C27" s="35" t="s">
         <v>59</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E27" s="36"/>
       <c r="F27" s="36" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G27" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H27" s="32" t="s">
         <v>188</v>
@@ -14733,7 +14755,7 @@
     </row>
     <row r="28" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A28" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B28" s="31" t="s">
         <v>16</v>
@@ -14751,7 +14773,9 @@
         <v>104</v>
       </c>
       <c r="G28" s="29"/>
-      <c r="H28" s="28"/>
+      <c r="H28" s="50" t="s">
+        <v>334</v>
+      </c>
       <c r="I28" s="27"/>
       <c r="J28" s="27"/>
       <c r="K28" s="27"/>
@@ -14774,7 +14798,7 @@
     </row>
     <row r="29" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B29" s="31" t="s">
         <v>17</v>
@@ -14787,7 +14811,7 @@
       </c>
       <c r="E29" s="30"/>
       <c r="F29" s="39" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G29" s="29"/>
       <c r="H29" s="28"/>
@@ -14813,7 +14837,7 @@
     </row>
     <row r="30" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B30" s="31" t="s">
         <v>18</v>
@@ -14852,7 +14876,7 @@
     </row>
     <row r="31" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A31" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B31" s="31" t="s">
         <v>19</v>
@@ -14891,20 +14915,20 @@
     </row>
     <row r="32" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C32" s="31" t="s">
         <v>59</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E32" s="30"/>
       <c r="F32" s="39" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G32" s="29"/>
       <c r="H32" s="28"/>
@@ -14930,7 +14954,7 @@
     </row>
     <row r="33" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B33" s="31" t="s">
         <v>20</v>
@@ -14969,7 +14993,7 @@
     </row>
     <row r="34" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B34" s="31" t="s">
         <v>21</v>
@@ -15008,7 +15032,7 @@
     </row>
     <row r="35" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B35" s="31" t="s">
         <v>22</v>
@@ -15047,7 +15071,7 @@
     </row>
     <row r="36" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B36" s="31" t="s">
         <v>23</v>
@@ -15086,10 +15110,10 @@
     </row>
     <row r="37" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C37" s="31" t="s">
         <v>59</v>
@@ -15104,10 +15128,10 @@
         <v>60</v>
       </c>
       <c r="G37" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="H37" s="28" t="s">
         <v>280</v>
-      </c>
-      <c r="H37" s="28" t="s">
-        <v>281</v>
       </c>
       <c r="I37" s="27"/>
       <c r="J37" s="27"/>
@@ -15131,7 +15155,7 @@
     </row>
     <row r="38" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A38" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B38" s="31" t="s">
         <v>24</v>
@@ -15140,19 +15164,19 @@
         <v>59</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E38" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="F38" s="39" t="s">
         <v>213</v>
       </c>
-      <c r="F38" s="39" t="s">
+      <c r="G38" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="H38" s="28" t="s">
         <v>214</v>
-      </c>
-      <c r="G38" s="29" t="s">
-        <v>226</v>
-      </c>
-      <c r="H38" s="28" t="s">
-        <v>215</v>
       </c>
       <c r="I38" s="27"/>
       <c r="J38" s="27"/>
@@ -15176,7 +15200,7 @@
     </row>
     <row r="39" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A39" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B39" s="31" t="s">
         <v>25</v>
@@ -15185,19 +15209,19 @@
         <v>59</v>
       </c>
       <c r="D39" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="E39" s="30" t="s">
         <v>217</v>
       </c>
-      <c r="E39" s="30" t="s">
+      <c r="F39" s="30" t="s">
         <v>218</v>
       </c>
-      <c r="F39" s="30" t="s">
+      <c r="G39" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="H39" s="28" t="s">
         <v>219</v>
-      </c>
-      <c r="G39" s="29" t="s">
-        <v>227</v>
-      </c>
-      <c r="H39" s="28" t="s">
-        <v>220</v>
       </c>
       <c r="I39" s="27"/>
       <c r="J39" s="27"/>
@@ -15221,7 +15245,7 @@
     </row>
     <row r="40" spans="1:27" ht="154" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B40" s="26" t="s">
         <v>26</v>
@@ -15239,10 +15263,10 @@
         <v>120</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H40" s="23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I40" s="27"/>
       <c r="J40" s="27"/>
@@ -15266,23 +15290,23 @@
     </row>
     <row r="41" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A41" s="34" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B41" s="35" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C41" s="35" t="s">
         <v>59</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E41" s="36"/>
       <c r="F41" s="36" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G41" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H41" s="32" t="s">
         <v>188</v>
@@ -15327,7 +15351,7 @@
         <v>124</v>
       </c>
       <c r="G42" s="29" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H42" s="28"/>
       <c r="I42" s="27"/>
@@ -15760,23 +15784,23 @@
     </row>
     <row r="53" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A53" s="34" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B53" s="35" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C53" s="35" t="s">
         <v>59</v>
       </c>
       <c r="D53" s="36" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E53" s="36"/>
       <c r="F53" s="36" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G53" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H53" s="32" t="s">
         <v>188</v>
@@ -15803,10 +15827,10 @@
     </row>
     <row r="54" spans="1:27" ht="205" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C54" s="26" t="s">
         <v>60</v>
@@ -15821,10 +15845,10 @@
         <v>60</v>
       </c>
       <c r="G54" s="24" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H54" s="23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I54" s="27"/>
       <c r="J54" s="27"/>
@@ -15848,7 +15872,7 @@
     </row>
     <row r="55" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A55" s="34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B55" s="35" t="s">
         <v>39</v>
@@ -15896,20 +15920,20 @@
         <v>157</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C56" s="31" t="s">
         <v>59</v>
       </c>
       <c r="D56" s="30" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E56" s="30"/>
       <c r="F56" s="30" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G56" s="29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H56" s="28" t="s">
         <v>188</v>
@@ -16027,17 +16051,21 @@
       <c r="B59" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="C59" s="50" t="s">
+      <c r="C59" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="30"/>
-      <c r="G59" s="49" t="s">
+      <c r="D59" s="51" t="s">
+        <v>331</v>
+      </c>
+      <c r="E59" s="51"/>
+      <c r="F59" s="51" t="s">
         <v>332</v>
       </c>
-      <c r="H59" s="51" t="s">
-        <v>331</v>
+      <c r="G59" s="48" t="s">
+        <v>330</v>
+      </c>
+      <c r="H59" s="50" t="s">
+        <v>329</v>
       </c>
       <c r="I59" s="27"/>
       <c r="J59" s="27"/>
@@ -16077,7 +16105,7 @@
         <v>168</v>
       </c>
       <c r="G60" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H60" s="28"/>
       <c r="I60" s="27"/>
@@ -43769,6 +43797,7 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="H59" r:id="rId1" location="/sequence/view/2846870" xr:uid="{4B790C9F-30C5-074B-889B-AF01508D65E9}"/>
+    <hyperlink ref="H28" r:id="rId2" xr:uid="{2AEC0F05-091F-594E-8685-79AB31594D12}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Restore ID concatenations in IPT views and explain in guide
Ideally, we want to output globally unique IDs for events and 
occurrences in DwC, 
but do not know whether users will provide such id:s. We now 
concatenate datasetID with eventID, by default, and explain this in our 
template. This may prompt users to only apply dataset-unique eventIDs, 
but if not, we also strip datasetID from eventID in R processing.
</commit_message>
<xml_diff>
--- a/molmod/static/downloads/SBDI-ASV-template.xlsx
+++ b/molmod/static/downloads/SBDI-ASV-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/molmod/static/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CA4445-5AFA-1645-B5B7-1E93A0200AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FBED10-BDA0-A549-B198-7378753CEB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9060" yWindow="1940" windowWidth="36360" windowHeight="18940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5820" yWindow="700" windowWidth="40920" windowHeight="18000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="guide" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">guide!$A$1:$AA$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">guide!$A$1:$AA$68</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="336">
   <si>
     <t>materialSampleID</t>
   </si>
@@ -716,9 +716,6 @@
     <t>Note that, for practical reasons, we currently follow GBIF in grouping prokaryote domains Archaea and Bacteria together with e.g. eukaryote kingdoms under header 'kingdom'.</t>
   </si>
   <si>
-    <t>Unique identifier for event, as provided by data contributor. Preferably use event (sample) names that correspond to what you use in related publications.</t>
-  </si>
-  <si>
     <t>Preferably, this value should correspond to environment (biome) in your ENA submission, when applicable. You can search for ENVO_00000428 in https://www.ebi.ac.uk/ols/index, then continue downwards in the biome subtree, until you find the most specific term that accurately describes your data.</t>
   </si>
   <si>
@@ -1003,9 +1000,6 @@
     <t>datasetID</t>
   </si>
   <si>
-    <t>SBDI-ASV-KTH-2013-Baltic-16S</t>
-  </si>
-  <si>
     <t>eventID</t>
   </si>
   <si>
@@ -1050,6 +1044,15 @@
   <si>
     <t>https://nf-co.re/ampliseq</t>
   </si>
+  <si>
+    <t>Unique identifier for event, as provided by data contributor. Preferably use event (sample) names that correspond to what you use in related publications. In DwC output, we concatenate this with datasetID to make it globally unique (if needed).</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>See Sheet:event, Field:eventID.</t>
+  </si>
 </sst>
 </file>
 
@@ -1059,11 +1062,18 @@
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1259,129 +1269,135 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2"/>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1631,8 +1647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH991"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1662,19 +1678,19 @@
   <sheetData>
     <row r="1" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -1683,13 +1699,13 @@
         <v>41</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>300</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>1</v>
@@ -1743,25 +1759,25 @@
         <v>188</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>191</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="N2" s="4">
         <v>55.185000000000002</v>
@@ -1787,26 +1803,26 @@
         <v>187</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>190</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="N3" s="4">
         <v>55.433999999999997</v>
@@ -1841,26 +1857,26 @@
         <v>186</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>189</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="N4" s="4">
         <v>56.031999999999996</v>
@@ -5235,7 +5251,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:Z9">
     <sortCondition ref="A3:A9"/>
   </sortState>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{693BAF2D-BDDF-0F46-A91B-2426EEB1769B}"/>
     <hyperlink ref="G3" r:id="rId2" xr:uid="{50F9EBAB-90C1-0945-B3A5-D73BA3A7019E}"/>
@@ -5253,8 +5269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N977"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5277,7 +5293,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>16</v>
@@ -5292,7 +5308,7 @@
         <v>19</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>20</v>
@@ -5307,7 +5323,7 @@
         <v>23</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>24</v>
@@ -5324,7 +5340,7 @@
         <v>188</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>192</v>
@@ -5336,7 +5352,7 @@
         <v>27</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>194</v>
@@ -5351,7 +5367,7 @@
         <v>117</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>198</v>
@@ -5368,7 +5384,7 @@
         <v>187</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>192</v>
@@ -5380,7 +5396,7 @@
         <v>27</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>194</v>
@@ -5395,7 +5411,7 @@
         <v>117</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>198</v>
@@ -5412,7 +5428,7 @@
         <v>186</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>192</v>
@@ -5424,7 +5440,7 @@
         <v>27</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>194</v>
@@ -5439,7 +5455,7 @@
         <v>117</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>198</v>
@@ -6425,7 +6441,7 @@
     <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -6446,7 +6462,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>28</v>
@@ -9736,7 +9752,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>205</v>
@@ -12801,28 +12817,28 @@
     </row>
     <row r="2" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>234</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="M2" s="4">
         <v>2235</v>
@@ -12836,28 +12852,28 @@
     </row>
     <row r="3" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="D3" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>240</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>241</v>
       </c>
       <c r="M3" s="4">
         <v>1033</v>
@@ -12871,22 +12887,22 @@
     </row>
     <row r="4" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>243</v>
-      </c>
       <c r="D4" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>232</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>233</v>
       </c>
       <c r="M4" s="4">
         <v>795</v>
@@ -12900,28 +12916,28 @@
     </row>
     <row r="5" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="D5" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>249</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>250</v>
       </c>
       <c r="M5" s="4">
         <v>134</v>
@@ -12935,28 +12951,28 @@
     </row>
     <row r="6" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="D6" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>252</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>253</v>
       </c>
       <c r="M6" s="4">
         <v>572</v>
@@ -12970,28 +12986,28 @@
     </row>
     <row r="7" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>249</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>250</v>
       </c>
       <c r="M7" s="4">
         <v>47</v>
@@ -13005,31 +13021,31 @@
     </row>
     <row r="8" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="D8" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>261</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>262</v>
       </c>
       <c r="M8" s="4">
         <v>40</v>
@@ -13043,28 +13059,28 @@
     </row>
     <row r="9" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="D9" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>264</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>265</v>
       </c>
       <c r="M9" s="4">
         <v>99</v>
@@ -13078,25 +13094,25 @@
     </row>
     <row r="10" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>267</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>239</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>240</v>
       </c>
       <c r="M10" s="4">
         <v>312</v>
@@ -13110,28 +13126,28 @@
     </row>
     <row r="11" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="D11" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>269</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>270</v>
       </c>
       <c r="M11" s="4">
         <v>147</v>
@@ -13622,9 +13638,9 @@
   <dimension ref="A1:AA1012"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13645,7 +13661,9 @@
       <c r="A1" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="47"/>
+      <c r="B1" s="54" t="s">
+        <v>334</v>
+      </c>
       <c r="C1" s="47" t="s">
         <v>53</v>
       </c>
@@ -13684,25 +13702,25 @@
       <c r="Z1" s="27"/>
       <c r="AA1" s="27"/>
     </row>
-    <row r="2" spans="1:27" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C2" s="35" t="s">
         <v>59</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E2" s="36"/>
       <c r="F2" s="36" t="s">
-        <v>321</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>224</v>
+        <v>319</v>
+      </c>
+      <c r="G2" s="53" t="s">
+        <v>333</v>
       </c>
       <c r="H2" s="32" t="s">
         <v>188</v>
@@ -13731,21 +13749,21 @@
         <v>61</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C3" s="31" t="s">
         <v>59</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E3" s="30"/>
       <c r="F3" s="30" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G3" s="29"/>
       <c r="H3" s="28" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J3" s="27"/>
       <c r="K3" s="27"/>
@@ -13771,21 +13789,21 @@
         <v>61</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C4" s="31" t="s">
         <v>80</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G4" s="29"/>
       <c r="H4" s="28" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I4" s="43"/>
       <c r="J4" s="43"/>
@@ -13812,25 +13830,25 @@
         <v>61</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>80</v>
       </c>
       <c r="D5" s="30" t="s">
+        <v>308</v>
+      </c>
+      <c r="E5" s="30" t="s">
         <v>309</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="F5" s="30" t="s">
         <v>310</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="G5" s="29" t="s">
         <v>311</v>
       </c>
-      <c r="G5" s="29" t="s">
-        <v>312</v>
-      </c>
       <c r="H5" s="28" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -13857,17 +13875,17 @@
         <v>61</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C6" s="31" t="s">
         <v>67</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E6" s="30"/>
       <c r="F6" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G6" s="29"/>
       <c r="H6" s="28"/>
@@ -13906,13 +13924,13 @@
       </c>
       <c r="E7" s="30"/>
       <c r="F7" s="30" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G7" s="29" t="s">
         <v>209</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -13945,17 +13963,17 @@
         <v>59</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E8" s="30"/>
       <c r="F8" s="30" t="s">
         <v>166</v>
       </c>
       <c r="G8" s="48" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -13982,17 +14000,17 @@
         <v>61</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>67</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E9" s="30"/>
       <c r="F9" s="30" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G9" s="29"/>
       <c r="H9" s="28"/>
@@ -14021,17 +14039,17 @@
         <v>61</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>67</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="30" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G10" s="29"/>
       <c r="H10" s="28"/>
@@ -14060,19 +14078,19 @@
         <v>61</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>67</v>
       </c>
       <c r="D11" s="30" t="s">
+        <v>314</v>
+      </c>
+      <c r="E11" s="30" t="s">
         <v>315</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="F11" s="30" t="s">
         <v>316</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>317</v>
       </c>
       <c r="G11" s="29"/>
       <c r="H11" s="28"/>
@@ -14159,10 +14177,10 @@
         <v>66</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H13" s="52" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="I13" s="27"/>
       <c r="J13" s="27"/>
@@ -14202,7 +14220,7 @@
         <v>69</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H14" s="42" t="s">
         <v>70</v>
@@ -14409,7 +14427,7 @@
         <v>85</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H19" s="28" t="s">
         <v>221</v>
@@ -14713,23 +14731,23 @@
     </row>
     <row r="27" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A27" s="35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B27" s="35" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C27" s="35" t="s">
         <v>59</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E27" s="36"/>
       <c r="F27" s="36" t="s">
-        <v>321</v>
-      </c>
-      <c r="G27" s="33" t="s">
-        <v>224</v>
+        <v>319</v>
+      </c>
+      <c r="G27" s="53" t="s">
+        <v>335</v>
       </c>
       <c r="H27" s="32" t="s">
         <v>188</v>
@@ -14755,7 +14773,7 @@
     </row>
     <row r="28" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A28" s="38" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B28" s="31" t="s">
         <v>16</v>
@@ -14774,7 +14792,7 @@
       </c>
       <c r="G28" s="29"/>
       <c r="H28" s="50" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="I28" s="27"/>
       <c r="J28" s="27"/>
@@ -14798,7 +14816,7 @@
     </row>
     <row r="29" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="38" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B29" s="31" t="s">
         <v>17</v>
@@ -14811,7 +14829,7 @@
       </c>
       <c r="E29" s="30"/>
       <c r="F29" s="39" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G29" s="29"/>
       <c r="H29" s="28"/>
@@ -14837,7 +14855,7 @@
     </row>
     <row r="30" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="38" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B30" s="31" t="s">
         <v>18</v>
@@ -14876,7 +14894,7 @@
     </row>
     <row r="31" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A31" s="38" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B31" s="31" t="s">
         <v>19</v>
@@ -14915,20 +14933,20 @@
     </row>
     <row r="32" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="38" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C32" s="31" t="s">
         <v>59</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E32" s="30"/>
       <c r="F32" s="39" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G32" s="29"/>
       <c r="H32" s="28"/>
@@ -14954,7 +14972,7 @@
     </row>
     <row r="33" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="38" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B33" s="31" t="s">
         <v>20</v>
@@ -14993,7 +15011,7 @@
     </row>
     <row r="34" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="38" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B34" s="31" t="s">
         <v>21</v>
@@ -15032,7 +15050,7 @@
     </row>
     <row r="35" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="38" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B35" s="31" t="s">
         <v>22</v>
@@ -15071,7 +15089,7 @@
     </row>
     <row r="36" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="38" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B36" s="31" t="s">
         <v>23</v>
@@ -15110,10 +15128,10 @@
     </row>
     <row r="37" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="38" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C37" s="31" t="s">
         <v>59</v>
@@ -15128,10 +15146,10 @@
         <v>60</v>
       </c>
       <c r="G37" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="H37" s="28" t="s">
         <v>279</v>
-      </c>
-      <c r="H37" s="28" t="s">
-        <v>280</v>
       </c>
       <c r="I37" s="27"/>
       <c r="J37" s="27"/>
@@ -15155,7 +15173,7 @@
     </row>
     <row r="38" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A38" s="38" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B38" s="31" t="s">
         <v>24</v>
@@ -15173,7 +15191,7 @@
         <v>213</v>
       </c>
       <c r="G38" s="29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H38" s="28" t="s">
         <v>214</v>
@@ -15200,7 +15218,7 @@
     </row>
     <row r="39" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A39" s="38" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B39" s="31" t="s">
         <v>25</v>
@@ -15218,7 +15236,7 @@
         <v>218</v>
       </c>
       <c r="G39" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H39" s="28" t="s">
         <v>219</v>
@@ -15245,7 +15263,7 @@
     </row>
     <row r="40" spans="1:27" ht="154" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B40" s="26" t="s">
         <v>26</v>
@@ -15263,7 +15281,7 @@
         <v>120</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H40" s="23" t="s">
         <v>220</v>
@@ -15290,23 +15308,23 @@
     </row>
     <row r="41" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A41" s="34" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B41" s="35" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C41" s="35" t="s">
         <v>59</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E41" s="36"/>
       <c r="F41" s="36" t="s">
-        <v>321</v>
-      </c>
-      <c r="G41" s="33" t="s">
-        <v>224</v>
+        <v>319</v>
+      </c>
+      <c r="G41" s="53" t="s">
+        <v>335</v>
       </c>
       <c r="H41" s="32" t="s">
         <v>188</v>
@@ -15351,7 +15369,7 @@
         <v>124</v>
       </c>
       <c r="G42" s="29" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H42" s="28"/>
       <c r="I42" s="27"/>
@@ -15784,23 +15802,23 @@
     </row>
     <row r="53" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A53" s="34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B53" s="35" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C53" s="35" t="s">
         <v>59</v>
       </c>
       <c r="D53" s="36" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E53" s="36"/>
       <c r="F53" s="36" t="s">
-        <v>321</v>
-      </c>
-      <c r="G53" s="33" t="s">
-        <v>224</v>
+        <v>319</v>
+      </c>
+      <c r="G53" s="53" t="s">
+        <v>335</v>
       </c>
       <c r="H53" s="32" t="s">
         <v>188</v>
@@ -15845,7 +15863,7 @@
         <v>60</v>
       </c>
       <c r="G54" s="24" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H54" s="23" t="s">
         <v>222</v>
@@ -15872,7 +15890,7 @@
     </row>
     <row r="55" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A55" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B55" s="35" t="s">
         <v>39</v>
@@ -15920,20 +15938,20 @@
         <v>157</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C56" s="31" t="s">
         <v>59</v>
       </c>
       <c r="D56" s="30" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E56" s="30"/>
       <c r="F56" s="30" t="s">
-        <v>321</v>
-      </c>
-      <c r="G56" s="29" t="s">
-        <v>224</v>
+        <v>319</v>
+      </c>
+      <c r="G56" s="53" t="s">
+        <v>335</v>
       </c>
       <c r="H56" s="28" t="s">
         <v>188</v>
@@ -16055,17 +16073,17 @@
         <v>67</v>
       </c>
       <c r="D59" s="51" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E59" s="51"/>
       <c r="F59" s="51" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G59" s="48" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H59" s="50" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="I59" s="27"/>
       <c r="J59" s="27"/>
@@ -43780,6 +43798,7 @@
       <c r="B1012" s="21"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AA68" xr:uid="{575A2C49-581A-6A45-BB35-37E08E101A4B}"/>
   <conditionalFormatting sqref="G1:H1">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="[ needs">
       <formula>NOT(ISERROR(SEARCH(("[ needs"),(G1))))</formula>

</xml_diff>

<commit_message>
Rename misspelled column to catalogNumber
</commit_message>
<xml_diff>
--- a/molmod/static/downloads/SBDI-ASV-template.xlsx
+++ b/molmod/static/downloads/SBDI-ASV-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/molmod/static/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FBED10-BDA0-A549-B198-7378753CEB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288D9CEC-578C-2C4A-B82A-8779D755FF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="700" windowWidth="40920" windowHeight="18000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2780" yWindow="500" windowWidth="40920" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">guide!$A$1:$AA$68</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataSignature="AMtx7mh33fER1yIp3D1vEqs8lBeXGWFROw=="/>
@@ -940,9 +940,6 @@
     <t>KTH</t>
   </si>
   <si>
-    <t>catalogueNumber</t>
-  </si>
-  <si>
     <t>references</t>
   </si>
   <si>
@@ -1053,6 +1050,9 @@
   <si>
     <t>See Sheet:event, Field:eventID.</t>
   </si>
+  <si>
+    <t>catalogNumber</t>
+  </si>
 </sst>
 </file>
 
@@ -1062,11 +1062,18 @@
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1269,134 +1276,137 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="2"/>
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2"/>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1647,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH991"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1678,16 +1688,16 @@
   <sheetData>
     <row r="1" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>296</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>295</v>
@@ -1702,10 +1712,10 @@
         <v>294</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>299</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>1</v>
@@ -1759,13 +1769,13 @@
         <v>188</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>297</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>288</v>
@@ -1777,7 +1787,7 @@
         <v>191</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="N2" s="4">
         <v>55.185000000000002</v>
@@ -1803,13 +1813,13 @@
         <v>187</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>297</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="17" t="s">
@@ -1822,7 +1832,7 @@
         <v>190</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="N3" s="4">
         <v>55.433999999999997</v>
@@ -1857,13 +1867,13 @@
         <v>186</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>297</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="17" t="s">
@@ -1876,7 +1886,7 @@
         <v>189</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="N4" s="4">
         <v>56.031999999999996</v>
@@ -5251,7 +5261,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:Z9">
     <sortCondition ref="A3:A9"/>
   </sortState>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{693BAF2D-BDDF-0F46-A91B-2426EEB1769B}"/>
     <hyperlink ref="G3" r:id="rId2" xr:uid="{50F9EBAB-90C1-0945-B3A5-D73BA3A7019E}"/>
@@ -5293,7 +5303,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>16</v>
@@ -5340,7 +5350,7 @@
         <v>188</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>192</v>
@@ -5384,7 +5394,7 @@
         <v>187</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>192</v>
@@ -5428,7 +5438,7 @@
         <v>186</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>192</v>
@@ -6441,7 +6451,7 @@
     <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -6462,7 +6472,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>28</v>
@@ -9752,7 +9762,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>205</v>
@@ -13637,10 +13647,10 @@
   </sheetPr>
   <dimension ref="A1:AA1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13662,7 +13672,7 @@
         <v>52</v>
       </c>
       <c r="B1" s="54" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C1" s="47" t="s">
         <v>53</v>
@@ -13707,20 +13717,20 @@
         <v>61</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C2" s="35" t="s">
         <v>59</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E2" s="36"/>
       <c r="F2" s="36" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G2" s="53" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H2" s="32" t="s">
         <v>188</v>
@@ -13749,21 +13759,21 @@
         <v>61</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C3" s="31" t="s">
         <v>59</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E3" s="30"/>
       <c r="F3" s="30" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G3" s="29"/>
       <c r="H3" s="28" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J3" s="27"/>
       <c r="K3" s="27"/>
@@ -13795,11 +13805,11 @@
         <v>80</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G4" s="29"/>
       <c r="H4" s="28" t="s">
@@ -13830,25 +13840,25 @@
         <v>61</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>80</v>
       </c>
       <c r="D5" s="30" t="s">
+        <v>307</v>
+      </c>
+      <c r="E5" s="30" t="s">
         <v>308</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="F5" s="30" t="s">
         <v>309</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="G5" s="29" t="s">
         <v>310</v>
       </c>
-      <c r="G5" s="29" t="s">
-        <v>311</v>
-      </c>
       <c r="H5" s="28" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -13881,11 +13891,11 @@
         <v>67</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E6" s="30"/>
       <c r="F6" s="30" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G6" s="29"/>
       <c r="H6" s="28"/>
@@ -13970,7 +13980,7 @@
         <v>166</v>
       </c>
       <c r="G8" s="48" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H8" s="28" t="s">
         <v>287</v>
@@ -14006,11 +14016,11 @@
         <v>67</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E9" s="30"/>
       <c r="F9" s="30" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G9" s="29"/>
       <c r="H9" s="28"/>
@@ -14038,18 +14048,18 @@
       <c r="A10" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="31" t="s">
-        <v>298</v>
+      <c r="B10" s="55" t="s">
+        <v>335</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>67</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="30" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G10" s="29"/>
       <c r="H10" s="28"/>
@@ -14078,19 +14088,19 @@
         <v>61</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>67</v>
       </c>
       <c r="D11" s="30" t="s">
+        <v>313</v>
+      </c>
+      <c r="E11" s="30" t="s">
         <v>314</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="F11" s="30" t="s">
         <v>315</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>316</v>
       </c>
       <c r="G11" s="29"/>
       <c r="H11" s="28"/>
@@ -14180,7 +14190,7 @@
         <v>274</v>
       </c>
       <c r="H13" s="52" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I13" s="27"/>
       <c r="J13" s="27"/>
@@ -14734,20 +14744,20 @@
         <v>281</v>
       </c>
       <c r="B27" s="35" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C27" s="35" t="s">
         <v>59</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E27" s="36"/>
       <c r="F27" s="36" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G27" s="53" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H27" s="32" t="s">
         <v>188</v>
@@ -14792,7 +14802,7 @@
       </c>
       <c r="G28" s="29"/>
       <c r="H28" s="50" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I28" s="27"/>
       <c r="J28" s="27"/>
@@ -15308,23 +15318,23 @@
     </row>
     <row r="41" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A41" s="34" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B41" s="35" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C41" s="35" t="s">
         <v>59</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E41" s="36"/>
       <c r="F41" s="36" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G41" s="53" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H41" s="32" t="s">
         <v>188</v>
@@ -15805,20 +15815,20 @@
         <v>284</v>
       </c>
       <c r="B53" s="35" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C53" s="35" t="s">
         <v>59</v>
       </c>
       <c r="D53" s="36" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E53" s="36"/>
       <c r="F53" s="36" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G53" s="53" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H53" s="32" t="s">
         <v>188</v>
@@ -15938,20 +15948,20 @@
         <v>157</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C56" s="31" t="s">
         <v>59</v>
       </c>
       <c r="D56" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E56" s="30"/>
       <c r="F56" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G56" s="53" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H56" s="28" t="s">
         <v>188</v>
@@ -16073,17 +16083,17 @@
         <v>67</v>
       </c>
       <c r="D59" s="51" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E59" s="51"/>
       <c r="F59" s="51" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G59" s="48" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H59" s="50" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I59" s="27"/>
       <c r="J59" s="27"/>

</xml_diff>

<commit_message>
Comply with GBIF recommendations regarding ENVO termIDs in DNA extension fields
I have previously mixed ':' and '_' in example data and guide tab, but
will now follow GBIF in using and recommending ':'.
</commit_message>
<xml_diff>
--- a/molmod/static/downloads/SBDI-ASV-template.xlsx
+++ b/molmod/static/downloads/SBDI-ASV-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/molmod/static/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8169E32-E75C-D74B-A80F-4CEE27112DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9045A539-E620-B743-8693-641B1DD8B8AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="500" windowWidth="28000" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="800" yWindow="500" windowWidth="28000" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="344">
   <si>
     <t>materialSampleID</t>
   </si>
@@ -632,15 +632,6 @@
     <t>805R</t>
   </si>
   <si>
-    <t>brackish water [ENVO_00002019]</t>
-  </si>
-  <si>
-    <t>marine biome [ENVO_00000447]</t>
-  </si>
-  <si>
-    <t>aquatic biome [ENVO_00002030]</t>
-  </si>
-  <si>
     <t>Baltic Proper</t>
   </si>
   <si>
@@ -686,9 +677,6 @@
     <t>Example: Annotating a water sample from the photic zone in middle of the Atlantic Ocean, consider: 'oceanic epipelagic zone biome [ENVO:01000033]'. Example: Annotating a sample from the Amazon rainforest consider: 'tropical moist broadleaf forest biome [ENVO:01000228]'. If needed, request new terms on the ENVO tracker, identified here: http://www.obofoundry.org/ontology/envo.htm</t>
   </si>
   <si>
-    <t>marine pelagic biome [ENVO_01000023]</t>
-  </si>
-  <si>
     <t xml:space="preserve">In this field, report which major environmental system your sample or specimen came from. The systems identified should have a coarse spatial grain, to provide the general environmental context of where the sampling was done (e.g. were you in the desert or a rainforest?). </t>
   </si>
   <si>
@@ -714,15 +702,6 @@
   </si>
   <si>
     <t>Note that, for practical reasons, we currently follow GBIF in grouping prokaryote domains Archaea and Bacteria together with e.g. eukaryote kingdoms under header 'kingdom'.</t>
-  </si>
-  <si>
-    <t>Preferably, this value should correspond to environment (biome) in your ENA submission, when applicable. You can search for ENVO_00000428 in https://www.ebi.ac.uk/ols/index, then continue downwards in the biome subtree, until you find the most specific term that accurately describes your data.</t>
-  </si>
-  <si>
-    <t>Preferably, this value should correspond to environment (feature) in your ENA submission, when applicable. A good starting point for searching in https://www.ebi.ac.uk/ols/index could be ENVO_01000813. Again, continue downwards in the subtree, until you find the most specific term that accurately describes your data.</t>
-  </si>
-  <si>
-    <t>Preferably, this value should correspond to environment (material) in your ENA submission, when applicable. A good starting point for searching in https://www.ebi.ac.uk/ols/index could be ENVO_00010483 . Again, continue downwards in the subtree, until you find the most specific term that accurately describes your data.</t>
   </si>
   <si>
     <t>919a2aa9d306e4cf3fa9ca02a2aa5730</t>
@@ -1080,6 +1059,24 @@
   <si>
     <t>Specify here if exact locations or coordinates have been generalized or obfuscated to e.g. protect sensitive species.</t>
   </si>
+  <si>
+    <t>Preferably, this value should correspond to 'broad-scale environmental context' in your ENA submission, when applicable. Note that we (after some initial confusion) follow GBIF recommendations in using a colon ':' (not '_') inside the ENVO termID.</t>
+  </si>
+  <si>
+    <t>Preferably, this value should correspond to 'local environmental context' in your ENA submission, when applicable. Note that we (after some initial confusion) follow GBIF recommendations in using a colon ':' (not '_') inside the ENVO termID.</t>
+  </si>
+  <si>
+    <t>Preferably, this value should correspond to 'environmental medium' in your ENA submission, when applicable. Note that we (after some initial confusion) follow GBIF recommendations in using a colon ':' (not '_') inside the ENVO termID.</t>
+  </si>
+  <si>
+    <t>marine pelagic biome [ENVO:01000023]</t>
+  </si>
+  <si>
+    <t>aquatic biome [ENVO:00002030]</t>
+  </si>
+  <si>
+    <t>marine biome [ENVO:00000447]</t>
+  </si>
 </sst>
 </file>
 
@@ -1089,11 +1086,18 @@
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1317,151 +1321,160 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="13" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="14" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2"/>
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="2"/>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1711,7 +1724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="T30" sqref="T30"/>
     </sheetView>
   </sheetViews>
@@ -1743,22 +1756,22 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>0</v>
@@ -1767,13 +1780,13 @@
         <v>41</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>1</v>
@@ -1797,7 +1810,7 @@
         <v>7</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>8</v>
@@ -1829,28 +1842,28 @@
         <v>188</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>191</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="O2" s="4">
         <v>55.185000000000002</v>
@@ -1863,7 +1876,7 @@
       </c>
       <c r="S2" s="11"/>
       <c r="W2" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="Z2" s="4">
         <v>3</v>
@@ -1877,28 +1890,28 @@
         <v>187</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>190</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="O3" s="4">
         <v>55.433999999999997</v>
@@ -1911,7 +1924,7 @@
       </c>
       <c r="S3" s="11"/>
       <c r="W3" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="Z3" s="4">
         <v>3</v>
@@ -1925,28 +1938,28 @@
         <v>186</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>189</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="O4" s="4">
         <v>56.031999999999996</v>
@@ -1959,7 +1972,7 @@
       </c>
       <c r="S4" s="11"/>
       <c r="W4" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="Z4" s="4">
         <v>3</v>
@@ -4984,7 +4997,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AB9">
     <sortCondition ref="A3:A9"/>
   </sortState>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" xr:uid="{693BAF2D-BDDF-0F46-A91B-2426EEB1769B}"/>
     <hyperlink ref="H3" r:id="rId2" xr:uid="{50F9EBAB-90C1-0945-B3A5-D73BA3A7019E}"/>
@@ -5002,8 +5015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N977"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5026,7 +5039,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>16</v>
@@ -5041,7 +5054,7 @@
         <v>19</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>20</v>
@@ -5056,7 +5069,7 @@
         <v>23</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>24</v>
@@ -5073,7 +5086,7 @@
         <v>188</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>192</v>
@@ -5085,7 +5098,7 @@
         <v>27</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>194</v>
@@ -5100,16 +5113,16 @@
         <v>117</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>198</v>
+        <v>342</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>197</v>
+        <v>343</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5117,7 +5130,7 @@
         <v>187</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>192</v>
@@ -5129,7 +5142,7 @@
         <v>27</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>194</v>
@@ -5144,16 +5157,16 @@
         <v>117</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>198</v>
+        <v>342</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>197</v>
+        <v>343</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5161,7 +5174,7 @@
         <v>186</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>192</v>
@@ -5173,7 +5186,7 @@
         <v>27</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>194</v>
@@ -5188,16 +5201,16 @@
         <v>117</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>198</v>
+        <v>342</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>197</v>
+        <v>343</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6174,7 +6187,7 @@
     <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -6195,7 +6208,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>28</v>
@@ -6236,13 +6249,13 @@
         <v>188</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D2" s="4">
         <v>7.25</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
@@ -6252,13 +6265,13 @@
         <v>187</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D3" s="4">
         <v>7.23</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6266,13 +6279,13 @@
         <v>186</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D4" s="4">
         <v>6.97</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6280,13 +6293,13 @@
         <v>188</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D5" s="4">
         <v>16.899999999999999</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6294,13 +6307,13 @@
         <v>187</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D6" s="4">
         <v>17.399999999999999</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6308,13 +6321,13 @@
         <v>186</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D7" s="4">
         <v>16.899999999999999</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="I7" s="10"/>
     </row>
@@ -9286,13 +9299,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12309,28 +12322,28 @@
     </row>
     <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="M2" s="4">
         <v>2235</v>
@@ -12344,28 +12357,28 @@
     </row>
     <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>236</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="M3" s="4">
         <v>1033</v>
@@ -12379,22 +12392,22 @@
     </row>
     <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="M4" s="4">
         <v>795</v>
@@ -12408,28 +12421,28 @@
     </row>
     <row r="5" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="M5" s="4">
         <v>134</v>
@@ -12443,28 +12456,28 @@
     </row>
     <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>236</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="M6" s="4">
         <v>572</v>
@@ -12478,28 +12491,28 @@
     </row>
     <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="M7" s="4">
         <v>47</v>
@@ -12513,31 +12526,31 @@
     </row>
     <row r="8" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="M8" s="4">
         <v>40</v>
@@ -12551,28 +12564,28 @@
     </row>
     <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="F9" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>257</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>264</v>
       </c>
       <c r="M9" s="4">
         <v>99</v>
@@ -12586,25 +12599,25 @@
     </row>
     <row r="10" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>236</v>
-      </c>
       <c r="F10" s="4" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="M10" s="4">
         <v>312</v>
@@ -12618,28 +12631,28 @@
     </row>
     <row r="11" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="M11" s="4">
         <v>147</v>
@@ -13130,9 +13143,9 @@
   <dimension ref="A1:AA1014"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomLeft" activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13154,7 +13167,7 @@
         <v>52</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="C1" s="45" t="s">
         <v>53</v>
@@ -13199,20 +13212,20 @@
         <v>61</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="C2" s="33" t="s">
         <v>59</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="E2" s="34"/>
       <c r="F2" s="34" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="G2" s="51" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="H2" s="30" t="s">
         <v>188</v>
@@ -13241,21 +13254,21 @@
         <v>61</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="C3" s="29" t="s">
         <v>59</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="E3" s="28"/>
       <c r="F3" s="28" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="G3" s="27"/>
       <c r="H3" s="26" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="J3" s="25"/>
       <c r="K3" s="25"/>
@@ -13281,23 +13294,23 @@
         <v>61</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="C4" s="29" t="s">
         <v>59</v>
       </c>
       <c r="D4" s="56" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="E4" s="28"/>
       <c r="F4" s="56" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="G4" s="58" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="H4" s="57" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
@@ -13318,26 +13331,26 @@
       <c r="Z4" s="25"/>
       <c r="AA4" s="25"/>
     </row>
-    <row r="5" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>61</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="C5" s="29" t="s">
         <v>80</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="28" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="G5" s="27"/>
       <c r="H5" s="26" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="I5" s="41"/>
       <c r="J5" s="41"/>
@@ -13364,25 +13377,25 @@
         <v>61</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="C6" s="29" t="s">
         <v>80</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="I6" s="41"/>
       <c r="J6" s="41"/>
@@ -13409,17 +13422,17 @@
         <v>61</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="C7" s="29" t="s">
         <v>67</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="28" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G7" s="27"/>
       <c r="H7" s="26"/>
@@ -13458,13 +13471,13 @@
       </c>
       <c r="E8" s="28"/>
       <c r="F8" s="28" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H8" s="26" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="I8" s="41"/>
       <c r="J8" s="41"/>
@@ -13497,17 +13510,17 @@
         <v>59</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="E9" s="28"/>
       <c r="F9" s="28" t="s">
         <v>166</v>
       </c>
       <c r="G9" s="46" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="H9" s="26" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="I9" s="41"/>
       <c r="J9" s="41"/>
@@ -13534,17 +13547,17 @@
         <v>61</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="C10" s="29" t="s">
         <v>67</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="E10" s="28"/>
       <c r="F10" s="28" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="G10" s="27"/>
       <c r="H10" s="26"/>
@@ -13573,17 +13586,17 @@
         <v>61</v>
       </c>
       <c r="B11" s="53" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="C11" s="29" t="s">
         <v>67</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="E11" s="28"/>
       <c r="F11" s="28" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="G11" s="27"/>
       <c r="H11" s="26"/>
@@ -13607,24 +13620,24 @@
       <c r="Z11" s="25"/>
       <c r="AA11" s="25"/>
     </row>
-    <row r="12" spans="1:27" ht="187" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
         <v>61</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="C12" s="29" t="s">
         <v>67</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="G12" s="27"/>
       <c r="H12" s="26"/>
@@ -13662,13 +13675,13 @@
         <v>63</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F13" s="28" t="s">
         <v>64</v>
       </c>
       <c r="G13" s="27" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H13" s="42" t="s">
         <v>191</v>
@@ -13693,7 +13706,7 @@
       <c r="Z13" s="25"/>
       <c r="AA13" s="25"/>
     </row>
-    <row r="14" spans="1:27" ht="204" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="221" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
         <v>61</v>
       </c>
@@ -13711,10 +13724,10 @@
         <v>66</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="H14" s="50" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="I14" s="25"/>
       <c r="J14" s="25"/>
@@ -13754,7 +13767,7 @@
         <v>69</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="H15" s="40" t="s">
         <v>70</v>
@@ -13857,7 +13870,7 @@
       <c r="Z17" s="25"/>
       <c r="AA17" s="25"/>
     </row>
-    <row r="18" spans="1:27" ht="119" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" ht="136" x14ac:dyDescent="0.2">
       <c r="A18" s="29" t="s">
         <v>61</v>
       </c>
@@ -13946,20 +13959,20 @@
         <v>61</v>
       </c>
       <c r="B20" s="55" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="C20" s="55" t="s">
         <v>67</v>
       </c>
       <c r="D20" s="56" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="E20" s="56"/>
       <c r="F20" s="56" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="G20" s="58" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="H20" s="26"/>
       <c r="I20" s="25"/>
@@ -14002,10 +14015,10 @@
         <v>85</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="H21" s="26" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="I21" s="25"/>
       <c r="J21" s="25"/>
@@ -14306,23 +14319,23 @@
     </row>
     <row r="29" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A29" s="33" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="C29" s="33" t="s">
         <v>59</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="E29" s="34"/>
       <c r="F29" s="34" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="G29" s="51" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="H29" s="30" t="s">
         <v>188</v>
@@ -14348,7 +14361,7 @@
     </row>
     <row r="30" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A30" s="36" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B30" s="29" t="s">
         <v>16</v>
@@ -14367,7 +14380,7 @@
       </c>
       <c r="G30" s="27"/>
       <c r="H30" s="48" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="I30" s="25"/>
       <c r="J30" s="25"/>
@@ -14391,7 +14404,7 @@
     </row>
     <row r="31" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="36" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B31" s="29" t="s">
         <v>17</v>
@@ -14404,7 +14417,7 @@
       </c>
       <c r="E31" s="28"/>
       <c r="F31" s="37" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="G31" s="27"/>
       <c r="H31" s="26"/>
@@ -14428,9 +14441,9 @@
       <c r="Z31" s="25"/>
       <c r="AA31" s="25"/>
     </row>
-    <row r="32" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A32" s="36" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B32" s="29" t="s">
         <v>18</v>
@@ -14469,7 +14482,7 @@
     </row>
     <row r="33" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A33" s="36" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B33" s="29" t="s">
         <v>19</v>
@@ -14508,20 +14521,20 @@
     </row>
     <row r="34" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="36" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="C34" s="29" t="s">
         <v>59</v>
       </c>
       <c r="D34" s="28" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="E34" s="28"/>
       <c r="F34" s="37" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="G34" s="27"/>
       <c r="H34" s="26"/>
@@ -14547,7 +14560,7 @@
     </row>
     <row r="35" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="36" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B35" s="29" t="s">
         <v>20</v>
@@ -14586,7 +14599,7 @@
     </row>
     <row r="36" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="36" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B36" s="29" t="s">
         <v>21</v>
@@ -14625,7 +14638,7 @@
     </row>
     <row r="37" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="36" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B37" s="29" t="s">
         <v>22</v>
@@ -14664,7 +14677,7 @@
     </row>
     <row r="38" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="36" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B38" s="29" t="s">
         <v>23</v>
@@ -14703,10 +14716,10 @@
     </row>
     <row r="39" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="36" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C39" s="29" t="s">
         <v>59</v>
@@ -14721,10 +14734,10 @@
         <v>60</v>
       </c>
       <c r="G39" s="27" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="H39" s="26" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="I39" s="25"/>
       <c r="J39" s="25"/>
@@ -14748,7 +14761,7 @@
     </row>
     <row r="40" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A40" s="36" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B40" s="29" t="s">
         <v>24</v>
@@ -14757,19 +14770,19 @@
         <v>59</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F40" s="37" t="s">
-        <v>213</v>
-      </c>
-      <c r="G40" s="27" t="s">
-        <v>224</v>
-      </c>
-      <c r="H40" s="26" t="s">
-        <v>214</v>
+        <v>210</v>
+      </c>
+      <c r="G40" s="59" t="s">
+        <v>338</v>
+      </c>
+      <c r="H40" s="61" t="s">
+        <v>341</v>
       </c>
       <c r="I40" s="25"/>
       <c r="J40" s="25"/>
@@ -14793,7 +14806,7 @@
     </row>
     <row r="41" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A41" s="36" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B41" s="29" t="s">
         <v>25</v>
@@ -14802,19 +14815,19 @@
         <v>59</v>
       </c>
       <c r="D41" s="28" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F41" s="28" t="s">
-        <v>218</v>
-      </c>
-      <c r="G41" s="27" t="s">
-        <v>225</v>
+        <v>214</v>
+      </c>
+      <c r="G41" s="59" t="s">
+        <v>339</v>
       </c>
       <c r="H41" s="26" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I41" s="25"/>
       <c r="J41" s="25"/>
@@ -14836,9 +14849,9 @@
       <c r="Z41" s="25"/>
       <c r="AA41" s="25"/>
     </row>
-    <row r="42" spans="1:27" ht="154" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" ht="103" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B42" s="24" t="s">
         <v>26</v>
@@ -14849,17 +14862,17 @@
       <c r="D42" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="E42" s="35" t="s">
+      <c r="E42" s="60" t="s">
         <v>119</v>
       </c>
       <c r="F42" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="G42" s="22" t="s">
-        <v>226</v>
+      <c r="G42" s="59" t="s">
+        <v>340</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="I42" s="25"/>
       <c r="J42" s="25"/>
@@ -14883,23 +14896,23 @@
     </row>
     <row r="43" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A43" s="54" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="B43" s="33" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="C43" s="33" t="s">
         <v>59</v>
       </c>
       <c r="D43" s="34" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="E43" s="34"/>
       <c r="F43" s="34" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="G43" s="51" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="H43" s="30" t="s">
         <v>188</v>
@@ -14944,7 +14957,7 @@
         <v>124</v>
       </c>
       <c r="G44" s="27" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H44" s="26"/>
       <c r="I44" s="25"/>
@@ -15047,7 +15060,7 @@
       <c r="Z46" s="25"/>
       <c r="AA46" s="25"/>
     </row>
-    <row r="47" spans="1:27" ht="119" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:27" ht="136" x14ac:dyDescent="0.2">
       <c r="A47" s="29" t="s">
         <v>121</v>
       </c>
@@ -15293,7 +15306,7 @@
       <c r="Z52" s="25"/>
       <c r="AA52" s="25"/>
     </row>
-    <row r="53" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A53" s="29" t="s">
         <v>121</v>
       </c>
@@ -15377,23 +15390,23 @@
     </row>
     <row r="55" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A55" s="32" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="B55" s="33" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="C55" s="33" t="s">
         <v>59</v>
       </c>
       <c r="D55" s="34" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="E55" s="34"/>
       <c r="F55" s="34" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="G55" s="51" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="H55" s="30" t="s">
         <v>188</v>
@@ -15420,10 +15433,10 @@
     </row>
     <row r="56" spans="1:27" ht="205" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C56" s="24" t="s">
         <v>60</v>
@@ -15438,10 +15451,10 @@
         <v>60</v>
       </c>
       <c r="G56" s="22" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="H56" s="21" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="I56" s="25"/>
       <c r="J56" s="25"/>
@@ -15465,7 +15478,7 @@
     </row>
     <row r="57" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A57" s="32" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="B57" s="33" t="s">
         <v>39</v>
@@ -15513,20 +15526,20 @@
         <v>157</v>
       </c>
       <c r="B58" s="29" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="C58" s="29" t="s">
         <v>59</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="E58" s="28"/>
       <c r="F58" s="28" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="G58" s="51" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="H58" s="26" t="s">
         <v>188</v>
@@ -15648,17 +15661,17 @@
         <v>67</v>
       </c>
       <c r="D61" s="49" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="E61" s="49"/>
       <c r="F61" s="49" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="G61" s="46" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="H61" s="48" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="I61" s="25"/>
       <c r="J61" s="25"/>
@@ -15698,7 +15711,7 @@
         <v>168</v>
       </c>
       <c r="G62" s="27" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="H62" s="26"/>
       <c r="I62" s="25"/>

</xml_diff>

<commit_message>
Add text box tips in Excel template
Mention TSV upload option, gene separation, emof vs. emof-simple 
selection, eventID and ASV inclusion in ASV-table tab, as these have 
been misunderstood by data providers.
</commit_message>
<xml_diff>
--- a/molmod/static/downloads/SBDI-ASV-template.xlsx
+++ b/molmod/static/downloads/SBDI-ASV-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/molmod/static/downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9045A539-E620-B743-8693-641B1DD8B8AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA4FA8A-67B6-0C4B-9942-0156F4DFFD74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="500" windowWidth="28000" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1100" yWindow="500" windowWidth="28000" windowHeight="17500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event" sheetId="1" r:id="rId1"/>
@@ -1524,6 +1524,537 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A3C99F4-DBAD-CB48-A06D-1287F4E0ED1C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="101600" y="876300"/>
+          <a:ext cx="3314700" cy="863600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>You can submit a tar.gz archive of TSV files instead of Excel. Each TSV should match an Excel tab.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:endParaRPr lang="en-GB" sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2641600</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{923770D5-4678-034A-80D9-8270283BBFE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="76200" y="850900"/>
+          <a:ext cx="3314700" cy="863600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400"/>
+            <a:t>If you have sequenced multiple target genes, please submit them as separate datasets.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64DDC696-724A-4140-A62C-99FC7B46AEF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="76200" y="1409700"/>
+          <a:ext cx="3314700" cy="863600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400"/>
+            <a:t>Fill</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+            <a:t> in</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="1"/>
+            <a:t>EITHER</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400"/>
+            <a:t> "emof" </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="1"/>
+            <a:t>OR</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400"/>
+            <a:t> "emof-simple" tab. Most providers should use "emof-simple" and leave "emof" blank.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:endParaRPr lang="en-GB" sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63C237A8-B4E5-0848-A156-A6207776357F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="76200" y="850900"/>
+          <a:ext cx="3314700" cy="863600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400"/>
+            <a:t>Fill</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+            <a:t> in</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="1"/>
+            <a:t>EITHER</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400"/>
+            <a:t> "emof" </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="1"/>
+            <a:t>OR</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400"/>
+            <a:t> "emof-simple" tab. Most providers should use "emof-simple" and leave "emof" blank.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:endParaRPr lang="en-GB" sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1346200</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA24C4EB-246B-B544-A828-28E243C31472}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="88900" y="2298700"/>
+          <a:ext cx="3505200" cy="863600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400"/>
+            <a:t>Ensure </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+            <a:t>event (=sample) headers match eventIDs in the other tabs, and only include ASVs that occur in at least one sample.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:endParaRPr lang="en-GB" sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -1724,8 +2255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA991"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="T30" sqref="T30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5008,6 +5539,7 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -5015,8 +5547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N977"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6190,6 +6722,7 @@
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6197,7 +6730,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L982"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9282,6 +9817,7 @@
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9289,7 +9825,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221FF7C6-E74E-E14F-A681-9750CC4E526F}">
   <dimension ref="A1:C973"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12251,6 +12789,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12258,8 +12797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O472"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13132,6 +13671,7 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13142,10 +13682,10 @@
   </sheetPr>
   <dimension ref="A1:AA1014"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="H42" sqref="H42"/>
+      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13331,7 +13871,7 @@
       <c r="Z4" s="25"/>
       <c r="AA4" s="25"/>
     </row>
-    <row r="5" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>61</v>
       </c>
@@ -13620,7 +14160,7 @@
       <c r="Z11" s="25"/>
       <c r="AA11" s="25"/>
     </row>
-    <row r="12" spans="1:27" ht="204" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="187" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
         <v>61</v>
       </c>
@@ -13706,7 +14246,7 @@
       <c r="Z13" s="25"/>
       <c r="AA13" s="25"/>
     </row>
-    <row r="14" spans="1:27" ht="221" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
         <v>61</v>
       </c>
@@ -13870,7 +14410,7 @@
       <c r="Z17" s="25"/>
       <c r="AA17" s="25"/>
     </row>
-    <row r="18" spans="1:27" ht="136" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" ht="119" x14ac:dyDescent="0.2">
       <c r="A18" s="29" t="s">
         <v>61</v>
       </c>
@@ -14441,7 +14981,7 @@
       <c r="Z31" s="25"/>
       <c r="AA31" s="25"/>
     </row>
-    <row r="32" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="36" t="s">
         <v>274</v>
       </c>
@@ -15060,7 +15600,7 @@
       <c r="Z46" s="25"/>
       <c r="AA46" s="25"/>
     </row>
-    <row r="47" spans="1:27" ht="136" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:27" ht="119" x14ac:dyDescent="0.2">
       <c r="A47" s="29" t="s">
         <v>121</v>
       </c>
@@ -15306,7 +15846,7 @@
       <c r="Z52" s="25"/>
       <c r="AA52" s="25"/>
     </row>
-    <row r="53" spans="1:27" ht="85" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A53" s="29" t="s">
         <v>121</v>
       </c>

</xml_diff>

<commit_message>
Clarify that template structure should not be edited
</commit_message>
<xml_diff>
--- a/molmod/static/downloads/SBDI-ASV-template.xlsx
+++ b/molmod/static/downloads/SBDI-ASV-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/molmod/static/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA4FA8A-67B6-0C4B-9942-0156F4DFFD74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B03D9F-967F-BD4F-B43A-B731EC87EE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="500" windowWidth="28000" windowHeight="17500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4880" yWindow="4360" windowWidth="28000" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event" sheetId="1" r:id="rId1"/>
@@ -1535,8 +1535,8 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:colOff>1193800</xdr:colOff>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1553,7 +1553,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="101600" y="876300"/>
-          <a:ext cx="3314700" cy="863600"/>
+          <a:ext cx="3771900" cy="1435100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1600,7 +1600,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>You can submit a tar.gz archive of TSV files instead of Excel. Each TSV should match an Excel tab.</a:t>
+            <a:t>Alternatively, you can submit a tar.gz archive of TSVs matching the Excel tabs. </a:t>
           </a:r>
           <a:br>
             <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike">
@@ -1624,6 +1624,66 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
           </a:br>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Some fields are optional to fill in (see </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>guide</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> tab)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>, but don't edit the template structure</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> by renaming or removing tabs or fields.</a:t>
+          </a:r>
           <a:endParaRPr lang="en-GB" sz="1400"/>
         </a:p>
       </xdr:txBody>
@@ -1790,20 +1850,20 @@
             <a:t> </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-GB" sz="1400" b="1"/>
-            <a:t>EITHER</a:t>
+            <a:rPr lang="en-GB" sz="1400" b="0"/>
+            <a:t>EITHER </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1400"/>
-            <a:t> "emof" </a:t>
+            <a:t>"emof" </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-GB" sz="1400" b="1"/>
-            <a:t>OR</a:t>
+            <a:rPr lang="en-GB" sz="1400" b="0"/>
+            <a:t>OR </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1400"/>
-            <a:t> "emof-simple" tab. Most providers should use "emof-simple" and leave "emof" blank.</a:t>
+            <a:t>"emof-simple" tab. Most providers should use "emof-simple" and leave "emof" blank.</a:t>
           </a:r>
           <a:br>
             <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike">
@@ -1841,22 +1901,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:colOff>165100</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
+      <xdr:colOff>863600</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
+        <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63C237A8-B4E5-0848-A156-A6207776357F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{354444C0-7F52-C64E-92B8-18FB99501B9C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1864,7 +1924,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="76200" y="850900"/>
+          <a:off x="165100" y="889000"/>
           <a:ext cx="3314700" cy="863600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1915,20 +1975,20 @@
             <a:t> </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-GB" sz="1400" b="1"/>
-            <a:t>EITHER</a:t>
+            <a:rPr lang="en-GB" sz="1400" b="0"/>
+            <a:t>EITHER </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1400"/>
-            <a:t> "emof" </a:t>
+            <a:t>"emof" </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-GB" sz="1400" b="1"/>
-            <a:t>OR</a:t>
+            <a:rPr lang="en-GB" sz="1400" b="0"/>
+            <a:t>OR </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1400"/>
-            <a:t> "emof-simple" tab. Most providers should use "emof-simple" and leave "emof" blank.</a:t>
+            <a:t>"emof-simple" tab. Most providers should use "emof-simple" and leave "emof" blank.</a:t>
           </a:r>
           <a:br>
             <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike">
@@ -2255,8 +2315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA991"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9826,7 +9886,7 @@
   <dimension ref="A1:C973"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12797,8 +12857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O472"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>